<commit_message>
Prepravke budzeta i prezentacije
</commit_message>
<xml_diff>
--- a/2b Format partner budget - Horizon2020.xlsx
+++ b/2b Format partner budget - Horizon2020.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ZORAN\Desktop\USP_projekat\CardioGuardian\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85368270-9341-49A4-812A-F0AEE366F4CB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Detaljno budzet" sheetId="1" r:id="rId1"/>
@@ -17,7 +18,7 @@
     <sheet name="Equipment - budzet" sheetId="3" r:id="rId3"/>
     <sheet name="Subcontracting - budzet" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -25,6 +26,7 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,12 +34,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Kampen, Jan-Joris van</author>
   </authors>
   <commentList>
-    <comment ref="O13" authorId="0" shapeId="0">
+    <comment ref="O13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -66,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="131">
   <si>
     <t>Partner budget Horizon 2020</t>
   </si>
@@ -405,16 +407,70 @@
   </si>
   <si>
     <t>Потрошни материјал, канцеларијски прибор</t>
+  </si>
+  <si>
+    <t>WP2</t>
+  </si>
+  <si>
+    <t>Будимпешта, Мађарска</t>
+  </si>
+  <si>
+    <t>Базел, Швајцарска</t>
+  </si>
+  <si>
+    <t>Лондон, Велика Британија</t>
+  </si>
+  <si>
+    <t>Токио, Јапан</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Превођење извештаја о напретку </t>
+  </si>
+  <si>
+    <t>WP3</t>
+  </si>
+  <si>
+    <t>Превођење корисничких захтева за хардверску и софтверску компоненту</t>
+  </si>
+  <si>
+    <t>Превођење анализе и детаља система</t>
+  </si>
+  <si>
+    <t>Превођење извештаја о успешности интеграције</t>
+  </si>
+  <si>
+    <t>WP6</t>
+  </si>
+  <si>
+    <t>Превођење извештаја тестирања</t>
+  </si>
+  <si>
+    <t>WP7</t>
+  </si>
+  <si>
+    <t>Адвокатске услуге</t>
+  </si>
+  <si>
+    <t>WP1, WP8</t>
+  </si>
+  <si>
+    <t>Организација тим билдинга</t>
+  </si>
+  <si>
+    <t>Израда промотивног материјала</t>
+  </si>
+  <si>
+    <t>Услуге фирме за маркетинг</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -518,6 +574,13 @@
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="10">
@@ -765,7 +828,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -870,7 +933,12 @@
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -988,7 +1056,7 @@
         <xdr:cNvPr id="3" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA4F558B-8D56-430D-AA83-772AD1DE26DE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA4F558B-8D56-430D-AA83-772AD1DE26DE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1123,6 +1191,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1158,6 +1243,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1333,7 +1435,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -1365,65 +1467,65 @@
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="E3" s="67"/>
-      <c r="F3" s="67"/>
-      <c r="G3" s="67"/>
-      <c r="H3" s="67"/>
-      <c r="I3" s="67"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="72"/>
+      <c r="I3" s="72"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D4" s="2"/>
-      <c r="E4" s="68" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" s="69"/>
-      <c r="G4" s="69"/>
-      <c r="H4" s="69"/>
-      <c r="I4" s="69"/>
+      <c r="E4" s="73" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="74"/>
+      <c r="G4" s="74"/>
+      <c r="H4" s="74"/>
+      <c r="I4" s="74"/>
       <c r="J4" s="3"/>
-      <c r="L4" s="69" t="s">
+      <c r="L4" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="M4" s="69"/>
-      <c r="N4" s="69"/>
+      <c r="M4" s="74"/>
+      <c r="N4" s="74"/>
       <c r="O4" s="4">
         <v>0.25</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D5" s="2"/>
-      <c r="E5" s="68" t="s">
+      <c r="E5" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="69"/>
-      <c r="G5" s="69"/>
-      <c r="H5" s="69"/>
-      <c r="I5" s="69"/>
+      <c r="F5" s="74"/>
+      <c r="G5" s="74"/>
+      <c r="H5" s="74"/>
+      <c r="I5" s="74"/>
       <c r="J5" s="3"/>
-      <c r="L5" s="69" t="s">
+      <c r="L5" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="M5" s="69"/>
-      <c r="N5" s="69"/>
+      <c r="M5" s="74"/>
+      <c r="N5" s="74"/>
       <c r="O5" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D6" s="2"/>
-      <c r="E6" s="68" t="s">
+      <c r="E6" s="73" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="69"/>
-      <c r="G6" s="69"/>
-      <c r="H6" s="69"/>
-      <c r="I6" s="69"/>
+      <c r="F6" s="74"/>
+      <c r="G6" s="74"/>
+      <c r="H6" s="74"/>
+      <c r="I6" s="74"/>
       <c r="J6" s="3"/>
-      <c r="L6" s="69" t="s">
+      <c r="L6" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="M6" s="69"/>
-      <c r="N6" s="69"/>
+      <c r="M6" s="74"/>
+      <c r="N6" s="74"/>
       <c r="O6" s="5">
         <v>0.7</v>
       </c>
@@ -1433,19 +1535,19 @@
       <c r="Q6" s="6"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="E7" s="69" t="s">
+      <c r="E7" s="74" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="69"/>
-      <c r="G7" s="69"/>
-      <c r="H7" s="69"/>
-      <c r="I7" s="69"/>
+      <c r="F7" s="74"/>
+      <c r="G7" s="74"/>
+      <c r="H7" s="74"/>
+      <c r="I7" s="74"/>
       <c r="J7" s="3"/>
-      <c r="L7" s="69" t="s">
+      <c r="L7" s="74" t="s">
         <v>9</v>
       </c>
-      <c r="M7" s="69"/>
-      <c r="N7" s="69"/>
+      <c r="M7" s="74"/>
+      <c r="N7" s="74"/>
       <c r="O7" s="4">
         <v>1</v>
       </c>
@@ -1456,56 +1558,56 @@
     </row>
     <row r="9" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="70" t="s">
+      <c r="A10" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="71"/>
-      <c r="C10" s="71"/>
-      <c r="D10" s="71"/>
-      <c r="E10" s="71"/>
-      <c r="F10" s="71"/>
-      <c r="G10" s="71"/>
-      <c r="H10" s="71"/>
-      <c r="I10" s="71"/>
-      <c r="J10" s="71"/>
-      <c r="K10" s="71"/>
-      <c r="L10" s="71"/>
-      <c r="M10" s="71"/>
-      <c r="N10" s="71"/>
-      <c r="O10" s="71"/>
-      <c r="P10" s="71"/>
-      <c r="Q10" s="71"/>
-      <c r="R10" s="71"/>
+      <c r="B10" s="76"/>
+      <c r="C10" s="76"/>
+      <c r="D10" s="76"/>
+      <c r="E10" s="76"/>
+      <c r="F10" s="76"/>
+      <c r="G10" s="76"/>
+      <c r="H10" s="76"/>
+      <c r="I10" s="76"/>
+      <c r="J10" s="76"/>
+      <c r="K10" s="76"/>
+      <c r="L10" s="76"/>
+      <c r="M10" s="76"/>
+      <c r="N10" s="76"/>
+      <c r="O10" s="76"/>
+      <c r="P10" s="76"/>
+      <c r="Q10" s="76"/>
+      <c r="R10" s="76"/>
       <c r="S10" s="8"/>
     </row>
     <row r="12" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D12" s="72" t="s">
+      <c r="D12" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="72"/>
-      <c r="F12" s="72"/>
-      <c r="G12" s="72"/>
-      <c r="H12" s="72"/>
-      <c r="I12" s="72"/>
-      <c r="J12" s="73" t="s">
+      <c r="E12" s="77"/>
+      <c r="F12" s="77"/>
+      <c r="G12" s="77"/>
+      <c r="H12" s="77"/>
+      <c r="I12" s="77"/>
+      <c r="J12" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="K12" s="73"/>
-      <c r="L12" s="73"/>
-      <c r="M12" s="73"/>
-      <c r="N12" s="73"/>
-      <c r="O12" s="73"/>
-      <c r="P12" s="73"/>
-      <c r="Q12" s="73"/>
-      <c r="R12" s="73"/>
+      <c r="K12" s="78"/>
+      <c r="L12" s="78"/>
+      <c r="M12" s="78"/>
+      <c r="N12" s="78"/>
+      <c r="O12" s="78"/>
+      <c r="P12" s="78"/>
+      <c r="Q12" s="78"/>
+      <c r="R12" s="78"/>
       <c r="S12" s="9"/>
     </row>
     <row r="13" spans="1:19" s="14" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="66" t="s">
+      <c r="A13" s="71" t="s">
         <v>61</v>
       </c>
-      <c r="B13" s="66"/>
-      <c r="C13" s="66"/>
+      <c r="B13" s="71"/>
+      <c r="C13" s="71"/>
       <c r="D13" s="48" t="s">
         <v>70</v>
       </c>
@@ -1556,11 +1658,11 @@
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="61" t="s">
+      <c r="A14" s="66" t="s">
         <v>42</v>
       </c>
-      <c r="B14" s="61"/>
-      <c r="C14" s="61"/>
+      <c r="B14" s="66"/>
+      <c r="C14" s="66"/>
       <c r="D14" s="15"/>
       <c r="E14" s="15"/>
       <c r="F14" s="15"/>
@@ -1591,11 +1693,11 @@
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="61" t="s">
+      <c r="A15" s="66" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="61"/>
-      <c r="C15" s="61"/>
+      <c r="B15" s="66"/>
+      <c r="C15" s="66"/>
       <c r="D15" s="15"/>
       <c r="E15" s="15"/>
       <c r="F15" s="15"/>
@@ -1626,11 +1728,11 @@
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" s="61" t="s">
+      <c r="A16" s="66" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="61"/>
-      <c r="C16" s="61"/>
+      <c r="B16" s="66"/>
+      <c r="C16" s="66"/>
       <c r="D16" s="15"/>
       <c r="E16" s="15"/>
       <c r="F16" s="15"/>
@@ -1661,11 +1763,11 @@
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" s="61" t="s">
+      <c r="A17" s="66" t="s">
         <v>45</v>
       </c>
-      <c r="B17" s="61"/>
-      <c r="C17" s="61"/>
+      <c r="B17" s="66"/>
+      <c r="C17" s="66"/>
       <c r="D17" s="15"/>
       <c r="E17" s="15"/>
       <c r="F17" s="15"/>
@@ -1696,11 +1798,11 @@
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A18" s="61" t="s">
+      <c r="A18" s="66" t="s">
         <v>46</v>
       </c>
-      <c r="B18" s="61"/>
-      <c r="C18" s="61"/>
+      <c r="B18" s="66"/>
+      <c r="C18" s="66"/>
       <c r="D18" s="15"/>
       <c r="E18" s="15"/>
       <c r="F18" s="15"/>
@@ -1731,11 +1833,11 @@
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" s="61" t="s">
+      <c r="A19" s="66" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="61"/>
-      <c r="C19" s="61"/>
+      <c r="B19" s="66"/>
+      <c r="C19" s="66"/>
       <c r="D19" s="15"/>
       <c r="E19" s="15"/>
       <c r="F19" s="15"/>
@@ -1766,11 +1868,11 @@
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A20" s="61" t="s">
+      <c r="A20" s="66" t="s">
         <v>48</v>
       </c>
-      <c r="B20" s="61"/>
-      <c r="C20" s="61"/>
+      <c r="B20" s="66"/>
+      <c r="C20" s="66"/>
       <c r="D20" s="15"/>
       <c r="E20" s="15"/>
       <c r="F20" s="15"/>
@@ -1801,11 +1903,11 @@
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A21" s="61" t="s">
+      <c r="A21" s="66" t="s">
         <v>49</v>
       </c>
-      <c r="B21" s="61"/>
-      <c r="C21" s="61"/>
+      <c r="B21" s="66"/>
+      <c r="C21" s="66"/>
       <c r="D21" s="15"/>
       <c r="E21" s="15"/>
       <c r="F21" s="15"/>
@@ -1836,11 +1938,11 @@
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A22" s="61" t="s">
+      <c r="A22" s="66" t="s">
         <v>50</v>
       </c>
-      <c r="B22" s="61"/>
-      <c r="C22" s="61"/>
+      <c r="B22" s="66"/>
+      <c r="C22" s="66"/>
       <c r="D22" s="15"/>
       <c r="E22" s="15"/>
       <c r="F22" s="15"/>
@@ -1871,11 +1973,11 @@
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A23" s="61" t="s">
+      <c r="A23" s="66" t="s">
         <v>51</v>
       </c>
-      <c r="B23" s="61"/>
-      <c r="C23" s="61"/>
+      <c r="B23" s="66"/>
+      <c r="C23" s="66"/>
       <c r="D23" s="15"/>
       <c r="E23" s="15"/>
       <c r="F23" s="15"/>
@@ -1906,11 +2008,11 @@
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A24" s="65" t="s">
+      <c r="A24" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="65"/>
-      <c r="C24" s="65"/>
+      <c r="B24" s="70"/>
+      <c r="C24" s="70"/>
       <c r="D24" s="15">
         <f>SUM(D14:D23)</f>
         <v>0</v>
@@ -2031,24 +2133,24 @@
       <c r="S27" s="31"/>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A28" s="64" t="s">
+      <c r="A28" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="B28" s="64"/>
-      <c r="C28" s="64"/>
-      <c r="D28" s="64"/>
-      <c r="E28" s="64"/>
-      <c r="F28" s="64"/>
-      <c r="G28" s="64"/>
-      <c r="H28" s="64"/>
-      <c r="I28" s="64"/>
-      <c r="J28" s="64"/>
-      <c r="K28" s="64"/>
-      <c r="L28" s="64"/>
-      <c r="M28" s="64"/>
-      <c r="N28" s="64"/>
-      <c r="O28" s="64"/>
-      <c r="P28" s="64"/>
+      <c r="B28" s="69"/>
+      <c r="C28" s="69"/>
+      <c r="D28" s="69"/>
+      <c r="E28" s="69"/>
+      <c r="F28" s="69"/>
+      <c r="G28" s="69"/>
+      <c r="H28" s="69"/>
+      <c r="I28" s="69"/>
+      <c r="J28" s="69"/>
+      <c r="K28" s="69"/>
+      <c r="L28" s="69"/>
+      <c r="M28" s="69"/>
+      <c r="N28" s="69"/>
+      <c r="O28" s="69"/>
+      <c r="P28" s="69"/>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="32"/>
@@ -2089,95 +2191,95 @@
       <c r="P30" s="32"/>
     </row>
     <row r="31" spans="1:20" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="57" t="str">
+      <c r="A31" s="62" t="str">
         <f>CONCATENATE("participant"," ",J6)</f>
         <v xml:space="preserve">participant </v>
       </c>
-      <c r="B31" s="58"/>
+      <c r="B31" s="63"/>
       <c r="C31" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="D31" s="61" t="s">
+      <c r="D31" s="66" t="s">
         <v>33</v>
       </c>
-      <c r="E31" s="62"/>
-      <c r="F31" s="62"/>
-      <c r="G31" s="62"/>
-      <c r="H31" s="62"/>
-      <c r="I31" s="62"/>
-      <c r="J31" s="62"/>
-      <c r="K31" s="62"/>
-      <c r="L31" s="62"/>
-      <c r="M31" s="62"/>
-      <c r="N31" s="62"/>
-      <c r="O31" s="62"/>
-      <c r="P31" s="62"/>
+      <c r="E31" s="67"/>
+      <c r="F31" s="67"/>
+      <c r="G31" s="67"/>
+      <c r="H31" s="67"/>
+      <c r="I31" s="67"/>
+      <c r="J31" s="67"/>
+      <c r="K31" s="67"/>
+      <c r="L31" s="67"/>
+      <c r="M31" s="67"/>
+      <c r="N31" s="67"/>
+      <c r="O31" s="67"/>
+      <c r="P31" s="67"/>
     </row>
     <row r="32" spans="1:20" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="51" t="s">
+      <c r="A32" s="56" t="s">
         <v>34</v>
       </c>
-      <c r="B32" s="51"/>
+      <c r="B32" s="56"/>
       <c r="C32" s="34"/>
-      <c r="D32" s="63" t="s">
+      <c r="D32" s="68" t="s">
         <v>67</v>
       </c>
-      <c r="E32" s="56"/>
-      <c r="F32" s="56"/>
-      <c r="G32" s="56"/>
-      <c r="H32" s="56"/>
-      <c r="I32" s="56"/>
-      <c r="J32" s="56"/>
-      <c r="K32" s="56"/>
-      <c r="L32" s="56"/>
-      <c r="M32" s="56"/>
-      <c r="N32" s="56"/>
-      <c r="O32" s="56"/>
-      <c r="P32" s="56"/>
+      <c r="E32" s="61"/>
+      <c r="F32" s="61"/>
+      <c r="G32" s="61"/>
+      <c r="H32" s="61"/>
+      <c r="I32" s="61"/>
+      <c r="J32" s="61"/>
+      <c r="K32" s="61"/>
+      <c r="L32" s="61"/>
+      <c r="M32" s="61"/>
+      <c r="N32" s="61"/>
+      <c r="O32" s="61"/>
+      <c r="P32" s="61"/>
       <c r="S32" s="31"/>
     </row>
     <row r="33" spans="1:19" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="51" t="s">
+      <c r="A33" s="56" t="s">
         <v>35</v>
       </c>
-      <c r="B33" s="51"/>
+      <c r="B33" s="56"/>
       <c r="C33" s="35"/>
-      <c r="D33" s="56" t="s">
+      <c r="D33" s="61" t="s">
         <v>68</v>
       </c>
-      <c r="E33" s="56"/>
-      <c r="F33" s="56"/>
-      <c r="G33" s="56"/>
-      <c r="H33" s="56"/>
-      <c r="I33" s="56"/>
-      <c r="J33" s="56"/>
-      <c r="K33" s="56"/>
-      <c r="L33" s="56"/>
-      <c r="M33" s="56"/>
-      <c r="N33" s="56"/>
-      <c r="O33" s="56"/>
-      <c r="P33" s="56"/>
+      <c r="E33" s="61"/>
+      <c r="F33" s="61"/>
+      <c r="G33" s="61"/>
+      <c r="H33" s="61"/>
+      <c r="I33" s="61"/>
+      <c r="J33" s="61"/>
+      <c r="K33" s="61"/>
+      <c r="L33" s="61"/>
+      <c r="M33" s="61"/>
+      <c r="N33" s="61"/>
+      <c r="O33" s="61"/>
+      <c r="P33" s="61"/>
       <c r="S33" s="31"/>
     </row>
     <row r="34" spans="1:19" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="51" t="s">
+      <c r="A34" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="B34" s="51"/>
+      <c r="B34" s="56"/>
       <c r="C34" s="35"/>
-      <c r="D34" s="56"/>
-      <c r="E34" s="56"/>
-      <c r="F34" s="56"/>
-      <c r="G34" s="56"/>
-      <c r="H34" s="56"/>
-      <c r="I34" s="56"/>
-      <c r="J34" s="56"/>
-      <c r="K34" s="56"/>
-      <c r="L34" s="56"/>
-      <c r="M34" s="56"/>
-      <c r="N34" s="56"/>
-      <c r="O34" s="56"/>
-      <c r="P34" s="56"/>
+      <c r="D34" s="61"/>
+      <c r="E34" s="61"/>
+      <c r="F34" s="61"/>
+      <c r="G34" s="61"/>
+      <c r="H34" s="61"/>
+      <c r="I34" s="61"/>
+      <c r="J34" s="61"/>
+      <c r="K34" s="61"/>
+      <c r="L34" s="61"/>
+      <c r="M34" s="61"/>
+      <c r="N34" s="61"/>
+      <c r="O34" s="61"/>
+      <c r="P34" s="61"/>
       <c r="S34" s="31"/>
     </row>
     <row r="35" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.25">
@@ -2211,97 +2313,97 @@
       <c r="P36" s="38"/>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A37" s="57" t="str">
+      <c r="A37" s="62" t="str">
         <f>CONCATENATE("participant"," ",C9)</f>
         <v xml:space="preserve">participant </v>
       </c>
-      <c r="B37" s="58"/>
+      <c r="B37" s="63"/>
       <c r="C37" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="D37" s="59" t="s">
+      <c r="D37" s="64" t="s">
         <v>33</v>
       </c>
-      <c r="E37" s="60"/>
-      <c r="F37" s="60"/>
-      <c r="G37" s="60"/>
-      <c r="H37" s="60"/>
-      <c r="I37" s="60"/>
-      <c r="J37" s="60"/>
-      <c r="K37" s="60"/>
-      <c r="L37" s="60"/>
-      <c r="M37" s="60"/>
-      <c r="N37" s="60"/>
-      <c r="O37" s="60"/>
-      <c r="P37" s="60"/>
+      <c r="E37" s="65"/>
+      <c r="F37" s="65"/>
+      <c r="G37" s="65"/>
+      <c r="H37" s="65"/>
+      <c r="I37" s="65"/>
+      <c r="J37" s="65"/>
+      <c r="K37" s="65"/>
+      <c r="L37" s="65"/>
+      <c r="M37" s="65"/>
+      <c r="N37" s="65"/>
+      <c r="O37" s="65"/>
+      <c r="P37" s="65"/>
     </row>
     <row r="38" spans="1:19" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="51" t="s">
+      <c r="A38" s="56" t="s">
         <v>37</v>
       </c>
-      <c r="B38" s="51"/>
+      <c r="B38" s="56"/>
       <c r="C38" s="35"/>
-      <c r="D38" s="55" t="s">
+      <c r="D38" s="60" t="s">
         <v>69</v>
       </c>
-      <c r="E38" s="56"/>
-      <c r="F38" s="56"/>
-      <c r="G38" s="56"/>
-      <c r="H38" s="56"/>
-      <c r="I38" s="56"/>
-      <c r="J38" s="56"/>
-      <c r="K38" s="56"/>
-      <c r="L38" s="56"/>
-      <c r="M38" s="56"/>
-      <c r="N38" s="56"/>
-      <c r="O38" s="56"/>
-      <c r="P38" s="56"/>
+      <c r="E38" s="61"/>
+      <c r="F38" s="61"/>
+      <c r="G38" s="61"/>
+      <c r="H38" s="61"/>
+      <c r="I38" s="61"/>
+      <c r="J38" s="61"/>
+      <c r="K38" s="61"/>
+      <c r="L38" s="61"/>
+      <c r="M38" s="61"/>
+      <c r="N38" s="61"/>
+      <c r="O38" s="61"/>
+      <c r="P38" s="61"/>
       <c r="S38" s="31"/>
     </row>
     <row r="39" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="51" t="s">
+      <c r="A39" s="56" t="s">
         <v>38</v>
       </c>
-      <c r="B39" s="51"/>
+      <c r="B39" s="56"/>
       <c r="C39" s="35"/>
-      <c r="D39" s="52" t="s">
+      <c r="D39" s="57" t="s">
         <v>39</v>
       </c>
-      <c r="E39" s="53"/>
-      <c r="F39" s="53"/>
-      <c r="G39" s="53"/>
-      <c r="H39" s="53"/>
-      <c r="I39" s="53"/>
-      <c r="J39" s="53"/>
-      <c r="K39" s="53"/>
-      <c r="L39" s="53"/>
-      <c r="M39" s="53"/>
-      <c r="N39" s="53"/>
-      <c r="O39" s="53"/>
-      <c r="P39" s="54"/>
+      <c r="E39" s="58"/>
+      <c r="F39" s="58"/>
+      <c r="G39" s="58"/>
+      <c r="H39" s="58"/>
+      <c r="I39" s="58"/>
+      <c r="J39" s="58"/>
+      <c r="K39" s="58"/>
+      <c r="L39" s="58"/>
+      <c r="M39" s="58"/>
+      <c r="N39" s="58"/>
+      <c r="O39" s="58"/>
+      <c r="P39" s="59"/>
       <c r="S39" s="31"/>
     </row>
     <row r="40" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="51" t="s">
+      <c r="A40" s="56" t="s">
         <v>40</v>
       </c>
-      <c r="B40" s="51"/>
+      <c r="B40" s="56"/>
       <c r="C40" s="35"/>
-      <c r="D40" s="55" t="s">
+      <c r="D40" s="60" t="s">
         <v>41</v>
       </c>
-      <c r="E40" s="56"/>
-      <c r="F40" s="56"/>
-      <c r="G40" s="56"/>
-      <c r="H40" s="56"/>
-      <c r="I40" s="56"/>
-      <c r="J40" s="56"/>
-      <c r="K40" s="56"/>
-      <c r="L40" s="56"/>
-      <c r="M40" s="56"/>
-      <c r="N40" s="56"/>
-      <c r="O40" s="56"/>
-      <c r="P40" s="56"/>
+      <c r="E40" s="61"/>
+      <c r="F40" s="61"/>
+      <c r="G40" s="61"/>
+      <c r="H40" s="61"/>
+      <c r="I40" s="61"/>
+      <c r="J40" s="61"/>
+      <c r="K40" s="61"/>
+      <c r="L40" s="61"/>
+      <c r="M40" s="61"/>
+      <c r="N40" s="61"/>
+      <c r="O40" s="61"/>
+      <c r="P40" s="61"/>
       <c r="S40" s="31"/>
     </row>
   </sheetData>
@@ -2357,7 +2459,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O6" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"70%, 100%"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2369,11 +2471,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:P36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="B1:P44"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28:E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2386,13 +2488,13 @@
   <sheetData>
     <row r="1" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="74" t="s">
+      <c r="B2" s="79" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="75"/>
+      <c r="C2" s="80"/>
       <c r="D2" s="43">
-        <f>SUM(P5:P36)</f>
-        <v>66660</v>
+        <f>SUM(P5:P44)</f>
+        <v>108760</v>
       </c>
     </row>
     <row r="4" spans="2:16" ht="162" x14ac:dyDescent="0.25">
@@ -2443,981 +2545,1128 @@
       </c>
     </row>
     <row r="5" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="52" t="s">
         <v>72</v>
       </c>
-      <c r="C5" s="39"/>
-      <c r="D5" s="50" t="s">
+      <c r="C5" s="52"/>
+      <c r="D5" s="53" t="s">
         <v>73</v>
       </c>
-      <c r="E5" s="39" t="s">
+      <c r="E5" s="52" t="s">
         <v>75</v>
       </c>
-      <c r="F5" s="39" t="s">
+      <c r="F5" s="52" t="s">
         <v>74</v>
       </c>
-      <c r="G5" s="39" t="s">
+      <c r="G5" s="52" t="s">
         <v>85</v>
       </c>
-      <c r="H5" s="39"/>
-      <c r="I5" s="39">
-        <v>1</v>
-      </c>
-      <c r="J5" s="39"/>
-      <c r="K5" s="39">
-        <v>1</v>
-      </c>
-      <c r="L5" s="39"/>
-      <c r="M5" s="39">
+      <c r="H5" s="52"/>
+      <c r="I5" s="52">
+        <v>1</v>
+      </c>
+      <c r="J5" s="52"/>
+      <c r="K5" s="52">
+        <v>1</v>
+      </c>
+      <c r="L5" s="52"/>
+      <c r="M5" s="52">
         <v>5</v>
       </c>
-      <c r="N5" s="39">
+      <c r="N5" s="52">
         <v>2000</v>
       </c>
-      <c r="O5" s="39">
+      <c r="O5" s="52">
         <v>620</v>
       </c>
-      <c r="P5" s="39">
+      <c r="P5" s="52">
         <f>N5+O5</f>
         <v>2620</v>
       </c>
     </row>
     <row r="6" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="52" t="s">
         <v>72</v>
       </c>
-      <c r="C6" s="39"/>
-      <c r="D6" s="50" t="s">
+      <c r="C6" s="52"/>
+      <c r="D6" s="53" t="s">
         <v>76</v>
       </c>
-      <c r="E6" s="39" t="s">
+      <c r="E6" s="52" t="s">
         <v>82</v>
       </c>
-      <c r="F6" s="39" t="s">
+      <c r="F6" s="52" t="s">
         <v>81</v>
       </c>
-      <c r="G6" s="47" t="s">
+      <c r="G6" s="52" t="s">
         <v>85</v>
       </c>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39"/>
-      <c r="J6" s="39">
-        <v>1</v>
-      </c>
-      <c r="K6" s="39"/>
-      <c r="L6" s="39">
-        <v>1</v>
-      </c>
-      <c r="M6" s="39">
+      <c r="H6" s="52"/>
+      <c r="I6" s="52"/>
+      <c r="J6" s="52">
+        <v>1</v>
+      </c>
+      <c r="K6" s="52"/>
+      <c r="L6" s="52">
+        <v>1</v>
+      </c>
+      <c r="M6" s="52">
         <v>5</v>
       </c>
-      <c r="N6" s="39">
+      <c r="N6" s="52">
         <v>1200</v>
       </c>
-      <c r="O6" s="39">
+      <c r="O6" s="52">
         <v>620</v>
       </c>
-      <c r="P6" s="39">
-        <f t="shared" ref="P6:P36" si="0">N6+O6</f>
+      <c r="P6" s="52">
+        <f t="shared" ref="P6:P25" si="0">N6+O6</f>
         <v>1820</v>
       </c>
     </row>
     <row r="7" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="47" t="s">
+      <c r="B7" s="52" t="s">
         <v>72</v>
       </c>
-      <c r="C7" s="39"/>
-      <c r="D7" s="50" t="s">
+      <c r="C7" s="52"/>
+      <c r="D7" s="54" t="s">
         <v>77</v>
       </c>
-      <c r="E7" s="39" t="s">
+      <c r="E7" s="52" t="s">
         <v>84</v>
       </c>
-      <c r="F7" s="39" t="s">
+      <c r="F7" s="52" t="s">
         <v>83</v>
       </c>
-      <c r="G7" s="47" t="s">
+      <c r="G7" s="52" t="s">
         <v>85</v>
       </c>
-      <c r="H7" s="39">
-        <v>1</v>
-      </c>
-      <c r="I7" s="39"/>
-      <c r="J7" s="39">
-        <v>1</v>
-      </c>
-      <c r="K7" s="39"/>
-      <c r="L7" s="39"/>
-      <c r="M7" s="39">
+      <c r="H7" s="52">
+        <v>1</v>
+      </c>
+      <c r="I7" s="52"/>
+      <c r="J7" s="52">
+        <v>1</v>
+      </c>
+      <c r="K7" s="52"/>
+      <c r="L7" s="52"/>
+      <c r="M7" s="52">
         <v>5</v>
       </c>
-      <c r="N7" s="39">
+      <c r="N7" s="52">
         <v>2000</v>
       </c>
-      <c r="O7" s="39">
+      <c r="O7" s="52">
         <v>620</v>
       </c>
-      <c r="P7" s="39">
+      <c r="P7" s="52">
         <f t="shared" si="0"/>
         <v>2620</v>
       </c>
     </row>
     <row r="8" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="47" t="s">
+      <c r="B8" s="52" t="s">
         <v>72</v>
       </c>
-      <c r="C8" s="39"/>
-      <c r="D8" s="50" t="s">
+      <c r="C8" s="52"/>
+      <c r="D8" s="54" t="s">
         <v>78</v>
       </c>
-      <c r="E8" s="39" t="s">
+      <c r="E8" s="52" t="s">
         <v>84</v>
       </c>
-      <c r="F8" s="39" t="s">
+      <c r="F8" s="52" t="s">
         <v>86</v>
       </c>
-      <c r="G8" s="47" t="s">
+      <c r="G8" s="52" t="s">
         <v>85</v>
       </c>
-      <c r="H8" s="39"/>
-      <c r="I8" s="39"/>
-      <c r="J8" s="39">
+      <c r="H8" s="52"/>
+      <c r="I8" s="52"/>
+      <c r="J8" s="52">
         <v>2</v>
       </c>
-      <c r="K8" s="39"/>
-      <c r="L8" s="39"/>
-      <c r="M8" s="39">
+      <c r="K8" s="52"/>
+      <c r="L8" s="52"/>
+      <c r="M8" s="52">
         <v>5</v>
       </c>
-      <c r="N8" s="39">
+      <c r="N8" s="52">
         <v>2000</v>
       </c>
-      <c r="O8" s="39">
+      <c r="O8" s="52">
         <v>620</v>
       </c>
-      <c r="P8" s="39">
+      <c r="P8" s="52">
         <f t="shared" si="0"/>
         <v>2620</v>
       </c>
     </row>
-    <row r="9" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="47" t="s">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B9" s="52" t="s">
         <v>72</v>
       </c>
-      <c r="C9" s="39"/>
-      <c r="D9" s="50" t="s">
+      <c r="C9" s="52"/>
+      <c r="D9" s="52" t="s">
         <v>79</v>
       </c>
-      <c r="E9" s="39" t="s">
+      <c r="E9" s="52" t="s">
         <v>87</v>
       </c>
-      <c r="F9" s="39" t="s">
+      <c r="F9" s="52" t="s">
         <v>88</v>
       </c>
-      <c r="G9" s="47" t="s">
+      <c r="G9" s="52" t="s">
         <v>85</v>
       </c>
-      <c r="H9" s="39"/>
-      <c r="I9" s="39"/>
-      <c r="J9" s="39">
+      <c r="H9" s="52"/>
+      <c r="I9" s="52"/>
+      <c r="J9" s="52">
         <v>2</v>
       </c>
-      <c r="K9" s="39"/>
-      <c r="L9" s="39"/>
-      <c r="M9" s="39">
+      <c r="K9" s="52"/>
+      <c r="L9" s="52"/>
+      <c r="M9" s="52">
         <v>5</v>
       </c>
-      <c r="N9" s="39">
+      <c r="N9" s="52">
         <v>1200</v>
       </c>
-      <c r="O9" s="39">
+      <c r="O9" s="52">
         <v>620</v>
       </c>
-      <c r="P9" s="39">
+      <c r="P9" s="52">
         <f t="shared" si="0"/>
         <v>1820</v>
       </c>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B10" s="47" t="s">
+      <c r="B10" s="52" t="s">
         <v>72</v>
       </c>
-      <c r="C10" s="39"/>
-      <c r="D10" s="39" t="s">
+      <c r="C10" s="52"/>
+      <c r="D10" s="52" t="s">
         <v>80</v>
       </c>
-      <c r="E10" s="39" t="s">
+      <c r="E10" s="52" t="s">
         <v>89</v>
       </c>
-      <c r="F10" s="39" t="s">
+      <c r="F10" s="52" t="s">
         <v>90</v>
       </c>
-      <c r="G10" s="47" t="s">
+      <c r="G10" s="52" t="s">
         <v>85</v>
       </c>
-      <c r="H10" s="39">
-        <v>1</v>
-      </c>
-      <c r="I10" s="39">
-        <v>1</v>
-      </c>
-      <c r="J10" s="39"/>
-      <c r="K10" s="39"/>
-      <c r="L10" s="39"/>
-      <c r="M10" s="39">
+      <c r="H10" s="52">
+        <v>1</v>
+      </c>
+      <c r="I10" s="52">
+        <v>1</v>
+      </c>
+      <c r="J10" s="52"/>
+      <c r="K10" s="52"/>
+      <c r="L10" s="52"/>
+      <c r="M10" s="52">
         <v>5</v>
       </c>
-      <c r="N10" s="39">
+      <c r="N10" s="52">
         <v>1200</v>
       </c>
-      <c r="O10" s="39">
+      <c r="O10" s="52">
         <v>620</v>
       </c>
-      <c r="P10" s="39">
+      <c r="P10" s="52">
         <f t="shared" si="0"/>
         <v>1820</v>
       </c>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B11" s="47" t="s">
+    <row r="11" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="52" t="s">
+        <v>113</v>
+      </c>
+      <c r="C11" s="52"/>
+      <c r="D11" s="54" t="s">
+        <v>73</v>
+      </c>
+      <c r="E11" s="52" t="s">
+        <v>75</v>
+      </c>
+      <c r="F11" s="52" t="s">
+        <v>74</v>
+      </c>
+      <c r="G11" s="52" t="s">
+        <v>114</v>
+      </c>
+      <c r="H11" s="52">
+        <v>1</v>
+      </c>
+      <c r="I11" s="52">
+        <v>1</v>
+      </c>
+      <c r="J11" s="52"/>
+      <c r="K11" s="52"/>
+      <c r="L11" s="52"/>
+      <c r="M11" s="52">
+        <v>7</v>
+      </c>
+      <c r="N11" s="52">
+        <v>1600</v>
+      </c>
+      <c r="O11" s="52">
+        <v>1020</v>
+      </c>
+      <c r="P11" s="52">
+        <f t="shared" si="0"/>
+        <v>2620</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="52" t="s">
+        <v>113</v>
+      </c>
+      <c r="C12" s="52"/>
+      <c r="D12" s="54" t="s">
+        <v>76</v>
+      </c>
+      <c r="E12" s="52" t="s">
+        <v>82</v>
+      </c>
+      <c r="F12" s="52" t="s">
+        <v>81</v>
+      </c>
+      <c r="G12" s="52" t="s">
+        <v>114</v>
+      </c>
+      <c r="H12" s="52"/>
+      <c r="I12" s="52"/>
+      <c r="J12" s="52">
+        <v>1</v>
+      </c>
+      <c r="K12" s="52"/>
+      <c r="L12" s="52">
+        <v>1</v>
+      </c>
+      <c r="M12" s="52">
+        <v>7</v>
+      </c>
+      <c r="N12" s="52">
+        <v>1600</v>
+      </c>
+      <c r="O12" s="52">
+        <v>1020</v>
+      </c>
+      <c r="P12" s="52">
+        <f t="shared" si="0"/>
+        <v>2620</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="52" t="s">
+        <v>113</v>
+      </c>
+      <c r="C13" s="52"/>
+      <c r="D13" s="54" t="s">
+        <v>73</v>
+      </c>
+      <c r="E13" s="52" t="s">
+        <v>75</v>
+      </c>
+      <c r="F13" s="52" t="s">
+        <v>74</v>
+      </c>
+      <c r="G13" s="52" t="s">
+        <v>115</v>
+      </c>
+      <c r="H13" s="52">
+        <v>1</v>
+      </c>
+      <c r="I13" s="52">
+        <v>1</v>
+      </c>
+      <c r="J13" s="52"/>
+      <c r="K13" s="52"/>
+      <c r="L13" s="52"/>
+      <c r="M13" s="52">
+        <v>7</v>
+      </c>
+      <c r="N13" s="52">
+        <v>1600</v>
+      </c>
+      <c r="O13" s="52">
+        <v>1620</v>
+      </c>
+      <c r="P13" s="52">
+        <f t="shared" si="0"/>
+        <v>3220</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B14" s="52" t="s">
+        <v>113</v>
+      </c>
+      <c r="C14" s="52"/>
+      <c r="D14" s="54" t="s">
+        <v>76</v>
+      </c>
+      <c r="E14" s="52" t="s">
+        <v>82</v>
+      </c>
+      <c r="F14" s="52" t="s">
+        <v>81</v>
+      </c>
+      <c r="G14" s="52" t="s">
+        <v>115</v>
+      </c>
+      <c r="H14" s="52"/>
+      <c r="I14" s="52"/>
+      <c r="J14" s="52">
+        <v>1</v>
+      </c>
+      <c r="K14" s="52"/>
+      <c r="L14" s="52">
+        <v>1</v>
+      </c>
+      <c r="M14" s="52">
+        <v>7</v>
+      </c>
+      <c r="N14" s="52">
+        <v>1600</v>
+      </c>
+      <c r="O14" s="52">
+        <v>1620</v>
+      </c>
+      <c r="P14" s="52">
+        <f t="shared" si="0"/>
+        <v>3220</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B15" s="52" t="s">
         <v>91</v>
       </c>
-      <c r="C11" s="39" t="s">
+      <c r="C15" s="52" t="s">
         <v>92</v>
       </c>
-      <c r="D11" s="39" t="s">
+      <c r="D15" s="52" t="s">
         <v>94</v>
       </c>
-      <c r="E11" s="39" t="s">
+      <c r="E15" s="52" t="s">
         <v>93</v>
       </c>
-      <c r="F11" s="39" t="s">
+      <c r="F15" s="52" t="s">
         <v>85</v>
       </c>
-      <c r="G11" s="39" t="s">
+      <c r="G15" s="52" t="s">
         <v>83</v>
       </c>
-      <c r="H11" s="39">
+      <c r="H15" s="52">
         <v>2</v>
       </c>
-      <c r="I11" s="39">
-        <v>1</v>
-      </c>
-      <c r="J11" s="39">
+      <c r="I15" s="52">
+        <v>1</v>
+      </c>
+      <c r="J15" s="52">
         <v>2</v>
       </c>
-      <c r="K11" s="39">
-        <v>1</v>
-      </c>
-      <c r="L11" s="39"/>
-      <c r="M11" s="39">
+      <c r="K15" s="52">
+        <v>1</v>
+      </c>
+      <c r="L15" s="52"/>
+      <c r="M15" s="52">
+        <v>10</v>
+      </c>
+      <c r="N15" s="52">
+        <v>6000</v>
+      </c>
+      <c r="O15" s="52">
+        <v>6660</v>
+      </c>
+      <c r="P15" s="52">
+        <f t="shared" si="0"/>
+        <v>12660</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B16" s="52" t="s">
+        <v>91</v>
+      </c>
+      <c r="C16" s="52"/>
+      <c r="D16" s="52" t="s">
+        <v>80</v>
+      </c>
+      <c r="E16" s="52" t="s">
+        <v>89</v>
+      </c>
+      <c r="F16" s="52" t="s">
+        <v>90</v>
+      </c>
+      <c r="G16" s="52" t="s">
+        <v>83</v>
+      </c>
+      <c r="H16" s="52">
+        <v>1</v>
+      </c>
+      <c r="I16" s="52"/>
+      <c r="J16" s="52">
+        <v>1</v>
+      </c>
+      <c r="K16" s="52"/>
+      <c r="L16" s="52"/>
+      <c r="M16" s="52">
+        <v>10</v>
+      </c>
+      <c r="N16" s="52">
+        <v>1600</v>
+      </c>
+      <c r="O16" s="52">
+        <v>2220</v>
+      </c>
+      <c r="P16" s="52">
+        <f t="shared" si="0"/>
+        <v>3820</v>
+      </c>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B17" s="52" t="s">
+        <v>95</v>
+      </c>
+      <c r="C17" s="52" t="s">
+        <v>92</v>
+      </c>
+      <c r="D17" s="52" t="s">
+        <v>94</v>
+      </c>
+      <c r="E17" s="52" t="s">
+        <v>93</v>
+      </c>
+      <c r="F17" s="52" t="s">
+        <v>85</v>
+      </c>
+      <c r="G17" s="52" t="s">
+        <v>90</v>
+      </c>
+      <c r="H17" s="52">
+        <v>2</v>
+      </c>
+      <c r="I17" s="52">
+        <v>1</v>
+      </c>
+      <c r="J17" s="52">
+        <v>2</v>
+      </c>
+      <c r="K17" s="52">
+        <v>1</v>
+      </c>
+      <c r="L17" s="52"/>
+      <c r="M17" s="52">
         <v>7</v>
       </c>
-      <c r="N11" s="39">
+      <c r="N17" s="52">
+        <v>4200</v>
+      </c>
+      <c r="O17" s="52">
+        <v>5460</v>
+      </c>
+      <c r="P17" s="52">
+        <f t="shared" si="0"/>
+        <v>9660</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B18" s="52" t="s">
+        <v>96</v>
+      </c>
+      <c r="C18" s="52" t="s">
+        <v>92</v>
+      </c>
+      <c r="D18" s="52" t="s">
+        <v>94</v>
+      </c>
+      <c r="E18" s="52" t="s">
+        <v>93</v>
+      </c>
+      <c r="F18" s="52" t="s">
+        <v>85</v>
+      </c>
+      <c r="G18" s="52" t="s">
+        <v>97</v>
+      </c>
+      <c r="H18" s="52">
+        <v>1</v>
+      </c>
+      <c r="I18" s="52"/>
+      <c r="J18" s="52">
+        <v>1</v>
+      </c>
+      <c r="K18" s="52"/>
+      <c r="L18" s="52">
+        <v>2</v>
+      </c>
+      <c r="M18" s="52">
+        <v>10</v>
+      </c>
+      <c r="N18" s="52">
+        <v>4000</v>
+      </c>
+      <c r="O18" s="52">
+        <v>4080</v>
+      </c>
+      <c r="P18" s="52">
+        <f t="shared" si="0"/>
+        <v>8080</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B19" s="52" t="s">
+        <v>96</v>
+      </c>
+      <c r="C19" s="52" t="s">
+        <v>92</v>
+      </c>
+      <c r="D19" s="52" t="s">
+        <v>94</v>
+      </c>
+      <c r="E19" s="52" t="s">
+        <v>93</v>
+      </c>
+      <c r="F19" s="52" t="s">
+        <v>85</v>
+      </c>
+      <c r="G19" s="52" t="s">
+        <v>98</v>
+      </c>
+      <c r="H19" s="52"/>
+      <c r="I19" s="52"/>
+      <c r="J19" s="52"/>
+      <c r="K19" s="52"/>
+      <c r="L19" s="52">
+        <v>2</v>
+      </c>
+      <c r="M19" s="52">
+        <v>10</v>
+      </c>
+      <c r="N19" s="52">
+        <v>1600</v>
+      </c>
+      <c r="O19" s="52">
+        <v>1680</v>
+      </c>
+      <c r="P19" s="52">
+        <f t="shared" si="0"/>
+        <v>3280</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B20" s="52" t="s">
+        <v>96</v>
+      </c>
+      <c r="C20" s="52"/>
+      <c r="D20" s="52" t="s">
+        <v>80</v>
+      </c>
+      <c r="E20" s="52" t="s">
+        <v>89</v>
+      </c>
+      <c r="F20" s="52" t="s">
+        <v>90</v>
+      </c>
+      <c r="G20" s="52" t="s">
+        <v>98</v>
+      </c>
+      <c r="H20" s="52">
+        <v>1</v>
+      </c>
+      <c r="I20" s="52"/>
+      <c r="J20" s="52">
+        <v>1</v>
+      </c>
+      <c r="K20" s="52"/>
+      <c r="L20" s="52"/>
+      <c r="M20" s="52">
+        <v>10</v>
+      </c>
+      <c r="N20" s="52">
+        <v>1200</v>
+      </c>
+      <c r="O20" s="52">
+        <v>1680</v>
+      </c>
+      <c r="P20" s="52">
+        <f t="shared" si="0"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B21" s="52" t="s">
+        <v>96</v>
+      </c>
+      <c r="C21" s="52" t="s">
+        <v>92</v>
+      </c>
+      <c r="D21" s="52" t="s">
+        <v>94</v>
+      </c>
+      <c r="E21" s="52" t="s">
+        <v>93</v>
+      </c>
+      <c r="F21" s="52" t="s">
+        <v>85</v>
+      </c>
+      <c r="G21" s="52" t="s">
+        <v>99</v>
+      </c>
+      <c r="H21" s="52">
+        <v>1</v>
+      </c>
+      <c r="I21" s="52"/>
+      <c r="J21" s="52"/>
+      <c r="K21" s="52"/>
+      <c r="L21" s="52">
+        <v>1</v>
+      </c>
+      <c r="M21" s="52">
+        <v>7</v>
+      </c>
+      <c r="N21" s="52">
+        <v>1200</v>
+      </c>
+      <c r="O21" s="52">
+        <v>900</v>
+      </c>
+      <c r="P21" s="52">
+        <f t="shared" si="0"/>
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B22" s="52" t="s">
+        <v>96</v>
+      </c>
+      <c r="C22" s="52"/>
+      <c r="D22" s="54" t="s">
+        <v>77</v>
+      </c>
+      <c r="E22" s="52" t="s">
+        <v>84</v>
+      </c>
+      <c r="F22" s="52" t="s">
+        <v>83</v>
+      </c>
+      <c r="G22" s="52" t="s">
+        <v>99</v>
+      </c>
+      <c r="H22" s="52"/>
+      <c r="I22" s="52"/>
+      <c r="J22" s="52">
+        <v>2</v>
+      </c>
+      <c r="K22" s="52"/>
+      <c r="L22" s="52"/>
+      <c r="M22" s="52">
+        <v>7</v>
+      </c>
+      <c r="N22" s="52">
+        <v>2000</v>
+      </c>
+      <c r="O22" s="52">
+        <v>900</v>
+      </c>
+      <c r="P22" s="52">
+        <f t="shared" si="0"/>
+        <v>2900</v>
+      </c>
+    </row>
+    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B23" s="52" t="s">
+        <v>96</v>
+      </c>
+      <c r="C23" s="52" t="s">
+        <v>92</v>
+      </c>
+      <c r="D23" s="52" t="s">
+        <v>94</v>
+      </c>
+      <c r="E23" s="52" t="s">
+        <v>93</v>
+      </c>
+      <c r="F23" s="52" t="s">
+        <v>85</v>
+      </c>
+      <c r="G23" s="52" t="s">
+        <v>116</v>
+      </c>
+      <c r="H23" s="52">
+        <v>1</v>
+      </c>
+      <c r="I23" s="52"/>
+      <c r="J23" s="52">
+        <v>1</v>
+      </c>
+      <c r="K23" s="52"/>
+      <c r="L23" s="52">
+        <v>2</v>
+      </c>
+      <c r="M23" s="52">
+        <v>10</v>
+      </c>
+      <c r="N23" s="52">
+        <v>4000</v>
+      </c>
+      <c r="O23" s="52">
+        <v>5520</v>
+      </c>
+      <c r="P23" s="52">
+        <f t="shared" si="0"/>
+        <v>9520</v>
+      </c>
+    </row>
+    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B24" s="52" t="s">
+        <v>96</v>
+      </c>
+      <c r="C24" s="52"/>
+      <c r="D24" s="52" t="s">
+        <v>80</v>
+      </c>
+      <c r="E24" s="52" t="s">
+        <v>89</v>
+      </c>
+      <c r="F24" s="52" t="s">
+        <v>90</v>
+      </c>
+      <c r="G24" s="52" t="s">
+        <v>116</v>
+      </c>
+      <c r="H24" s="52">
+        <v>1</v>
+      </c>
+      <c r="I24" s="52"/>
+      <c r="J24" s="52">
+        <v>1</v>
+      </c>
+      <c r="K24" s="52"/>
+      <c r="L24" s="52"/>
+      <c r="M24" s="52">
+        <v>10</v>
+      </c>
+      <c r="N24" s="52">
+        <v>1200</v>
+      </c>
+      <c r="O24" s="52">
+        <v>2760</v>
+      </c>
+      <c r="P24" s="52">
+        <f t="shared" si="0"/>
+        <v>3960</v>
+      </c>
+    </row>
+    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B25" s="52" t="s">
+        <v>96</v>
+      </c>
+      <c r="C25" s="52" t="s">
+        <v>92</v>
+      </c>
+      <c r="D25" s="52" t="s">
+        <v>94</v>
+      </c>
+      <c r="E25" s="52" t="s">
+        <v>93</v>
+      </c>
+      <c r="F25" s="52" t="s">
+        <v>85</v>
+      </c>
+      <c r="G25" s="52" t="s">
+        <v>117</v>
+      </c>
+      <c r="H25" s="52">
+        <v>2</v>
+      </c>
+      <c r="I25" s="52">
+        <v>1</v>
+      </c>
+      <c r="J25" s="52">
+        <v>2</v>
+      </c>
+      <c r="K25" s="52">
+        <v>1</v>
+      </c>
+      <c r="L25" s="52"/>
+      <c r="M25" s="52">
+        <v>10</v>
+      </c>
+      <c r="N25" s="52">
         <v>6000</v>
       </c>
-      <c r="O11" s="39">
-        <v>4260</v>
-      </c>
-      <c r="P11" s="39">
-        <f t="shared" si="0"/>
-        <v>10260</v>
-      </c>
-    </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="47" t="s">
-        <v>91</v>
-      </c>
-      <c r="C12" s="47"/>
-      <c r="D12" s="47" t="s">
-        <v>80</v>
-      </c>
-      <c r="E12" s="47" t="s">
-        <v>89</v>
-      </c>
-      <c r="F12" s="47" t="s">
-        <v>90</v>
-      </c>
-      <c r="G12" s="47" t="s">
+      <c r="O25" s="52">
+        <v>5580</v>
+      </c>
+      <c r="P25" s="52">
+        <f t="shared" si="0"/>
+        <v>11580</v>
+      </c>
+    </row>
+    <row r="26" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B26" s="50" t="s">
+        <v>72</v>
+      </c>
+      <c r="C26" s="50"/>
+      <c r="D26" s="55" t="s">
+        <v>73</v>
+      </c>
+      <c r="E26" s="50" t="s">
+        <v>75</v>
+      </c>
+      <c r="F26" s="50" t="s">
+        <v>74</v>
+      </c>
+      <c r="G26" s="50" t="s">
+        <v>85</v>
+      </c>
+      <c r="H26" s="50"/>
+      <c r="I26" s="50">
+        <v>1</v>
+      </c>
+      <c r="J26" s="50"/>
+      <c r="K26" s="50"/>
+      <c r="L26" s="50">
+        <v>1</v>
+      </c>
+      <c r="M26" s="50">
+        <v>5</v>
+      </c>
+      <c r="N26" s="50">
+        <v>2000</v>
+      </c>
+      <c r="O26" s="50">
+        <v>620</v>
+      </c>
+      <c r="P26" s="50">
+        <f>N26+O26</f>
+        <v>2620</v>
+      </c>
+    </row>
+    <row r="27" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B27" s="50" t="s">
+        <v>72</v>
+      </c>
+      <c r="C27" s="50"/>
+      <c r="D27" s="55" t="s">
+        <v>76</v>
+      </c>
+      <c r="E27" s="50" t="s">
+        <v>82</v>
+      </c>
+      <c r="F27" s="50" t="s">
+        <v>81</v>
+      </c>
+      <c r="G27" s="50" t="s">
+        <v>85</v>
+      </c>
+      <c r="H27" s="50"/>
+      <c r="I27" s="50"/>
+      <c r="J27" s="50">
+        <v>1</v>
+      </c>
+      <c r="K27" s="50"/>
+      <c r="L27" s="50">
+        <v>1</v>
+      </c>
+      <c r="M27" s="50">
+        <v>5</v>
+      </c>
+      <c r="N27" s="50">
+        <v>1200</v>
+      </c>
+      <c r="O27" s="50">
+        <v>620</v>
+      </c>
+      <c r="P27" s="50">
+        <f t="shared" ref="P27:P31" si="1">N27+O27</f>
+        <v>1820</v>
+      </c>
+    </row>
+    <row r="28" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B28" s="50" t="s">
+        <v>72</v>
+      </c>
+      <c r="C28" s="50"/>
+      <c r="D28" s="55" t="s">
+        <v>77</v>
+      </c>
+      <c r="E28" s="50" t="s">
+        <v>84</v>
+      </c>
+      <c r="F28" s="50" t="s">
         <v>83</v>
       </c>
-      <c r="H12" s="47">
-        <v>1</v>
-      </c>
-      <c r="I12" s="47"/>
-      <c r="J12" s="47">
-        <v>1</v>
-      </c>
-      <c r="K12" s="47"/>
-      <c r="L12" s="47"/>
-      <c r="M12" s="47">
-        <v>7</v>
-      </c>
-      <c r="N12" s="47">
-        <v>1600</v>
-      </c>
-      <c r="O12" s="47">
-        <v>1420</v>
-      </c>
-      <c r="P12" s="47">
-        <f t="shared" si="0"/>
-        <v>3020</v>
-      </c>
-    </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B13" s="39" t="s">
-        <v>95</v>
-      </c>
-      <c r="C13" s="39" t="s">
-        <v>92</v>
-      </c>
-      <c r="D13" s="47" t="s">
-        <v>94</v>
-      </c>
-      <c r="E13" s="47" t="s">
-        <v>93</v>
-      </c>
-      <c r="F13" s="47" t="s">
+      <c r="G28" s="50" t="s">
         <v>85</v>
       </c>
-      <c r="G13" s="47" t="s">
-        <v>90</v>
-      </c>
-      <c r="H13" s="39">
-        <v>2</v>
-      </c>
-      <c r="I13" s="39">
-        <v>1</v>
-      </c>
-      <c r="J13" s="39">
-        <v>2</v>
-      </c>
-      <c r="K13" s="39">
-        <v>1</v>
-      </c>
-      <c r="L13" s="39"/>
-      <c r="M13" s="39">
-        <v>7</v>
-      </c>
-      <c r="N13" s="39">
-        <v>4200</v>
-      </c>
-      <c r="O13" s="39">
-        <v>5460</v>
-      </c>
-      <c r="P13" s="39">
-        <f t="shared" si="0"/>
-        <v>9660</v>
-      </c>
-    </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B14" s="39" t="s">
-        <v>96</v>
-      </c>
-      <c r="C14" s="39" t="s">
-        <v>92</v>
-      </c>
-      <c r="D14" s="47" t="s">
-        <v>94</v>
-      </c>
-      <c r="E14" s="47" t="s">
-        <v>93</v>
-      </c>
-      <c r="F14" s="47" t="s">
-        <v>85</v>
-      </c>
-      <c r="G14" s="39" t="s">
-        <v>97</v>
-      </c>
-      <c r="H14" s="39">
-        <v>1</v>
-      </c>
-      <c r="I14" s="39"/>
-      <c r="J14" s="39">
-        <v>1</v>
-      </c>
-      <c r="K14" s="39"/>
-      <c r="L14" s="39">
-        <v>2</v>
-      </c>
-      <c r="M14" s="39">
-        <v>10</v>
-      </c>
-      <c r="N14" s="39">
-        <v>4000</v>
-      </c>
-      <c r="O14" s="39">
-        <v>4080</v>
-      </c>
-      <c r="P14" s="39">
-        <f t="shared" si="0"/>
-        <v>8080</v>
-      </c>
-    </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B15" s="47" t="s">
-        <v>96</v>
-      </c>
-      <c r="C15" s="47" t="s">
-        <v>92</v>
-      </c>
-      <c r="D15" s="47" t="s">
-        <v>94</v>
-      </c>
-      <c r="E15" s="47" t="s">
-        <v>93</v>
-      </c>
-      <c r="F15" s="47" t="s">
-        <v>85</v>
-      </c>
-      <c r="G15" s="39" t="s">
-        <v>98</v>
-      </c>
-      <c r="H15" s="39"/>
-      <c r="I15" s="39"/>
-      <c r="J15" s="39"/>
-      <c r="K15" s="39"/>
-      <c r="L15" s="39">
-        <v>2</v>
-      </c>
-      <c r="M15" s="39">
-        <v>4</v>
-      </c>
-      <c r="N15" s="39">
-        <v>1600</v>
-      </c>
-      <c r="O15" s="39">
-        <v>600</v>
-      </c>
-      <c r="P15" s="39">
-        <f t="shared" si="0"/>
-        <v>2200</v>
-      </c>
-    </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B16" s="47" t="s">
-        <v>96</v>
-      </c>
-      <c r="C16" s="47"/>
-      <c r="D16" s="47" t="s">
-        <v>80</v>
-      </c>
-      <c r="E16" s="47" t="s">
-        <v>89</v>
-      </c>
-      <c r="F16" s="47" t="s">
-        <v>90</v>
-      </c>
-      <c r="G16" s="47" t="s">
-        <v>98</v>
-      </c>
-      <c r="H16" s="39">
-        <v>1</v>
-      </c>
-      <c r="I16" s="39"/>
-      <c r="J16" s="39">
-        <v>1</v>
-      </c>
-      <c r="K16" s="39"/>
-      <c r="L16" s="39"/>
-      <c r="M16" s="39">
-        <v>4</v>
-      </c>
-      <c r="N16" s="39">
-        <v>1200</v>
-      </c>
-      <c r="O16" s="39">
-        <v>600</v>
-      </c>
-      <c r="P16" s="39">
-        <f t="shared" si="0"/>
-        <v>1800</v>
-      </c>
-    </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B17" s="47" t="s">
-        <v>96</v>
-      </c>
-      <c r="C17" s="47" t="s">
-        <v>92</v>
-      </c>
-      <c r="D17" s="47" t="s">
-        <v>94</v>
-      </c>
-      <c r="E17" s="47" t="s">
-        <v>93</v>
-      </c>
-      <c r="F17" s="47" t="s">
-        <v>85</v>
-      </c>
-      <c r="G17" s="39" t="s">
-        <v>99</v>
-      </c>
-      <c r="H17" s="39">
-        <v>1</v>
-      </c>
-      <c r="I17" s="39"/>
-      <c r="J17" s="39"/>
-      <c r="K17" s="39"/>
-      <c r="L17" s="39">
-        <v>1</v>
-      </c>
-      <c r="M17" s="39">
-        <v>7</v>
-      </c>
-      <c r="N17" s="39">
-        <v>1200</v>
-      </c>
-      <c r="O17" s="39">
-        <v>900</v>
-      </c>
-      <c r="P17" s="39">
-        <f t="shared" si="0"/>
-        <v>2100</v>
-      </c>
-    </row>
-    <row r="18" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="47" t="s">
-        <v>96</v>
-      </c>
-      <c r="C18" s="39"/>
-      <c r="D18" s="50" t="s">
-        <v>77</v>
-      </c>
-      <c r="E18" s="47" t="s">
-        <v>84</v>
-      </c>
-      <c r="F18" s="47" t="s">
-        <v>83</v>
-      </c>
-      <c r="G18" s="47" t="s">
-        <v>99</v>
-      </c>
-      <c r="H18" s="39"/>
-      <c r="I18" s="39"/>
-      <c r="J18" s="39">
-        <v>2</v>
-      </c>
-      <c r="K18" s="39"/>
-      <c r="L18" s="39"/>
-      <c r="M18" s="39">
-        <v>7</v>
-      </c>
-      <c r="N18" s="39">
+      <c r="H28" s="50">
+        <v>1</v>
+      </c>
+      <c r="I28" s="50"/>
+      <c r="J28" s="50">
+        <v>1</v>
+      </c>
+      <c r="K28" s="50"/>
+      <c r="L28" s="50"/>
+      <c r="M28" s="50">
+        <v>5</v>
+      </c>
+      <c r="N28" s="50">
         <v>2000</v>
       </c>
-      <c r="O18" s="39">
-        <v>900</v>
-      </c>
-      <c r="P18" s="39">
-        <f t="shared" si="0"/>
-        <v>2900</v>
-      </c>
-    </row>
-    <row r="19" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="47" t="s">
-        <v>72</v>
-      </c>
-      <c r="C19" s="47"/>
-      <c r="D19" s="50" t="s">
-        <v>73</v>
-      </c>
-      <c r="E19" s="47" t="s">
-        <v>75</v>
-      </c>
-      <c r="F19" s="47" t="s">
-        <v>74</v>
-      </c>
-      <c r="G19" s="47" t="s">
-        <v>85</v>
-      </c>
-      <c r="H19" s="47"/>
-      <c r="I19" s="47">
-        <v>1</v>
-      </c>
-      <c r="J19" s="47"/>
-      <c r="K19" s="47"/>
-      <c r="L19" s="47">
-        <v>1</v>
-      </c>
-      <c r="M19" s="47">
-        <v>5</v>
-      </c>
-      <c r="N19" s="47">
-        <v>2000</v>
-      </c>
-      <c r="O19" s="47">
+      <c r="O28" s="50">
         <v>620</v>
       </c>
-      <c r="P19" s="47">
-        <f>N19+O19</f>
-        <v>2620</v>
-      </c>
-    </row>
-    <row r="20" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B20" s="47" t="s">
-        <v>72</v>
-      </c>
-      <c r="C20" s="47"/>
-      <c r="D20" s="50" t="s">
-        <v>76</v>
-      </c>
-      <c r="E20" s="47" t="s">
-        <v>82</v>
-      </c>
-      <c r="F20" s="47" t="s">
-        <v>81</v>
-      </c>
-      <c r="G20" s="47" t="s">
-        <v>85</v>
-      </c>
-      <c r="H20" s="47"/>
-      <c r="I20" s="47"/>
-      <c r="J20" s="47">
-        <v>1</v>
-      </c>
-      <c r="K20" s="47"/>
-      <c r="L20" s="47">
-        <v>1</v>
-      </c>
-      <c r="M20" s="47">
-        <v>5</v>
-      </c>
-      <c r="N20" s="47">
-        <v>1200</v>
-      </c>
-      <c r="O20" s="47">
-        <v>620</v>
-      </c>
-      <c r="P20" s="47">
-        <f t="shared" ref="P20:P24" si="1">N20+O20</f>
-        <v>1820</v>
-      </c>
-    </row>
-    <row r="21" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="47" t="s">
-        <v>72</v>
-      </c>
-      <c r="C21" s="47"/>
-      <c r="D21" s="50" t="s">
-        <v>77</v>
-      </c>
-      <c r="E21" s="47" t="s">
-        <v>84</v>
-      </c>
-      <c r="F21" s="47" t="s">
-        <v>83</v>
-      </c>
-      <c r="G21" s="47" t="s">
-        <v>85</v>
-      </c>
-      <c r="H21" s="47">
-        <v>1</v>
-      </c>
-      <c r="I21" s="47"/>
-      <c r="J21" s="47">
-        <v>1</v>
-      </c>
-      <c r="K21" s="47"/>
-      <c r="L21" s="47"/>
-      <c r="M21" s="47">
-        <v>5</v>
-      </c>
-      <c r="N21" s="47">
-        <v>2000</v>
-      </c>
-      <c r="O21" s="47">
-        <v>620</v>
-      </c>
-      <c r="P21" s="47">
+      <c r="P28" s="50">
         <f t="shared" si="1"/>
         <v>2620</v>
       </c>
     </row>
-    <row r="22" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B22" s="47" t="s">
+    <row r="29" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B29" s="50" t="s">
         <v>72</v>
       </c>
-      <c r="C22" s="47"/>
-      <c r="D22" s="50" t="s">
+      <c r="C29" s="50"/>
+      <c r="D29" s="55" t="s">
         <v>78</v>
       </c>
-      <c r="E22" s="47" t="s">
+      <c r="E29" s="50" t="s">
         <v>84</v>
       </c>
-      <c r="F22" s="47" t="s">
+      <c r="F29" s="50" t="s">
         <v>86</v>
       </c>
-      <c r="G22" s="47" t="s">
+      <c r="G29" s="50" t="s">
         <v>85</v>
       </c>
-      <c r="H22" s="47"/>
-      <c r="I22" s="47"/>
-      <c r="J22" s="47">
-        <v>1</v>
-      </c>
-      <c r="K22" s="47"/>
-      <c r="L22" s="47">
-        <v>1</v>
-      </c>
-      <c r="M22" s="47">
+      <c r="H29" s="50"/>
+      <c r="I29" s="50"/>
+      <c r="J29" s="50">
+        <v>1</v>
+      </c>
+      <c r="K29" s="50"/>
+      <c r="L29" s="50">
+        <v>1</v>
+      </c>
+      <c r="M29" s="50">
         <v>5</v>
       </c>
-      <c r="N22" s="47">
+      <c r="N29" s="50">
         <v>2000</v>
       </c>
-      <c r="O22" s="47">
+      <c r="O29" s="50">
         <v>620</v>
       </c>
-      <c r="P22" s="47">
+      <c r="P29" s="50">
         <f t="shared" si="1"/>
         <v>2620</v>
       </c>
     </row>
-    <row r="23" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="47" t="s">
+    <row r="30" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B30" s="50" t="s">
         <v>72</v>
       </c>
-      <c r="C23" s="47"/>
-      <c r="D23" s="50" t="s">
+      <c r="C30" s="50"/>
+      <c r="D30" s="55" t="s">
         <v>79</v>
       </c>
-      <c r="E23" s="47" t="s">
+      <c r="E30" s="50" t="s">
         <v>87</v>
       </c>
-      <c r="F23" s="47" t="s">
+      <c r="F30" s="50" t="s">
         <v>88</v>
       </c>
-      <c r="G23" s="47" t="s">
+      <c r="G30" s="50" t="s">
         <v>85</v>
       </c>
-      <c r="H23" s="47"/>
-      <c r="I23" s="47"/>
-      <c r="J23" s="47">
-        <v>1</v>
-      </c>
-      <c r="K23" s="47"/>
-      <c r="L23" s="47">
-        <v>1</v>
-      </c>
-      <c r="M23" s="47">
+      <c r="H30" s="50"/>
+      <c r="I30" s="50"/>
+      <c r="J30" s="50">
+        <v>1</v>
+      </c>
+      <c r="K30" s="50"/>
+      <c r="L30" s="50">
+        <v>1</v>
+      </c>
+      <c r="M30" s="50">
         <v>5</v>
       </c>
-      <c r="N23" s="47">
+      <c r="N30" s="50">
         <v>1200</v>
       </c>
-      <c r="O23" s="47">
+      <c r="O30" s="50">
         <v>620</v>
       </c>
-      <c r="P23" s="47">
+      <c r="P30" s="50">
         <f t="shared" si="1"/>
         <v>1820</v>
       </c>
     </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B24" s="47" t="s">
+    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B31" s="50" t="s">
         <v>72</v>
       </c>
-      <c r="C24" s="47"/>
-      <c r="D24" s="47" t="s">
+      <c r="C31" s="50"/>
+      <c r="D31" s="50" t="s">
         <v>80</v>
       </c>
-      <c r="E24" s="47" t="s">
+      <c r="E31" s="50" t="s">
         <v>89</v>
       </c>
-      <c r="F24" s="47" t="s">
+      <c r="F31" s="50" t="s">
         <v>90</v>
       </c>
-      <c r="G24" s="47" t="s">
+      <c r="G31" s="50" t="s">
         <v>85</v>
       </c>
-      <c r="H24" s="47">
-        <v>1</v>
-      </c>
-      <c r="I24" s="47">
-        <v>1</v>
-      </c>
-      <c r="J24" s="47"/>
-      <c r="K24" s="47"/>
-      <c r="L24" s="47"/>
-      <c r="M24" s="47">
+      <c r="H31" s="50">
+        <v>1</v>
+      </c>
+      <c r="I31" s="50">
+        <v>1</v>
+      </c>
+      <c r="J31" s="50"/>
+      <c r="K31" s="50"/>
+      <c r="L31" s="50"/>
+      <c r="M31" s="50">
         <v>5</v>
       </c>
-      <c r="N24" s="47">
+      <c r="N31" s="50">
         <v>1200</v>
       </c>
-      <c r="O24" s="47">
+      <c r="O31" s="50">
         <v>620</v>
       </c>
-      <c r="P24" s="47">
+      <c r="P31" s="50">
         <f t="shared" si="1"/>
         <v>1820</v>
       </c>
     </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B25" s="39"/>
-      <c r="C25" s="39"/>
-      <c r="D25" s="39"/>
-      <c r="E25" s="39"/>
-      <c r="F25" s="39"/>
-      <c r="G25" s="39"/>
-      <c r="H25" s="39"/>
-      <c r="I25" s="39"/>
-      <c r="J25" s="39"/>
-      <c r="K25" s="39"/>
-      <c r="L25" s="39"/>
-      <c r="M25" s="39"/>
-      <c r="N25" s="39"/>
-      <c r="O25" s="39"/>
-      <c r="P25" s="39">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B26" s="39"/>
-      <c r="C26" s="39"/>
-      <c r="D26" s="39"/>
-      <c r="E26" s="39"/>
-      <c r="F26" s="39"/>
-      <c r="G26" s="39"/>
-      <c r="H26" s="39"/>
-      <c r="I26" s="39"/>
-      <c r="J26" s="39"/>
-      <c r="K26" s="39"/>
-      <c r="L26" s="39"/>
-      <c r="M26" s="39"/>
-      <c r="N26" s="39"/>
-      <c r="O26" s="39"/>
-      <c r="P26" s="39">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B27" s="39"/>
-      <c r="C27" s="39"/>
-      <c r="D27" s="39"/>
-      <c r="E27" s="39"/>
-      <c r="F27" s="39"/>
-      <c r="G27" s="39"/>
-      <c r="H27" s="39"/>
-      <c r="I27" s="39"/>
-      <c r="J27" s="39"/>
-      <c r="K27" s="39"/>
-      <c r="L27" s="39"/>
-      <c r="M27" s="39"/>
-      <c r="N27" s="39"/>
-      <c r="O27" s="39"/>
-      <c r="P27" s="39">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B28" s="39"/>
-      <c r="C28" s="39"/>
-      <c r="D28" s="39"/>
-      <c r="E28" s="39"/>
-      <c r="F28" s="39"/>
-      <c r="G28" s="39"/>
-      <c r="H28" s="39"/>
-      <c r="I28" s="39"/>
-      <c r="J28" s="39"/>
-      <c r="K28" s="39"/>
-      <c r="L28" s="39"/>
-      <c r="M28" s="39"/>
-      <c r="N28" s="39"/>
-      <c r="O28" s="39"/>
-      <c r="P28" s="39">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B29" s="39"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="39"/>
-      <c r="K29" s="39"/>
-      <c r="L29" s="39"/>
-      <c r="M29" s="39"/>
-      <c r="N29" s="39"/>
-      <c r="O29" s="39"/>
-      <c r="P29" s="39">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B30" s="39"/>
-      <c r="C30" s="39"/>
-      <c r="D30" s="39"/>
-      <c r="E30" s="39"/>
-      <c r="F30" s="39"/>
-      <c r="G30" s="39"/>
-      <c r="H30" s="39"/>
-      <c r="I30" s="39"/>
-      <c r="J30" s="39"/>
-      <c r="K30" s="39"/>
-      <c r="L30" s="39"/>
-      <c r="M30" s="39"/>
-      <c r="N30" s="39"/>
-      <c r="O30" s="39"/>
-      <c r="P30" s="39">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B31" s="39"/>
-      <c r="C31" s="39"/>
-      <c r="D31" s="39"/>
-      <c r="E31" s="39"/>
-      <c r="F31" s="39"/>
-      <c r="G31" s="39"/>
-      <c r="H31" s="39"/>
-      <c r="I31" s="39"/>
-      <c r="J31" s="39"/>
-      <c r="K31" s="39"/>
-      <c r="L31" s="39"/>
-      <c r="M31" s="39"/>
-      <c r="N31" s="39"/>
-      <c r="O31" s="39"/>
-      <c r="P31" s="39">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
     <row r="32" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B32" s="39"/>
-      <c r="C32" s="39"/>
-      <c r="D32" s="39"/>
-      <c r="E32" s="39"/>
-      <c r="F32" s="39"/>
-      <c r="G32" s="39"/>
-      <c r="H32" s="39"/>
-      <c r="I32" s="39"/>
-      <c r="J32" s="39"/>
-      <c r="K32" s="39"/>
-      <c r="L32" s="39"/>
-      <c r="M32" s="39"/>
-      <c r="N32" s="39"/>
-      <c r="O32" s="39"/>
-      <c r="P32" s="39">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="B32" s="47"/>
+      <c r="C32" s="47"/>
+      <c r="D32" s="50"/>
+      <c r="E32" s="47"/>
+      <c r="F32" s="47"/>
+      <c r="G32" s="47"/>
+      <c r="H32" s="47"/>
+      <c r="I32" s="47"/>
+      <c r="J32" s="47"/>
+      <c r="K32" s="47"/>
+      <c r="L32" s="47"/>
+      <c r="M32" s="47"/>
+      <c r="N32" s="47"/>
+      <c r="O32" s="47"/>
+      <c r="P32" s="47"/>
     </row>
     <row r="33" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B33" s="39"/>
       <c r="C33" s="39"/>
-      <c r="D33" s="39"/>
+      <c r="D33" s="50"/>
       <c r="E33" s="39"/>
       <c r="F33" s="39"/>
       <c r="G33" s="39"/>
@@ -3429,15 +3678,12 @@
       <c r="M33" s="39"/>
       <c r="N33" s="39"/>
       <c r="O33" s="39"/>
-      <c r="P33" s="39">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="P33" s="39"/>
     </row>
     <row r="34" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B34" s="39"/>
       <c r="C34" s="39"/>
-      <c r="D34" s="39"/>
+      <c r="D34" s="50"/>
       <c r="E34" s="39"/>
       <c r="F34" s="39"/>
       <c r="G34" s="39"/>
@@ -3449,50 +3695,177 @@
       <c r="M34" s="39"/>
       <c r="N34" s="39"/>
       <c r="O34" s="39"/>
-      <c r="P34" s="39">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="P34" s="39"/>
     </row>
     <row r="35" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B35" s="39"/>
-      <c r="C35" s="39"/>
-      <c r="D35" s="39"/>
-      <c r="E35" s="39"/>
-      <c r="F35" s="39"/>
-      <c r="G35" s="39"/>
-      <c r="H35" s="39"/>
-      <c r="I35" s="39"/>
-      <c r="J35" s="39"/>
-      <c r="K35" s="39"/>
-      <c r="L35" s="39"/>
-      <c r="M35" s="39"/>
-      <c r="N35" s="39"/>
-      <c r="O35" s="39"/>
-      <c r="P35" s="39">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="B35" s="50"/>
+      <c r="C35" s="50"/>
+      <c r="D35" s="50"/>
+      <c r="E35" s="50"/>
+      <c r="F35" s="50"/>
+      <c r="G35" s="50"/>
+      <c r="H35" s="50"/>
+      <c r="I35" s="50"/>
+      <c r="J35" s="50"/>
+      <c r="K35" s="50"/>
+      <c r="L35" s="50"/>
+      <c r="M35" s="50"/>
+      <c r="N35" s="50"/>
+      <c r="O35" s="50"/>
+      <c r="P35" s="50"/>
     </row>
     <row r="36" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B36" s="39"/>
-      <c r="C36" s="39"/>
-      <c r="D36" s="39"/>
-      <c r="E36" s="39"/>
-      <c r="F36" s="39"/>
-      <c r="G36" s="39"/>
-      <c r="H36" s="39"/>
-      <c r="I36" s="39"/>
-      <c r="J36" s="39"/>
-      <c r="K36" s="39"/>
-      <c r="L36" s="39"/>
-      <c r="M36" s="39"/>
-      <c r="N36" s="39"/>
-      <c r="O36" s="39"/>
-      <c r="P36" s="39">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="B36" s="50"/>
+      <c r="C36" s="50"/>
+      <c r="D36" s="50"/>
+      <c r="E36" s="50"/>
+      <c r="F36" s="50"/>
+      <c r="G36" s="50"/>
+      <c r="H36" s="50"/>
+      <c r="I36" s="50"/>
+      <c r="J36" s="50"/>
+      <c r="K36" s="50"/>
+      <c r="L36" s="50"/>
+      <c r="M36" s="50"/>
+      <c r="N36" s="50"/>
+      <c r="O36" s="50"/>
+      <c r="P36" s="50"/>
+    </row>
+    <row r="37" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B37" s="50"/>
+      <c r="C37" s="50"/>
+      <c r="D37" s="50"/>
+      <c r="E37" s="50"/>
+      <c r="F37" s="50"/>
+      <c r="G37" s="50"/>
+      <c r="H37" s="50"/>
+      <c r="I37" s="50"/>
+      <c r="J37" s="50"/>
+      <c r="K37" s="50"/>
+      <c r="L37" s="50"/>
+      <c r="M37" s="50"/>
+      <c r="N37" s="50"/>
+      <c r="O37" s="50"/>
+      <c r="P37" s="50"/>
+    </row>
+    <row r="38" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B38" s="50"/>
+      <c r="C38" s="50"/>
+      <c r="D38" s="50"/>
+      <c r="E38" s="50"/>
+      <c r="F38" s="50"/>
+      <c r="G38" s="50"/>
+      <c r="H38" s="50"/>
+      <c r="I38" s="50"/>
+      <c r="J38" s="50"/>
+      <c r="K38" s="50"/>
+      <c r="L38" s="50"/>
+      <c r="M38" s="50"/>
+      <c r="N38" s="50"/>
+      <c r="O38" s="50"/>
+      <c r="P38" s="50"/>
+    </row>
+    <row r="39" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B39" s="50"/>
+      <c r="C39" s="50"/>
+      <c r="D39" s="50"/>
+      <c r="E39" s="50"/>
+      <c r="F39" s="50"/>
+      <c r="G39" s="50"/>
+      <c r="H39" s="50"/>
+      <c r="I39" s="50"/>
+      <c r="J39" s="50"/>
+      <c r="K39" s="50"/>
+      <c r="L39" s="50"/>
+      <c r="M39" s="50"/>
+      <c r="N39" s="50"/>
+      <c r="O39" s="50"/>
+      <c r="P39" s="50"/>
+    </row>
+    <row r="40" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B40" s="50"/>
+      <c r="C40" s="50"/>
+      <c r="D40" s="50"/>
+      <c r="E40" s="50"/>
+      <c r="F40" s="50"/>
+      <c r="G40" s="50"/>
+      <c r="H40" s="50"/>
+      <c r="I40" s="50"/>
+      <c r="J40" s="50"/>
+      <c r="K40" s="50"/>
+      <c r="L40" s="50"/>
+      <c r="M40" s="50"/>
+      <c r="N40" s="50"/>
+      <c r="O40" s="50"/>
+      <c r="P40" s="50"/>
+    </row>
+    <row r="41" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B41" s="39"/>
+      <c r="C41" s="39"/>
+      <c r="D41" s="39"/>
+      <c r="E41" s="39"/>
+      <c r="F41" s="39"/>
+      <c r="G41" s="39"/>
+      <c r="H41" s="39"/>
+      <c r="I41" s="39"/>
+      <c r="J41" s="39"/>
+      <c r="K41" s="39"/>
+      <c r="L41" s="39"/>
+      <c r="M41" s="39"/>
+      <c r="N41" s="39"/>
+      <c r="O41" s="39"/>
+      <c r="P41" s="39"/>
+    </row>
+    <row r="42" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B42" s="39"/>
+      <c r="C42" s="39"/>
+      <c r="D42" s="39"/>
+      <c r="E42" s="39"/>
+      <c r="F42" s="39"/>
+      <c r="G42" s="39"/>
+      <c r="H42" s="39"/>
+      <c r="I42" s="39"/>
+      <c r="J42" s="39"/>
+      <c r="K42" s="39"/>
+      <c r="L42" s="39"/>
+      <c r="M42" s="39"/>
+      <c r="N42" s="39"/>
+      <c r="O42" s="39"/>
+      <c r="P42" s="39"/>
+    </row>
+    <row r="43" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B43" s="39"/>
+      <c r="C43" s="39"/>
+      <c r="D43" s="39"/>
+      <c r="E43" s="39"/>
+      <c r="F43" s="39"/>
+      <c r="G43" s="39"/>
+      <c r="H43" s="39"/>
+      <c r="I43" s="39"/>
+      <c r="J43" s="39"/>
+      <c r="K43" s="39"/>
+      <c r="L43" s="39"/>
+      <c r="M43" s="39"/>
+      <c r="N43" s="39"/>
+      <c r="O43" s="39"/>
+      <c r="P43" s="39"/>
+    </row>
+    <row r="44" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B44" s="39"/>
+      <c r="C44" s="39"/>
+      <c r="D44" s="39"/>
+      <c r="E44" s="39"/>
+      <c r="F44" s="39"/>
+      <c r="G44" s="39"/>
+      <c r="H44" s="39"/>
+      <c r="I44" s="39"/>
+      <c r="J44" s="39"/>
+      <c r="K44" s="39"/>
+      <c r="L44" s="39"/>
+      <c r="M44" s="39"/>
+      <c r="N44" s="39"/>
+      <c r="O44" s="39"/>
+      <c r="P44" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3504,11 +3877,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3523,13 +3896,13 @@
   <sheetData>
     <row r="1" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="74" t="s">
+      <c r="B2" s="79" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="75"/>
+      <c r="C2" s="80"/>
       <c r="D2" s="43">
         <f>SUM(I5:I35)</f>
-        <v>17120</v>
+        <v>20720</v>
       </c>
     </row>
     <row r="4" spans="2:9" ht="45" x14ac:dyDescent="0.25">
@@ -3726,14 +4099,14 @@
         <v>110</v>
       </c>
       <c r="G11" s="39">
-        <v>1000</v>
+        <v>1200</v>
       </c>
       <c r="H11" s="39">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I11" s="39">
         <f t="shared" si="0"/>
-        <v>3000</v>
+        <v>4800</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
@@ -3751,14 +4124,14 @@
         <v>111</v>
       </c>
       <c r="G12" s="39">
-        <v>1000</v>
+        <v>1200</v>
       </c>
       <c r="H12" s="39">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I12" s="39">
         <f t="shared" si="0"/>
-        <v>3000</v>
+        <v>4800</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
@@ -4109,31 +4482,31 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:I35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="B1:I36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18.5703125" customWidth="1"/>
-    <col min="4" max="4" width="22" customWidth="1"/>
-    <col min="6" max="6" width="38.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.7109375" customWidth="1"/>
+    <col min="6" max="6" width="70.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="34.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="74" t="s">
+      <c r="B2" s="79" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="75"/>
+      <c r="C2" s="80"/>
       <c r="D2" s="43">
         <f>SUM(I5:I35)</f>
-        <v>0</v>
+        <v>61200</v>
       </c>
     </row>
     <row r="4" spans="2:9" ht="45" x14ac:dyDescent="0.25">
@@ -4163,133 +4536,261 @@
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="39"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
+      <c r="B5" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="C5" s="51" t="s">
+        <v>92</v>
+      </c>
+      <c r="D5" s="51" t="s">
+        <v>94</v>
+      </c>
+      <c r="E5" s="51" t="s">
+        <v>100</v>
+      </c>
+      <c r="F5" s="39" t="s">
+        <v>118</v>
+      </c>
+      <c r="G5" s="39">
+        <v>140</v>
+      </c>
+      <c r="H5" s="39">
+        <v>5</v>
+      </c>
       <c r="I5" s="39">
         <f>G5*H5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="39"/>
+        <v>700</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="51" t="s">
+        <v>113</v>
+      </c>
       <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
+      <c r="D6" s="54" t="s">
+        <v>73</v>
+      </c>
+      <c r="E6" s="52" t="s">
+        <v>75</v>
+      </c>
+      <c r="F6" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="G6" s="39">
+        <v>40</v>
+      </c>
+      <c r="H6" s="39">
+        <v>5</v>
+      </c>
       <c r="I6" s="39">
-        <f t="shared" ref="I6:I35" si="0">G6*H6</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="39"/>
+        <f t="shared" ref="I6:I11" si="0">G6*H6</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="51" t="s">
+        <v>119</v>
+      </c>
       <c r="C7" s="39"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
-      <c r="G7" s="39"/>
-      <c r="H7" s="39"/>
+      <c r="D7" s="55" t="s">
+        <v>76</v>
+      </c>
+      <c r="E7" s="51" t="s">
+        <v>82</v>
+      </c>
+      <c r="F7" s="39" t="s">
+        <v>121</v>
+      </c>
+      <c r="G7" s="39">
+        <v>20</v>
+      </c>
+      <c r="H7" s="39">
+        <v>5</v>
+      </c>
       <c r="I7" s="39">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="39"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="51" t="s">
+        <v>123</v>
+      </c>
       <c r="C8" s="39"/>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="39"/>
-      <c r="H8" s="39"/>
+      <c r="D8" s="55" t="s">
+        <v>78</v>
+      </c>
+      <c r="E8" s="51" t="s">
+        <v>84</v>
+      </c>
+      <c r="F8" s="39" t="s">
+        <v>122</v>
+      </c>
+      <c r="G8" s="39">
+        <v>20</v>
+      </c>
+      <c r="H8" s="39">
+        <v>5</v>
+      </c>
       <c r="I8" s="39">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="39"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="51" t="s">
+        <v>125</v>
+      </c>
       <c r="C9" s="39"/>
-      <c r="D9" s="39"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="39"/>
-      <c r="H9" s="39"/>
+      <c r="D9" s="55" t="s">
+        <v>79</v>
+      </c>
+      <c r="E9" s="51" t="s">
+        <v>87</v>
+      </c>
+      <c r="F9" s="39" t="s">
+        <v>124</v>
+      </c>
+      <c r="G9" s="39">
+        <v>20</v>
+      </c>
+      <c r="H9" s="39">
+        <v>5</v>
+      </c>
       <c r="I9" s="39">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="39"/>
-      <c r="C10" s="39"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="39"/>
-      <c r="H10" s="39"/>
+      <c r="B10" s="39" t="s">
+        <v>127</v>
+      </c>
+      <c r="C10" s="51" t="s">
+        <v>92</v>
+      </c>
+      <c r="D10" s="51" t="s">
+        <v>94</v>
+      </c>
+      <c r="E10" s="51" t="s">
+        <v>100</v>
+      </c>
+      <c r="F10" s="39" t="s">
+        <v>126</v>
+      </c>
+      <c r="G10" s="39">
+        <v>30000</v>
+      </c>
+      <c r="H10" s="39">
+        <v>1</v>
+      </c>
       <c r="I10" s="39">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="39"/>
-      <c r="C11" s="39"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
-      <c r="G11" s="39"/>
-      <c r="H11" s="39"/>
+      <c r="B11" s="39" t="s">
+        <v>95</v>
+      </c>
+      <c r="C11" s="51" t="s">
+        <v>92</v>
+      </c>
+      <c r="D11" s="51" t="s">
+        <v>94</v>
+      </c>
+      <c r="E11" s="51" t="s">
+        <v>100</v>
+      </c>
+      <c r="F11" s="39" t="s">
+        <v>128</v>
+      </c>
+      <c r="G11" s="39">
+        <v>7000</v>
+      </c>
+      <c r="H11" s="39">
+        <v>1</v>
+      </c>
       <c r="I11" s="39">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="39"/>
-      <c r="C12" s="39"/>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="39"/>
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="51" t="s">
+        <v>91</v>
+      </c>
+      <c r="C12" s="51"/>
+      <c r="D12" s="55" t="s">
+        <v>77</v>
+      </c>
+      <c r="E12" s="51" t="s">
+        <v>84</v>
+      </c>
+      <c r="F12" s="51" t="s">
+        <v>128</v>
+      </c>
+      <c r="G12" s="51">
+        <v>7000</v>
+      </c>
+      <c r="H12" s="51">
+        <v>1</v>
+      </c>
       <c r="I12" s="39">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>G12*H12</f>
+        <v>7000</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="39"/>
-      <c r="C13" s="39"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="39"/>
-      <c r="G13" s="39"/>
-      <c r="H13" s="39"/>
+      <c r="B13" s="39" t="s">
+        <v>96</v>
+      </c>
+      <c r="C13" s="51" t="s">
+        <v>92</v>
+      </c>
+      <c r="D13" s="51" t="s">
+        <v>94</v>
+      </c>
+      <c r="E13" s="51" t="s">
+        <v>100</v>
+      </c>
+      <c r="F13" s="39" t="s">
+        <v>129</v>
+      </c>
+      <c r="G13" s="39">
+        <v>1000</v>
+      </c>
+      <c r="H13" s="39">
+        <v>1</v>
+      </c>
       <c r="I13" s="39">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="39"/>
-      <c r="C14" s="39"/>
-      <c r="D14" s="39"/>
-      <c r="E14" s="39"/>
-      <c r="F14" s="39"/>
-      <c r="G14" s="39"/>
-      <c r="H14" s="39"/>
+        <f>G13*H13</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B14" s="39" t="s">
+        <v>96</v>
+      </c>
+      <c r="C14" s="51"/>
+      <c r="D14" s="55" t="s">
+        <v>77</v>
+      </c>
+      <c r="E14" s="51" t="s">
+        <v>84</v>
+      </c>
+      <c r="F14" s="39" t="s">
+        <v>130</v>
+      </c>
+      <c r="G14" s="39">
+        <v>15000</v>
+      </c>
+      <c r="H14" s="39">
+        <v>1</v>
+      </c>
       <c r="I14" s="39">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>G14*H14</f>
+        <v>15000</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
@@ -4301,7 +4802,7 @@
       <c r="G15" s="39"/>
       <c r="H15" s="39"/>
       <c r="I15" s="39">
-        <f t="shared" si="0"/>
+        <f>G16*H16</f>
         <v>0</v>
       </c>
     </row>
@@ -4314,7 +4815,7 @@
       <c r="G16" s="39"/>
       <c r="H16" s="39"/>
       <c r="I16" s="39">
-        <f t="shared" si="0"/>
+        <f>G17*H17</f>
         <v>0</v>
       </c>
     </row>
@@ -4327,7 +4828,7 @@
       <c r="G17" s="39"/>
       <c r="H17" s="39"/>
       <c r="I17" s="39">
-        <f t="shared" si="0"/>
+        <f>G18*H18</f>
         <v>0</v>
       </c>
     </row>
@@ -4340,7 +4841,7 @@
       <c r="G18" s="39"/>
       <c r="H18" s="39"/>
       <c r="I18" s="39">
-        <f t="shared" si="0"/>
+        <f>G19*H19</f>
         <v>0</v>
       </c>
     </row>
@@ -4353,7 +4854,7 @@
       <c r="G19" s="39"/>
       <c r="H19" s="39"/>
       <c r="I19" s="39">
-        <f t="shared" si="0"/>
+        <f>G20*H20</f>
         <v>0</v>
       </c>
     </row>
@@ -4366,7 +4867,7 @@
       <c r="G20" s="39"/>
       <c r="H20" s="39"/>
       <c r="I20" s="39">
-        <f t="shared" si="0"/>
+        <f>G21*H21</f>
         <v>0</v>
       </c>
     </row>
@@ -4379,7 +4880,7 @@
       <c r="G21" s="39"/>
       <c r="H21" s="39"/>
       <c r="I21" s="39">
-        <f t="shared" si="0"/>
+        <f>G22*H22</f>
         <v>0</v>
       </c>
     </row>
@@ -4392,7 +4893,7 @@
       <c r="G22" s="39"/>
       <c r="H22" s="39"/>
       <c r="I22" s="39">
-        <f t="shared" si="0"/>
+        <f>G23*H23</f>
         <v>0</v>
       </c>
     </row>
@@ -4405,7 +4906,7 @@
       <c r="G23" s="39"/>
       <c r="H23" s="39"/>
       <c r="I23" s="39">
-        <f t="shared" si="0"/>
+        <f>G24*H24</f>
         <v>0</v>
       </c>
     </row>
@@ -4418,7 +4919,7 @@
       <c r="G24" s="39"/>
       <c r="H24" s="39"/>
       <c r="I24" s="39">
-        <f t="shared" si="0"/>
+        <f>G25*H25</f>
         <v>0</v>
       </c>
     </row>
@@ -4431,7 +4932,7 @@
       <c r="G25" s="39"/>
       <c r="H25" s="39"/>
       <c r="I25" s="39">
-        <f t="shared" si="0"/>
+        <f>G26*H26</f>
         <v>0</v>
       </c>
     </row>
@@ -4444,7 +4945,7 @@
       <c r="G26" s="39"/>
       <c r="H26" s="39"/>
       <c r="I26" s="39">
-        <f t="shared" si="0"/>
+        <f>G27*H27</f>
         <v>0</v>
       </c>
     </row>
@@ -4457,7 +4958,7 @@
       <c r="G27" s="39"/>
       <c r="H27" s="39"/>
       <c r="I27" s="39">
-        <f t="shared" si="0"/>
+        <f>G28*H28</f>
         <v>0</v>
       </c>
     </row>
@@ -4470,7 +4971,7 @@
       <c r="G28" s="39"/>
       <c r="H28" s="39"/>
       <c r="I28" s="39">
-        <f t="shared" si="0"/>
+        <f>G29*H29</f>
         <v>0</v>
       </c>
     </row>
@@ -4483,7 +4984,7 @@
       <c r="G29" s="39"/>
       <c r="H29" s="39"/>
       <c r="I29" s="39">
-        <f t="shared" si="0"/>
+        <f>G30*H30</f>
         <v>0</v>
       </c>
     </row>
@@ -4496,7 +4997,7 @@
       <c r="G30" s="39"/>
       <c r="H30" s="39"/>
       <c r="I30" s="39">
-        <f t="shared" si="0"/>
+        <f>G31*H31</f>
         <v>0</v>
       </c>
     </row>
@@ -4509,7 +5010,7 @@
       <c r="G31" s="39"/>
       <c r="H31" s="39"/>
       <c r="I31" s="39">
-        <f t="shared" si="0"/>
+        <f>G32*H32</f>
         <v>0</v>
       </c>
     </row>
@@ -4522,7 +5023,7 @@
       <c r="G32" s="39"/>
       <c r="H32" s="39"/>
       <c r="I32" s="39">
-        <f t="shared" si="0"/>
+        <f>G33*H33</f>
         <v>0</v>
       </c>
     </row>
@@ -4535,7 +5036,7 @@
       <c r="G33" s="39"/>
       <c r="H33" s="39"/>
       <c r="I33" s="39">
-        <f t="shared" si="0"/>
+        <f>G34*H34</f>
         <v>0</v>
       </c>
     </row>
@@ -4548,7 +5049,7 @@
       <c r="G34" s="39"/>
       <c r="H34" s="39"/>
       <c r="I34" s="39">
-        <f t="shared" si="0"/>
+        <f>G35*H35</f>
         <v>0</v>
       </c>
     </row>
@@ -4561,9 +5062,18 @@
       <c r="G35" s="39"/>
       <c r="H35" s="39"/>
       <c r="I35" s="39">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+        <f>G36*H36</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B36" s="39"/>
+      <c r="C36" s="39"/>
+      <c r="D36" s="39"/>
+      <c r="E36" s="39"/>
+      <c r="F36" s="39"/>
+      <c r="G36" s="39"/>
+      <c r="H36" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Dodat goods and services i serveri
</commit_message>
<xml_diff>
--- a/2b Format partner budget - Horizon2020.xlsx
+++ b/2b Format partner budget - Horizon2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ZORAN\Desktop\USP_projekat\CardioGuardian\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85368270-9341-49A4-812A-F0AEE366F4CB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{777409D9-2E42-4446-AB45-E2DD7C6A2C8B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Detaljno budzet" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,9 @@
     <sheet name="Equipment - budzet" sheetId="3" r:id="rId3"/>
     <sheet name="Subcontracting - budzet" sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Travel - budzet'!$B$4:$P$34</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -68,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="134">
   <si>
     <t>Partner budget Horizon 2020</t>
   </si>
@@ -406,9 +409,6 @@
     <t>рачунар- 500GB SSD, 16GB RAM, CPU 7 или новија генерација</t>
   </si>
   <si>
-    <t>Потрошни материјал, канцеларијски прибор</t>
-  </si>
-  <si>
     <t>WP2</t>
   </si>
   <si>
@@ -461,6 +461,18 @@
   </si>
   <si>
     <t>Услуге фирме за маркетинг</t>
+  </si>
+  <si>
+    <t>Сервер - минимум: 256GB REG ECC DDR4 RAM, CPU: 22 језгра, 2.20GHz, 55MB Cache</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Сервер - минимум: 4 CPU: 22 jezgra, 2.10GHz, 55MB Cache; 1024GB REG DDR4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Windows Server Standard 2019 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Windows Server Datacenter 2019 </t>
   </si>
 </sst>
 </file>
@@ -828,7 +840,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -939,51 +951,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1003,6 +971,51 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1467,65 +1480,65 @@
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="E3" s="72"/>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="72"/>
-      <c r="I3" s="72"/>
+      <c r="E3" s="58"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="58"/>
+      <c r="H3" s="58"/>
+      <c r="I3" s="58"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D4" s="2"/>
-      <c r="E4" s="73" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" s="74"/>
-      <c r="G4" s="74"/>
-      <c r="H4" s="74"/>
-      <c r="I4" s="74"/>
+      <c r="E4" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="60"/>
+      <c r="I4" s="60"/>
       <c r="J4" s="3"/>
-      <c r="L4" s="74" t="s">
+      <c r="L4" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="M4" s="74"/>
-      <c r="N4" s="74"/>
+      <c r="M4" s="60"/>
+      <c r="N4" s="60"/>
       <c r="O4" s="4">
         <v>0.25</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D5" s="2"/>
-      <c r="E5" s="73" t="s">
+      <c r="E5" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="74"/>
-      <c r="G5" s="74"/>
-      <c r="H5" s="74"/>
-      <c r="I5" s="74"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="60"/>
+      <c r="H5" s="60"/>
+      <c r="I5" s="60"/>
       <c r="J5" s="3"/>
-      <c r="L5" s="74" t="s">
+      <c r="L5" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="M5" s="74"/>
-      <c r="N5" s="74"/>
+      <c r="M5" s="60"/>
+      <c r="N5" s="60"/>
       <c r="O5" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D6" s="2"/>
-      <c r="E6" s="73" t="s">
+      <c r="E6" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="74"/>
-      <c r="G6" s="74"/>
-      <c r="H6" s="74"/>
-      <c r="I6" s="74"/>
+      <c r="F6" s="60"/>
+      <c r="G6" s="60"/>
+      <c r="H6" s="60"/>
+      <c r="I6" s="60"/>
       <c r="J6" s="3"/>
-      <c r="L6" s="74" t="s">
+      <c r="L6" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="M6" s="74"/>
-      <c r="N6" s="74"/>
+      <c r="M6" s="60"/>
+      <c r="N6" s="60"/>
       <c r="O6" s="5">
         <v>0.7</v>
       </c>
@@ -1535,19 +1548,19 @@
       <c r="Q6" s="6"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="E7" s="74" t="s">
+      <c r="E7" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="74"/>
-      <c r="G7" s="74"/>
-      <c r="H7" s="74"/>
-      <c r="I7" s="74"/>
+      <c r="F7" s="60"/>
+      <c r="G7" s="60"/>
+      <c r="H7" s="60"/>
+      <c r="I7" s="60"/>
       <c r="J7" s="3"/>
-      <c r="L7" s="74" t="s">
+      <c r="L7" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="M7" s="74"/>
-      <c r="N7" s="74"/>
+      <c r="M7" s="60"/>
+      <c r="N7" s="60"/>
       <c r="O7" s="4">
         <v>1</v>
       </c>
@@ -1558,56 +1571,56 @@
     </row>
     <row r="9" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="75" t="s">
+      <c r="A10" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="76"/>
-      <c r="C10" s="76"/>
-      <c r="D10" s="76"/>
-      <c r="E10" s="76"/>
-      <c r="F10" s="76"/>
-      <c r="G10" s="76"/>
-      <c r="H10" s="76"/>
-      <c r="I10" s="76"/>
-      <c r="J10" s="76"/>
-      <c r="K10" s="76"/>
-      <c r="L10" s="76"/>
-      <c r="M10" s="76"/>
-      <c r="N10" s="76"/>
-      <c r="O10" s="76"/>
-      <c r="P10" s="76"/>
-      <c r="Q10" s="76"/>
-      <c r="R10" s="76"/>
+      <c r="B10" s="62"/>
+      <c r="C10" s="62"/>
+      <c r="D10" s="62"/>
+      <c r="E10" s="62"/>
+      <c r="F10" s="62"/>
+      <c r="G10" s="62"/>
+      <c r="H10" s="62"/>
+      <c r="I10" s="62"/>
+      <c r="J10" s="62"/>
+      <c r="K10" s="62"/>
+      <c r="L10" s="62"/>
+      <c r="M10" s="62"/>
+      <c r="N10" s="62"/>
+      <c r="O10" s="62"/>
+      <c r="P10" s="62"/>
+      <c r="Q10" s="62"/>
+      <c r="R10" s="62"/>
       <c r="S10" s="8"/>
     </row>
     <row r="12" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D12" s="77" t="s">
+      <c r="D12" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="77"/>
-      <c r="F12" s="77"/>
-      <c r="G12" s="77"/>
-      <c r="H12" s="77"/>
-      <c r="I12" s="77"/>
-      <c r="J12" s="78" t="s">
+      <c r="E12" s="63"/>
+      <c r="F12" s="63"/>
+      <c r="G12" s="63"/>
+      <c r="H12" s="63"/>
+      <c r="I12" s="63"/>
+      <c r="J12" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="K12" s="78"/>
-      <c r="L12" s="78"/>
-      <c r="M12" s="78"/>
-      <c r="N12" s="78"/>
-      <c r="O12" s="78"/>
-      <c r="P12" s="78"/>
-      <c r="Q12" s="78"/>
-      <c r="R12" s="78"/>
+      <c r="K12" s="64"/>
+      <c r="L12" s="64"/>
+      <c r="M12" s="64"/>
+      <c r="N12" s="64"/>
+      <c r="O12" s="64"/>
+      <c r="P12" s="64"/>
+      <c r="Q12" s="64"/>
+      <c r="R12" s="64"/>
       <c r="S12" s="9"/>
     </row>
     <row r="13" spans="1:19" s="14" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="71" t="s">
+      <c r="A13" s="57" t="s">
         <v>61</v>
       </c>
-      <c r="B13" s="71"/>
-      <c r="C13" s="71"/>
+      <c r="B13" s="57"/>
+      <c r="C13" s="57"/>
       <c r="D13" s="48" t="s">
         <v>70</v>
       </c>
@@ -2008,11 +2021,11 @@
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A24" s="70" t="s">
+      <c r="A24" s="67" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="70"/>
-      <c r="C24" s="70"/>
+      <c r="B24" s="67"/>
+      <c r="C24" s="67"/>
       <c r="D24" s="15">
         <f>SUM(D14:D23)</f>
         <v>0</v>
@@ -2133,24 +2146,24 @@
       <c r="S27" s="31"/>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A28" s="69" t="s">
+      <c r="A28" s="65" t="s">
         <v>30</v>
       </c>
-      <c r="B28" s="69"/>
-      <c r="C28" s="69"/>
-      <c r="D28" s="69"/>
-      <c r="E28" s="69"/>
-      <c r="F28" s="69"/>
-      <c r="G28" s="69"/>
-      <c r="H28" s="69"/>
-      <c r="I28" s="69"/>
-      <c r="J28" s="69"/>
-      <c r="K28" s="69"/>
-      <c r="L28" s="69"/>
-      <c r="M28" s="69"/>
-      <c r="N28" s="69"/>
-      <c r="O28" s="69"/>
-      <c r="P28" s="69"/>
+      <c r="B28" s="65"/>
+      <c r="C28" s="65"/>
+      <c r="D28" s="65"/>
+      <c r="E28" s="65"/>
+      <c r="F28" s="65"/>
+      <c r="G28" s="65"/>
+      <c r="H28" s="65"/>
+      <c r="I28" s="65"/>
+      <c r="J28" s="65"/>
+      <c r="K28" s="65"/>
+      <c r="L28" s="65"/>
+      <c r="M28" s="65"/>
+      <c r="N28" s="65"/>
+      <c r="O28" s="65"/>
+      <c r="P28" s="65"/>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="32"/>
@@ -2191,95 +2204,95 @@
       <c r="P30" s="32"/>
     </row>
     <row r="31" spans="1:20" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="62" t="str">
+      <c r="A31" s="68" t="str">
         <f>CONCATENATE("participant"," ",J6)</f>
         <v xml:space="preserve">participant </v>
       </c>
-      <c r="B31" s="63"/>
+      <c r="B31" s="69"/>
       <c r="C31" s="33" t="s">
         <v>32</v>
       </c>
       <c r="D31" s="66" t="s">
         <v>33</v>
       </c>
-      <c r="E31" s="67"/>
-      <c r="F31" s="67"/>
-      <c r="G31" s="67"/>
-      <c r="H31" s="67"/>
-      <c r="I31" s="67"/>
-      <c r="J31" s="67"/>
-      <c r="K31" s="67"/>
-      <c r="L31" s="67"/>
-      <c r="M31" s="67"/>
-      <c r="N31" s="67"/>
-      <c r="O31" s="67"/>
-      <c r="P31" s="67"/>
+      <c r="E31" s="70"/>
+      <c r="F31" s="70"/>
+      <c r="G31" s="70"/>
+      <c r="H31" s="70"/>
+      <c r="I31" s="70"/>
+      <c r="J31" s="70"/>
+      <c r="K31" s="70"/>
+      <c r="L31" s="70"/>
+      <c r="M31" s="70"/>
+      <c r="N31" s="70"/>
+      <c r="O31" s="70"/>
+      <c r="P31" s="70"/>
     </row>
     <row r="32" spans="1:20" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="56" t="s">
+      <c r="A32" s="71" t="s">
         <v>34</v>
       </c>
-      <c r="B32" s="56"/>
+      <c r="B32" s="71"/>
       <c r="C32" s="34"/>
-      <c r="D32" s="68" t="s">
+      <c r="D32" s="72" t="s">
         <v>67</v>
       </c>
-      <c r="E32" s="61"/>
-      <c r="F32" s="61"/>
-      <c r="G32" s="61"/>
-      <c r="H32" s="61"/>
-      <c r="I32" s="61"/>
-      <c r="J32" s="61"/>
-      <c r="K32" s="61"/>
-      <c r="L32" s="61"/>
-      <c r="M32" s="61"/>
-      <c r="N32" s="61"/>
-      <c r="O32" s="61"/>
-      <c r="P32" s="61"/>
+      <c r="E32" s="73"/>
+      <c r="F32" s="73"/>
+      <c r="G32" s="73"/>
+      <c r="H32" s="73"/>
+      <c r="I32" s="73"/>
+      <c r="J32" s="73"/>
+      <c r="K32" s="73"/>
+      <c r="L32" s="73"/>
+      <c r="M32" s="73"/>
+      <c r="N32" s="73"/>
+      <c r="O32" s="73"/>
+      <c r="P32" s="73"/>
       <c r="S32" s="31"/>
     </row>
     <row r="33" spans="1:19" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="56" t="s">
+      <c r="A33" s="71" t="s">
         <v>35</v>
       </c>
-      <c r="B33" s="56"/>
+      <c r="B33" s="71"/>
       <c r="C33" s="35"/>
-      <c r="D33" s="61" t="s">
+      <c r="D33" s="73" t="s">
         <v>68</v>
       </c>
-      <c r="E33" s="61"/>
-      <c r="F33" s="61"/>
-      <c r="G33" s="61"/>
-      <c r="H33" s="61"/>
-      <c r="I33" s="61"/>
-      <c r="J33" s="61"/>
-      <c r="K33" s="61"/>
-      <c r="L33" s="61"/>
-      <c r="M33" s="61"/>
-      <c r="N33" s="61"/>
-      <c r="O33" s="61"/>
-      <c r="P33" s="61"/>
+      <c r="E33" s="73"/>
+      <c r="F33" s="73"/>
+      <c r="G33" s="73"/>
+      <c r="H33" s="73"/>
+      <c r="I33" s="73"/>
+      <c r="J33" s="73"/>
+      <c r="K33" s="73"/>
+      <c r="L33" s="73"/>
+      <c r="M33" s="73"/>
+      <c r="N33" s="73"/>
+      <c r="O33" s="73"/>
+      <c r="P33" s="73"/>
       <c r="S33" s="31"/>
     </row>
     <row r="34" spans="1:19" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="56" t="s">
+      <c r="A34" s="71" t="s">
         <v>36</v>
       </c>
-      <c r="B34" s="56"/>
+      <c r="B34" s="71"/>
       <c r="C34" s="35"/>
-      <c r="D34" s="61"/>
-      <c r="E34" s="61"/>
-      <c r="F34" s="61"/>
-      <c r="G34" s="61"/>
-      <c r="H34" s="61"/>
-      <c r="I34" s="61"/>
-      <c r="J34" s="61"/>
-      <c r="K34" s="61"/>
-      <c r="L34" s="61"/>
-      <c r="M34" s="61"/>
-      <c r="N34" s="61"/>
-      <c r="O34" s="61"/>
-      <c r="P34" s="61"/>
+      <c r="D34" s="73"/>
+      <c r="E34" s="73"/>
+      <c r="F34" s="73"/>
+      <c r="G34" s="73"/>
+      <c r="H34" s="73"/>
+      <c r="I34" s="73"/>
+      <c r="J34" s="73"/>
+      <c r="K34" s="73"/>
+      <c r="L34" s="73"/>
+      <c r="M34" s="73"/>
+      <c r="N34" s="73"/>
+      <c r="O34" s="73"/>
+      <c r="P34" s="73"/>
       <c r="S34" s="31"/>
     </row>
     <row r="35" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.25">
@@ -2313,97 +2326,97 @@
       <c r="P36" s="38"/>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A37" s="62" t="str">
+      <c r="A37" s="68" t="str">
         <f>CONCATENATE("participant"," ",C9)</f>
         <v xml:space="preserve">participant </v>
       </c>
-      <c r="B37" s="63"/>
+      <c r="B37" s="69"/>
       <c r="C37" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="D37" s="64" t="s">
+      <c r="D37" s="78" t="s">
         <v>33</v>
       </c>
-      <c r="E37" s="65"/>
-      <c r="F37" s="65"/>
-      <c r="G37" s="65"/>
-      <c r="H37" s="65"/>
-      <c r="I37" s="65"/>
-      <c r="J37" s="65"/>
-      <c r="K37" s="65"/>
-      <c r="L37" s="65"/>
-      <c r="M37" s="65"/>
-      <c r="N37" s="65"/>
-      <c r="O37" s="65"/>
-      <c r="P37" s="65"/>
+      <c r="E37" s="79"/>
+      <c r="F37" s="79"/>
+      <c r="G37" s="79"/>
+      <c r="H37" s="79"/>
+      <c r="I37" s="79"/>
+      <c r="J37" s="79"/>
+      <c r="K37" s="79"/>
+      <c r="L37" s="79"/>
+      <c r="M37" s="79"/>
+      <c r="N37" s="79"/>
+      <c r="O37" s="79"/>
+      <c r="P37" s="79"/>
     </row>
     <row r="38" spans="1:19" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="56" t="s">
+      <c r="A38" s="71" t="s">
         <v>37</v>
       </c>
-      <c r="B38" s="56"/>
+      <c r="B38" s="71"/>
       <c r="C38" s="35"/>
-      <c r="D38" s="60" t="s">
+      <c r="D38" s="77" t="s">
         <v>69</v>
       </c>
-      <c r="E38" s="61"/>
-      <c r="F38" s="61"/>
-      <c r="G38" s="61"/>
-      <c r="H38" s="61"/>
-      <c r="I38" s="61"/>
-      <c r="J38" s="61"/>
-      <c r="K38" s="61"/>
-      <c r="L38" s="61"/>
-      <c r="M38" s="61"/>
-      <c r="N38" s="61"/>
-      <c r="O38" s="61"/>
-      <c r="P38" s="61"/>
+      <c r="E38" s="73"/>
+      <c r="F38" s="73"/>
+      <c r="G38" s="73"/>
+      <c r="H38" s="73"/>
+      <c r="I38" s="73"/>
+      <c r="J38" s="73"/>
+      <c r="K38" s="73"/>
+      <c r="L38" s="73"/>
+      <c r="M38" s="73"/>
+      <c r="N38" s="73"/>
+      <c r="O38" s="73"/>
+      <c r="P38" s="73"/>
       <c r="S38" s="31"/>
     </row>
     <row r="39" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="56" t="s">
+      <c r="A39" s="71" t="s">
         <v>38</v>
       </c>
-      <c r="B39" s="56"/>
+      <c r="B39" s="71"/>
       <c r="C39" s="35"/>
-      <c r="D39" s="57" t="s">
+      <c r="D39" s="74" t="s">
         <v>39</v>
       </c>
-      <c r="E39" s="58"/>
-      <c r="F39" s="58"/>
-      <c r="G39" s="58"/>
-      <c r="H39" s="58"/>
-      <c r="I39" s="58"/>
-      <c r="J39" s="58"/>
-      <c r="K39" s="58"/>
-      <c r="L39" s="58"/>
-      <c r="M39" s="58"/>
-      <c r="N39" s="58"/>
-      <c r="O39" s="58"/>
-      <c r="P39" s="59"/>
+      <c r="E39" s="75"/>
+      <c r="F39" s="75"/>
+      <c r="G39" s="75"/>
+      <c r="H39" s="75"/>
+      <c r="I39" s="75"/>
+      <c r="J39" s="75"/>
+      <c r="K39" s="75"/>
+      <c r="L39" s="75"/>
+      <c r="M39" s="75"/>
+      <c r="N39" s="75"/>
+      <c r="O39" s="75"/>
+      <c r="P39" s="76"/>
       <c r="S39" s="31"/>
     </row>
     <row r="40" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="56" t="s">
+      <c r="A40" s="71" t="s">
         <v>40</v>
       </c>
-      <c r="B40" s="56"/>
+      <c r="B40" s="71"/>
       <c r="C40" s="35"/>
-      <c r="D40" s="60" t="s">
+      <c r="D40" s="77" t="s">
         <v>41</v>
       </c>
-      <c r="E40" s="61"/>
-      <c r="F40" s="61"/>
-      <c r="G40" s="61"/>
-      <c r="H40" s="61"/>
-      <c r="I40" s="61"/>
-      <c r="J40" s="61"/>
-      <c r="K40" s="61"/>
-      <c r="L40" s="61"/>
-      <c r="M40" s="61"/>
-      <c r="N40" s="61"/>
-      <c r="O40" s="61"/>
-      <c r="P40" s="61"/>
+      <c r="E40" s="73"/>
+      <c r="F40" s="73"/>
+      <c r="G40" s="73"/>
+      <c r="H40" s="73"/>
+      <c r="I40" s="73"/>
+      <c r="J40" s="73"/>
+      <c r="K40" s="73"/>
+      <c r="L40" s="73"/>
+      <c r="M40" s="73"/>
+      <c r="N40" s="73"/>
+      <c r="O40" s="73"/>
+      <c r="P40" s="73"/>
       <c r="S40" s="31"/>
     </row>
   </sheetData>
@@ -2411,6 +2424,34 @@
     <protectedRange sqref="J14:N23 C32:P40 D14:H23 P14:P23 R14:S23 O6" name="Range1"/>
   </protectedRanges>
   <mergeCells count="41">
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="D39:P39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="D40:P40"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="D34:P34"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="D37:P37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="D38:P38"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="D31:P31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="D32:P32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="D33:P33"/>
+    <mergeCell ref="A28:P28"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A24:C24"/>
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="E3:I3"/>
     <mergeCell ref="E4:I4"/>
@@ -2424,34 +2465,6 @@
     <mergeCell ref="A10:R10"/>
     <mergeCell ref="D12:I12"/>
     <mergeCell ref="J12:R12"/>
-    <mergeCell ref="A28:P28"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="D31:P31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="D32:P32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="D33:P33"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="D39:P39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="D40:P40"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="D34:P34"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="D37:P37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="D38:P38"/>
   </mergeCells>
   <conditionalFormatting sqref="O4">
     <cfRule type="expression" dxfId="0" priority="1">
@@ -2472,10 +2485,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B1:P44"/>
+  <dimension ref="B1:P59"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28:E28"/>
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2488,13 +2501,13 @@
   <sheetData>
     <row r="1" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="79" t="s">
+      <c r="B2" s="80" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="80"/>
+      <c r="C2" s="81"/>
       <c r="D2" s="43">
-        <f>SUM(P5:P44)</f>
-        <v>108760</v>
+        <f>SUM(P5:P60)</f>
+        <v>129580</v>
       </c>
     </row>
     <row r="4" spans="2:16" ht="162" x14ac:dyDescent="0.25">
@@ -2549,7 +2562,7 @@
         <v>72</v>
       </c>
       <c r="C5" s="52"/>
-      <c r="D5" s="53" t="s">
+      <c r="D5" s="54" t="s">
         <v>73</v>
       </c>
       <c r="E5" s="52" t="s">
@@ -2782,7 +2795,7 @@
     </row>
     <row r="11" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="52" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C11" s="52"/>
       <c r="D11" s="54" t="s">
@@ -2795,34 +2808,36 @@
         <v>74</v>
       </c>
       <c r="G11" s="52" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H11" s="52">
         <v>1</v>
       </c>
       <c r="I11" s="52">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J11" s="52"/>
-      <c r="K11" s="52"/>
+      <c r="K11" s="52">
+        <v>1</v>
+      </c>
       <c r="L11" s="52"/>
       <c r="M11" s="52">
         <v>7</v>
       </c>
       <c r="N11" s="52">
-        <v>1600</v>
+        <v>3200</v>
       </c>
       <c r="O11" s="52">
-        <v>1020</v>
+        <v>2040</v>
       </c>
       <c r="P11" s="52">
         <f t="shared" si="0"/>
-        <v>2620</v>
+        <v>5240</v>
       </c>
     </row>
     <row r="12" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="52" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C12" s="52"/>
       <c r="D12" s="54" t="s">
@@ -2835,7 +2850,7 @@
         <v>81</v>
       </c>
       <c r="G12" s="52" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H12" s="52"/>
       <c r="I12" s="52"/>
@@ -2862,7 +2877,7 @@
     </row>
     <row r="13" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="52" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C13" s="52"/>
       <c r="D13" s="54" t="s">
@@ -2875,34 +2890,36 @@
         <v>74</v>
       </c>
       <c r="G13" s="52" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H13" s="52">
         <v>1</v>
       </c>
       <c r="I13" s="52">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J13" s="52"/>
-      <c r="K13" s="52"/>
+      <c r="K13" s="52">
+        <v>1</v>
+      </c>
       <c r="L13" s="52"/>
       <c r="M13" s="52">
         <v>7</v>
       </c>
       <c r="N13" s="52">
-        <v>1600</v>
+        <v>3200</v>
       </c>
       <c r="O13" s="52">
-        <v>1620</v>
+        <v>3240</v>
       </c>
       <c r="P13" s="52">
         <f t="shared" si="0"/>
-        <v>3220</v>
+        <v>6440</v>
       </c>
     </row>
     <row r="14" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="52" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C14" s="52"/>
       <c r="D14" s="54" t="s">
@@ -2915,16 +2932,16 @@
         <v>81</v>
       </c>
       <c r="G14" s="52" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H14" s="52"/>
       <c r="I14" s="52"/>
       <c r="J14" s="52">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K14" s="52"/>
       <c r="L14" s="52">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M14" s="52">
         <v>7</v>
@@ -2942,7 +2959,7 @@
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B15" s="52" t="s">
-        <v>91</v>
+        <v>112</v>
       </c>
       <c r="C15" s="52" t="s">
         <v>92</v>
@@ -2957,124 +2974,120 @@
         <v>85</v>
       </c>
       <c r="G15" s="52" t="s">
-        <v>83</v>
+        <v>114</v>
       </c>
       <c r="H15" s="52">
-        <v>2</v>
-      </c>
-      <c r="I15" s="52">
-        <v>1</v>
-      </c>
-      <c r="J15" s="52">
-        <v>2</v>
-      </c>
-      <c r="K15" s="52">
-        <v>1</v>
-      </c>
-      <c r="L15" s="52"/>
+        <v>1</v>
+      </c>
+      <c r="I15" s="52"/>
+      <c r="J15" s="52"/>
+      <c r="K15" s="52"/>
+      <c r="L15" s="52">
+        <v>1</v>
+      </c>
       <c r="M15" s="52">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="N15" s="52">
-        <v>6000</v>
+        <v>1600</v>
       </c>
       <c r="O15" s="52">
-        <v>6660</v>
+        <v>1620</v>
       </c>
       <c r="P15" s="52">
-        <f t="shared" si="0"/>
-        <v>12660</v>
+        <f>SUM(N15:O15)</f>
+        <v>3220</v>
       </c>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B16" s="52" t="s">
         <v>91</v>
       </c>
-      <c r="C16" s="52"/>
+      <c r="C16" s="52" t="s">
+        <v>92</v>
+      </c>
       <c r="D16" s="52" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="E16" s="52" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="F16" s="52" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="G16" s="52" t="s">
         <v>83</v>
       </c>
       <c r="H16" s="52">
-        <v>1</v>
-      </c>
-      <c r="I16" s="52"/>
+        <v>2</v>
+      </c>
+      <c r="I16" s="52">
+        <v>1</v>
+      </c>
       <c r="J16" s="52">
-        <v>1</v>
-      </c>
-      <c r="K16" s="52"/>
+        <v>2</v>
+      </c>
+      <c r="K16" s="52">
+        <v>1</v>
+      </c>
       <c r="L16" s="52"/>
       <c r="M16" s="52">
         <v>10</v>
       </c>
       <c r="N16" s="52">
-        <v>1600</v>
+        <v>6000</v>
       </c>
       <c r="O16" s="52">
-        <v>2220</v>
+        <v>6660</v>
       </c>
       <c r="P16" s="52">
-        <f t="shared" si="0"/>
-        <v>3820</v>
+        <f t="shared" ref="P16:P32" si="1">N16+O16</f>
+        <v>12660</v>
       </c>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B17" s="52" t="s">
-        <v>95</v>
-      </c>
-      <c r="C17" s="52" t="s">
-        <v>92</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="C17" s="52"/>
       <c r="D17" s="52" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="E17" s="52" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F17" s="52" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="G17" s="52" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="H17" s="52">
-        <v>2</v>
-      </c>
-      <c r="I17" s="52">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="I17" s="52"/>
       <c r="J17" s="52">
-        <v>2</v>
-      </c>
-      <c r="K17" s="52">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="K17" s="52"/>
       <c r="L17" s="52"/>
       <c r="M17" s="52">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="N17" s="52">
-        <v>4200</v>
+        <v>1600</v>
       </c>
       <c r="O17" s="52">
-        <v>5460</v>
+        <v>2220</v>
       </c>
       <c r="P17" s="52">
-        <f t="shared" si="0"/>
-        <v>9660</v>
+        <f t="shared" si="1"/>
+        <v>3820</v>
       </c>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B18" s="52" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C18" s="52" t="s">
         <v>92</v>
@@ -3089,31 +3102,33 @@
         <v>85</v>
       </c>
       <c r="G18" s="52" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="H18" s="52">
-        <v>1</v>
-      </c>
-      <c r="I18" s="52"/>
+        <v>2</v>
+      </c>
+      <c r="I18" s="52">
+        <v>1</v>
+      </c>
       <c r="J18" s="52">
-        <v>1</v>
-      </c>
-      <c r="K18" s="52"/>
-      <c r="L18" s="52">
         <v>2</v>
       </c>
+      <c r="K18" s="52">
+        <v>1</v>
+      </c>
+      <c r="L18" s="52"/>
       <c r="M18" s="52">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="N18" s="52">
-        <v>4000</v>
+        <v>4200</v>
       </c>
       <c r="O18" s="52">
-        <v>4080</v>
+        <v>5460</v>
       </c>
       <c r="P18" s="52">
-        <f t="shared" si="0"/>
-        <v>8080</v>
+        <f t="shared" si="1"/>
+        <v>9660</v>
       </c>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.25">
@@ -3133,12 +3148,20 @@
         <v>85</v>
       </c>
       <c r="G19" s="52" t="s">
-        <v>98</v>
-      </c>
-      <c r="H19" s="52"/>
-      <c r="I19" s="52"/>
-      <c r="J19" s="52"/>
-      <c r="K19" s="52"/>
+        <v>97</v>
+      </c>
+      <c r="H19" s="52">
+        <v>1</v>
+      </c>
+      <c r="I19" s="52">
+        <v>1</v>
+      </c>
+      <c r="J19" s="52">
+        <v>1</v>
+      </c>
+      <c r="K19" s="52">
+        <v>1</v>
+      </c>
       <c r="L19" s="52">
         <v>2</v>
       </c>
@@ -3146,196 +3169,194 @@
         <v>10</v>
       </c>
       <c r="N19" s="52">
-        <v>1600</v>
+        <v>6000</v>
       </c>
       <c r="O19" s="52">
-        <v>1680</v>
+        <v>6120</v>
       </c>
       <c r="P19" s="52">
-        <f t="shared" si="0"/>
-        <v>3280</v>
+        <f t="shared" si="1"/>
+        <v>12120</v>
       </c>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B20" s="52" t="s">
         <v>96</v>
       </c>
-      <c r="C20" s="52"/>
+      <c r="C20" s="52" t="s">
+        <v>92</v>
+      </c>
       <c r="D20" s="52" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="E20" s="52" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="F20" s="52" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="G20" s="52" t="s">
         <v>98</v>
       </c>
-      <c r="H20" s="52">
-        <v>1</v>
-      </c>
+      <c r="H20" s="52"/>
       <c r="I20" s="52"/>
-      <c r="J20" s="52">
-        <v>1</v>
-      </c>
+      <c r="J20" s="52"/>
       <c r="K20" s="52"/>
-      <c r="L20" s="52"/>
+      <c r="L20" s="52">
+        <v>2</v>
+      </c>
       <c r="M20" s="52">
         <v>10</v>
       </c>
       <c r="N20" s="52">
-        <v>1200</v>
+        <v>1600</v>
       </c>
       <c r="O20" s="52">
         <v>1680</v>
       </c>
       <c r="P20" s="52">
-        <f t="shared" si="0"/>
-        <v>2880</v>
+        <f t="shared" si="1"/>
+        <v>3280</v>
       </c>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B21" s="52" t="s">
         <v>96</v>
       </c>
-      <c r="C21" s="52" t="s">
-        <v>92</v>
-      </c>
+      <c r="C21" s="52"/>
       <c r="D21" s="52" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="E21" s="52" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F21" s="52" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="G21" s="52" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H21" s="52">
         <v>1</v>
       </c>
       <c r="I21" s="52"/>
-      <c r="J21" s="52"/>
+      <c r="J21" s="52">
+        <v>1</v>
+      </c>
       <c r="K21" s="52"/>
-      <c r="L21" s="52">
-        <v>1</v>
-      </c>
+      <c r="L21" s="52"/>
       <c r="M21" s="52">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="N21" s="52">
         <v>1200</v>
       </c>
       <c r="O21" s="52">
-        <v>900</v>
+        <v>1680</v>
       </c>
       <c r="P21" s="52">
-        <f t="shared" si="0"/>
-        <v>2100</v>
-      </c>
-    </row>
-    <row r="22" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B22" s="52" t="s">
         <v>96</v>
       </c>
-      <c r="C22" s="52"/>
-      <c r="D22" s="54" t="s">
-        <v>77</v>
+      <c r="C22" s="52" t="s">
+        <v>92</v>
+      </c>
+      <c r="D22" s="52" t="s">
+        <v>94</v>
       </c>
       <c r="E22" s="52" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="F22" s="52" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G22" s="52" t="s">
         <v>99</v>
       </c>
-      <c r="H22" s="52"/>
+      <c r="H22" s="52">
+        <v>1</v>
+      </c>
       <c r="I22" s="52"/>
-      <c r="J22" s="52">
-        <v>2</v>
-      </c>
+      <c r="J22" s="52"/>
       <c r="K22" s="52"/>
-      <c r="L22" s="52"/>
+      <c r="L22" s="52">
+        <v>1</v>
+      </c>
       <c r="M22" s="52">
         <v>7</v>
       </c>
       <c r="N22" s="52">
-        <v>2000</v>
+        <v>1200</v>
       </c>
       <c r="O22" s="52">
         <v>900</v>
       </c>
       <c r="P22" s="52">
-        <f t="shared" si="0"/>
-        <v>2900</v>
-      </c>
-    </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="23" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B23" s="52" t="s">
         <v>96</v>
       </c>
-      <c r="C23" s="52" t="s">
-        <v>92</v>
-      </c>
-      <c r="D23" s="52" t="s">
-        <v>94</v>
+      <c r="C23" s="52"/>
+      <c r="D23" s="54" t="s">
+        <v>77</v>
       </c>
       <c r="E23" s="52" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="F23" s="52" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G23" s="52" t="s">
-        <v>116</v>
-      </c>
-      <c r="H23" s="52">
-        <v>1</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="H23" s="52"/>
       <c r="I23" s="52"/>
       <c r="J23" s="52">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K23" s="52"/>
-      <c r="L23" s="52">
-        <v>2</v>
-      </c>
+      <c r="L23" s="52"/>
       <c r="M23" s="52">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="N23" s="52">
-        <v>4000</v>
+        <v>2000</v>
       </c>
       <c r="O23" s="52">
-        <v>5520</v>
+        <v>900</v>
       </c>
       <c r="P23" s="52">
-        <f t="shared" si="0"/>
-        <v>9520</v>
+        <f t="shared" si="1"/>
+        <v>2900</v>
       </c>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B24" s="52" t="s">
         <v>96</v>
       </c>
-      <c r="C24" s="52"/>
+      <c r="C24" s="52" t="s">
+        <v>92</v>
+      </c>
       <c r="D24" s="52" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="E24" s="52" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="F24" s="52" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="G24" s="52" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H24" s="52">
         <v>1</v>
@@ -3345,357 +3366,428 @@
         <v>1</v>
       </c>
       <c r="K24" s="52"/>
-      <c r="L24" s="52"/>
+      <c r="L24" s="52">
+        <v>2</v>
+      </c>
       <c r="M24" s="52">
         <v>10</v>
       </c>
       <c r="N24" s="52">
-        <v>1200</v>
+        <v>4000</v>
       </c>
       <c r="O24" s="52">
-        <v>2760</v>
+        <v>5520</v>
       </c>
       <c r="P24" s="52">
-        <f t="shared" si="0"/>
-        <v>3960</v>
+        <f t="shared" si="1"/>
+        <v>9520</v>
       </c>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B25" s="52" t="s">
         <v>96</v>
       </c>
-      <c r="C25" s="52" t="s">
-        <v>92</v>
-      </c>
+      <c r="C25" s="52"/>
       <c r="D25" s="52" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="E25" s="52" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F25" s="52" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="G25" s="52" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H25" s="52">
-        <v>2</v>
-      </c>
-      <c r="I25" s="52">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="I25" s="52"/>
       <c r="J25" s="52">
-        <v>2</v>
-      </c>
-      <c r="K25" s="52">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="K25" s="52"/>
       <c r="L25" s="52"/>
       <c r="M25" s="52">
         <v>10</v>
       </c>
       <c r="N25" s="52">
+        <v>1200</v>
+      </c>
+      <c r="O25" s="52">
+        <v>2760</v>
+      </c>
+      <c r="P25" s="52">
+        <f t="shared" si="1"/>
+        <v>3960</v>
+      </c>
+    </row>
+    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B26" s="52" t="s">
+        <v>96</v>
+      </c>
+      <c r="C26" s="52" t="s">
+        <v>92</v>
+      </c>
+      <c r="D26" s="52" t="s">
+        <v>94</v>
+      </c>
+      <c r="E26" s="52" t="s">
+        <v>93</v>
+      </c>
+      <c r="F26" s="52" t="s">
+        <v>85</v>
+      </c>
+      <c r="G26" s="52" t="s">
+        <v>116</v>
+      </c>
+      <c r="H26" s="52">
+        <v>2</v>
+      </c>
+      <c r="I26" s="52">
+        <v>1</v>
+      </c>
+      <c r="J26" s="52">
+        <v>1</v>
+      </c>
+      <c r="K26" s="52">
+        <v>1</v>
+      </c>
+      <c r="L26" s="52">
+        <v>1</v>
+      </c>
+      <c r="M26" s="52">
+        <v>10</v>
+      </c>
+      <c r="N26" s="52">
         <v>6000</v>
       </c>
-      <c r="O25" s="52">
+      <c r="O26" s="52">
         <v>5580</v>
       </c>
-      <c r="P25" s="52">
-        <f t="shared" si="0"/>
+      <c r="P26" s="52">
+        <f t="shared" si="1"/>
         <v>11580</v>
       </c>
     </row>
-    <row r="26" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B26" s="50" t="s">
+    <row r="27" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B27" s="52" t="s">
+        <v>96</v>
+      </c>
+      <c r="C27" s="56"/>
+      <c r="D27" s="54" t="s">
+        <v>77</v>
+      </c>
+      <c r="E27" s="52" t="s">
+        <v>84</v>
+      </c>
+      <c r="F27" s="52" t="s">
+        <v>83</v>
+      </c>
+      <c r="G27" s="52" t="s">
+        <v>116</v>
+      </c>
+      <c r="H27" s="56"/>
+      <c r="I27" s="56"/>
+      <c r="J27" s="56">
+        <v>2</v>
+      </c>
+      <c r="K27" s="56"/>
+      <c r="L27" s="56"/>
+      <c r="M27" s="56">
+        <v>10</v>
+      </c>
+      <c r="N27" s="56">
+        <v>2000</v>
+      </c>
+      <c r="O27" s="56">
+        <v>1860</v>
+      </c>
+      <c r="P27" s="56">
+        <f t="shared" si="1"/>
+        <v>3860</v>
+      </c>
+    </row>
+    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B28" s="52" t="s">
+        <v>96</v>
+      </c>
+      <c r="C28" s="56"/>
+      <c r="D28" s="52" t="s">
+        <v>80</v>
+      </c>
+      <c r="E28" s="52" t="s">
+        <v>89</v>
+      </c>
+      <c r="F28" s="52" t="s">
+        <v>90</v>
+      </c>
+      <c r="G28" s="52" t="s">
+        <v>116</v>
+      </c>
+      <c r="H28" s="52">
+        <v>1</v>
+      </c>
+      <c r="I28" s="52">
+        <v>1</v>
+      </c>
+      <c r="J28" s="52"/>
+      <c r="K28" s="56"/>
+      <c r="L28" s="56"/>
+      <c r="M28" s="56">
+        <v>10</v>
+      </c>
+      <c r="N28" s="56">
+        <v>2000</v>
+      </c>
+      <c r="O28" s="56">
+        <v>1860</v>
+      </c>
+      <c r="P28" s="56">
+        <f t="shared" si="1"/>
+        <v>3860</v>
+      </c>
+    </row>
+    <row r="29" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B29" s="56" t="s">
         <v>72</v>
       </c>
-      <c r="C26" s="50"/>
-      <c r="D26" s="55" t="s">
+      <c r="C29" s="56"/>
+      <c r="D29" s="54" t="s">
         <v>73</v>
       </c>
-      <c r="E26" s="50" t="s">
+      <c r="E29" s="56" t="s">
         <v>75</v>
       </c>
-      <c r="F26" s="50" t="s">
+      <c r="F29" s="56" t="s">
         <v>74</v>
       </c>
-      <c r="G26" s="50" t="s">
+      <c r="G29" s="56" t="s">
         <v>85</v>
       </c>
-      <c r="H26" s="50"/>
-      <c r="I26" s="50">
-        <v>1</v>
-      </c>
-      <c r="J26" s="50"/>
-      <c r="K26" s="50"/>
-      <c r="L26" s="50">
-        <v>1</v>
-      </c>
-      <c r="M26" s="50">
+      <c r="H29" s="56"/>
+      <c r="I29" s="56">
+        <v>1</v>
+      </c>
+      <c r="J29" s="56"/>
+      <c r="K29" s="56"/>
+      <c r="L29" s="56">
+        <v>1</v>
+      </c>
+      <c r="M29" s="56">
         <v>5</v>
       </c>
-      <c r="N26" s="50">
+      <c r="N29" s="56">
         <v>2000</v>
       </c>
-      <c r="O26" s="50">
+      <c r="O29" s="56">
         <v>620</v>
       </c>
-      <c r="P26" s="50">
-        <f>N26+O26</f>
+      <c r="P29" s="56">
+        <f>N29+O29</f>
         <v>2620</v>
       </c>
     </row>
-    <row r="27" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B27" s="50" t="s">
+    <row r="30" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B30" s="56" t="s">
         <v>72</v>
       </c>
-      <c r="C27" s="50"/>
-      <c r="D27" s="55" t="s">
+      <c r="C30" s="56"/>
+      <c r="D30" s="54" t="s">
         <v>76</v>
       </c>
-      <c r="E27" s="50" t="s">
+      <c r="E30" s="56" t="s">
         <v>82</v>
       </c>
-      <c r="F27" s="50" t="s">
+      <c r="F30" s="56" t="s">
         <v>81</v>
       </c>
-      <c r="G27" s="50" t="s">
+      <c r="G30" s="56" t="s">
         <v>85</v>
       </c>
-      <c r="H27" s="50"/>
-      <c r="I27" s="50"/>
-      <c r="J27" s="50">
-        <v>1</v>
-      </c>
-      <c r="K27" s="50"/>
-      <c r="L27" s="50">
-        <v>1</v>
-      </c>
-      <c r="M27" s="50">
+      <c r="H30" s="56"/>
+      <c r="I30" s="56"/>
+      <c r="J30" s="56">
+        <v>1</v>
+      </c>
+      <c r="K30" s="56"/>
+      <c r="L30" s="56">
+        <v>1</v>
+      </c>
+      <c r="M30" s="56">
         <v>5</v>
       </c>
-      <c r="N27" s="50">
+      <c r="N30" s="56">
         <v>1200</v>
       </c>
-      <c r="O27" s="50">
+      <c r="O30" s="56">
         <v>620</v>
       </c>
-      <c r="P27" s="50">
-        <f t="shared" ref="P27:P31" si="1">N27+O27</f>
+      <c r="P30" s="56">
+        <f t="shared" ref="P30:P34" si="2">N30+O30</f>
         <v>1820</v>
       </c>
     </row>
-    <row r="28" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B28" s="50" t="s">
+    <row r="31" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B31" s="56" t="s">
         <v>72</v>
       </c>
-      <c r="C28" s="50"/>
-      <c r="D28" s="55" t="s">
+      <c r="C31" s="56"/>
+      <c r="D31" s="54" t="s">
         <v>77</v>
       </c>
-      <c r="E28" s="50" t="s">
+      <c r="E31" s="56" t="s">
         <v>84</v>
       </c>
-      <c r="F28" s="50" t="s">
+      <c r="F31" s="56" t="s">
         <v>83</v>
       </c>
-      <c r="G28" s="50" t="s">
+      <c r="G31" s="56" t="s">
         <v>85</v>
       </c>
-      <c r="H28" s="50">
-        <v>1</v>
-      </c>
-      <c r="I28" s="50"/>
-      <c r="J28" s="50">
-        <v>1</v>
-      </c>
-      <c r="K28" s="50"/>
-      <c r="L28" s="50"/>
-      <c r="M28" s="50">
+      <c r="H31" s="56">
+        <v>1</v>
+      </c>
+      <c r="I31" s="56"/>
+      <c r="J31" s="56">
+        <v>1</v>
+      </c>
+      <c r="K31" s="56"/>
+      <c r="L31" s="56"/>
+      <c r="M31" s="56">
         <v>5</v>
       </c>
-      <c r="N28" s="50">
+      <c r="N31" s="56">
         <v>2000</v>
       </c>
-      <c r="O28" s="50">
+      <c r="O31" s="56">
         <v>620</v>
       </c>
-      <c r="P28" s="50">
-        <f t="shared" si="1"/>
+      <c r="P31" s="56">
+        <f t="shared" si="2"/>
         <v>2620</v>
       </c>
     </row>
-    <row r="29" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B29" s="50" t="s">
+    <row r="32" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B32" s="56" t="s">
         <v>72</v>
       </c>
-      <c r="C29" s="50"/>
-      <c r="D29" s="55" t="s">
+      <c r="C32" s="56"/>
+      <c r="D32" s="54" t="s">
         <v>78</v>
       </c>
-      <c r="E29" s="50" t="s">
+      <c r="E32" s="56" t="s">
         <v>84</v>
       </c>
-      <c r="F29" s="50" t="s">
+      <c r="F32" s="56" t="s">
         <v>86</v>
       </c>
-      <c r="G29" s="50" t="s">
+      <c r="G32" s="56" t="s">
         <v>85</v>
       </c>
-      <c r="H29" s="50"/>
-      <c r="I29" s="50"/>
-      <c r="J29" s="50">
-        <v>1</v>
-      </c>
-      <c r="K29" s="50"/>
-      <c r="L29" s="50">
-        <v>1</v>
-      </c>
-      <c r="M29" s="50">
+      <c r="H32" s="56"/>
+      <c r="I32" s="56"/>
+      <c r="J32" s="56">
+        <v>1</v>
+      </c>
+      <c r="K32" s="56"/>
+      <c r="L32" s="56">
+        <v>1</v>
+      </c>
+      <c r="M32" s="56">
         <v>5</v>
       </c>
-      <c r="N29" s="50">
+      <c r="N32" s="56">
         <v>2000</v>
       </c>
-      <c r="O29" s="50">
+      <c r="O32" s="56">
         <v>620</v>
       </c>
-      <c r="P29" s="50">
-        <f t="shared" si="1"/>
+      <c r="P32" s="56">
+        <f t="shared" si="2"/>
         <v>2620</v>
       </c>
     </row>
-    <row r="30" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B30" s="50" t="s">
+    <row r="33" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B33" s="56" t="s">
         <v>72</v>
       </c>
-      <c r="C30" s="50"/>
-      <c r="D30" s="55" t="s">
+      <c r="C33" s="56"/>
+      <c r="D33" s="54" t="s">
         <v>79</v>
       </c>
-      <c r="E30" s="50" t="s">
+      <c r="E33" s="56" t="s">
         <v>87</v>
       </c>
-      <c r="F30" s="50" t="s">
+      <c r="F33" s="56" t="s">
         <v>88</v>
       </c>
-      <c r="G30" s="50" t="s">
+      <c r="G33" s="56" t="s">
         <v>85</v>
       </c>
-      <c r="H30" s="50"/>
-      <c r="I30" s="50"/>
-      <c r="J30" s="50">
-        <v>1</v>
-      </c>
-      <c r="K30" s="50"/>
-      <c r="L30" s="50">
-        <v>1</v>
-      </c>
-      <c r="M30" s="50">
+      <c r="H33" s="56"/>
+      <c r="I33" s="56"/>
+      <c r="J33" s="56">
+        <v>1</v>
+      </c>
+      <c r="K33" s="56"/>
+      <c r="L33" s="56">
+        <v>1</v>
+      </c>
+      <c r="M33" s="56">
         <v>5</v>
       </c>
-      <c r="N30" s="50">
+      <c r="N33" s="56">
         <v>1200</v>
       </c>
-      <c r="O30" s="50">
+      <c r="O33" s="56">
         <v>620</v>
       </c>
-      <c r="P30" s="50">
-        <f t="shared" si="1"/>
+      <c r="P33" s="56">
+        <f t="shared" si="2"/>
         <v>1820</v>
       </c>
     </row>
-    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B31" s="50" t="s">
+    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B34" s="56" t="s">
         <v>72</v>
       </c>
-      <c r="C31" s="50"/>
-      <c r="D31" s="50" t="s">
+      <c r="C34" s="56"/>
+      <c r="D34" s="52" t="s">
         <v>80</v>
       </c>
-      <c r="E31" s="50" t="s">
+      <c r="E34" s="56" t="s">
         <v>89</v>
       </c>
-      <c r="F31" s="50" t="s">
+      <c r="F34" s="56" t="s">
         <v>90</v>
       </c>
-      <c r="G31" s="50" t="s">
+      <c r="G34" s="56" t="s">
         <v>85</v>
       </c>
-      <c r="H31" s="50">
-        <v>1</v>
-      </c>
-      <c r="I31" s="50">
-        <v>1</v>
-      </c>
-      <c r="J31" s="50"/>
-      <c r="K31" s="50"/>
-      <c r="L31" s="50"/>
-      <c r="M31" s="50">
+      <c r="H34" s="56">
+        <v>1</v>
+      </c>
+      <c r="I34" s="56">
+        <v>1</v>
+      </c>
+      <c r="J34" s="56"/>
+      <c r="K34" s="56"/>
+      <c r="L34" s="56"/>
+      <c r="M34" s="56">
         <v>5</v>
       </c>
-      <c r="N31" s="50">
+      <c r="N34" s="56">
         <v>1200</v>
       </c>
-      <c r="O31" s="50">
+      <c r="O34" s="56">
         <v>620</v>
       </c>
-      <c r="P31" s="50">
-        <f t="shared" si="1"/>
+      <c r="P34" s="56">
+        <f t="shared" si="2"/>
         <v>1820</v>
       </c>
-    </row>
-    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B32" s="47"/>
-      <c r="C32" s="47"/>
-      <c r="D32" s="50"/>
-      <c r="E32" s="47"/>
-      <c r="F32" s="47"/>
-      <c r="G32" s="47"/>
-      <c r="H32" s="47"/>
-      <c r="I32" s="47"/>
-      <c r="J32" s="47"/>
-      <c r="K32" s="47"/>
-      <c r="L32" s="47"/>
-      <c r="M32" s="47"/>
-      <c r="N32" s="47"/>
-      <c r="O32" s="47"/>
-      <c r="P32" s="47"/>
-    </row>
-    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B33" s="39"/>
-      <c r="C33" s="39"/>
-      <c r="D33" s="50"/>
-      <c r="E33" s="39"/>
-      <c r="F33" s="39"/>
-      <c r="G33" s="39"/>
-      <c r="H33" s="39"/>
-      <c r="I33" s="39"/>
-      <c r="J33" s="39"/>
-      <c r="K33" s="39"/>
-      <c r="L33" s="39"/>
-      <c r="M33" s="39"/>
-      <c r="N33" s="39"/>
-      <c r="O33" s="39"/>
-      <c r="P33" s="39"/>
-    </row>
-    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B34" s="39"/>
-      <c r="C34" s="39"/>
-      <c r="D34" s="50"/>
-      <c r="E34" s="39"/>
-      <c r="F34" s="39"/>
-      <c r="G34" s="39"/>
-      <c r="H34" s="39"/>
-      <c r="I34" s="39"/>
-      <c r="J34" s="39"/>
-      <c r="K34" s="39"/>
-      <c r="L34" s="39"/>
-      <c r="M34" s="39"/>
-      <c r="N34" s="39"/>
-      <c r="O34" s="39"/>
-      <c r="P34" s="39"/>
     </row>
     <row r="35" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B35" s="50"/>
@@ -3715,164 +3807,423 @@
       <c r="P35" s="50"/>
     </row>
     <row r="36" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B36" s="50"/>
-      <c r="C36" s="50"/>
-      <c r="D36" s="50"/>
-      <c r="E36" s="50"/>
-      <c r="F36" s="50"/>
-      <c r="G36" s="50"/>
-      <c r="H36" s="50"/>
-      <c r="I36" s="50"/>
-      <c r="J36" s="50"/>
-      <c r="K36" s="50"/>
-      <c r="L36" s="50"/>
-      <c r="M36" s="50"/>
-      <c r="N36" s="50"/>
-      <c r="O36" s="50"/>
-      <c r="P36" s="50"/>
+      <c r="B36" s="52"/>
+      <c r="C36" s="52"/>
+      <c r="D36" s="52"/>
+      <c r="E36" s="52"/>
+      <c r="F36" s="52"/>
+      <c r="G36" s="52"/>
+      <c r="H36" s="52"/>
+      <c r="I36" s="52"/>
+      <c r="J36" s="52"/>
+      <c r="K36" s="52"/>
+      <c r="L36" s="52"/>
+      <c r="M36" s="52"/>
+      <c r="N36" s="52"/>
+      <c r="O36" s="52"/>
+      <c r="P36" s="52"/>
     </row>
     <row r="37" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B37" s="50"/>
-      <c r="C37" s="50"/>
-      <c r="D37" s="50"/>
-      <c r="E37" s="50"/>
-      <c r="F37" s="50"/>
-      <c r="G37" s="50"/>
-      <c r="H37" s="50"/>
-      <c r="I37" s="50"/>
-      <c r="J37" s="50"/>
-      <c r="K37" s="50"/>
-      <c r="L37" s="50"/>
-      <c r="M37" s="50"/>
-      <c r="N37" s="50"/>
-      <c r="O37" s="50"/>
-      <c r="P37" s="50"/>
+      <c r="B37" s="52"/>
+      <c r="C37" s="52"/>
+      <c r="D37" s="52"/>
+      <c r="E37" s="52"/>
+      <c r="F37" s="52"/>
+      <c r="G37" s="52"/>
+      <c r="H37" s="52"/>
+      <c r="I37" s="52"/>
+      <c r="J37" s="52"/>
+      <c r="K37" s="52"/>
+      <c r="L37" s="52"/>
+      <c r="M37" s="52"/>
+      <c r="N37" s="52"/>
+      <c r="O37" s="52"/>
+      <c r="P37" s="52"/>
     </row>
     <row r="38" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B38" s="50"/>
-      <c r="C38" s="50"/>
-      <c r="D38" s="50"/>
-      <c r="E38" s="50"/>
-      <c r="F38" s="50"/>
-      <c r="G38" s="50"/>
-      <c r="H38" s="50"/>
-      <c r="I38" s="50"/>
-      <c r="J38" s="50"/>
-      <c r="K38" s="50"/>
-      <c r="L38" s="50"/>
-      <c r="M38" s="50"/>
-      <c r="N38" s="50"/>
-      <c r="O38" s="50"/>
-      <c r="P38" s="50"/>
+      <c r="B38" s="52"/>
+      <c r="C38" s="52"/>
+      <c r="D38" s="52"/>
+      <c r="E38" s="52"/>
+      <c r="F38" s="52"/>
+      <c r="G38" s="52"/>
+      <c r="H38" s="52"/>
+      <c r="I38" s="52"/>
+      <c r="J38" s="52"/>
+      <c r="K38" s="52"/>
+      <c r="L38" s="52"/>
+      <c r="M38" s="52"/>
+      <c r="N38" s="52"/>
+      <c r="O38" s="52"/>
+      <c r="P38" s="52"/>
     </row>
     <row r="39" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B39" s="50"/>
-      <c r="C39" s="50"/>
-      <c r="D39" s="50"/>
-      <c r="E39" s="50"/>
-      <c r="F39" s="50"/>
-      <c r="G39" s="50"/>
-      <c r="H39" s="50"/>
-      <c r="I39" s="50"/>
-      <c r="J39" s="50"/>
-      <c r="K39" s="50"/>
-      <c r="L39" s="50"/>
-      <c r="M39" s="50"/>
-      <c r="N39" s="50"/>
-      <c r="O39" s="50"/>
-      <c r="P39" s="50"/>
+      <c r="B39" s="52"/>
+      <c r="C39" s="52"/>
+      <c r="D39" s="52"/>
+      <c r="E39" s="52"/>
+      <c r="F39" s="52"/>
+      <c r="G39" s="52"/>
+      <c r="H39" s="52"/>
+      <c r="I39" s="52"/>
+      <c r="J39" s="52"/>
+      <c r="K39" s="52"/>
+      <c r="L39" s="52"/>
+      <c r="M39" s="52"/>
+      <c r="N39" s="52"/>
+      <c r="O39" s="52"/>
+      <c r="P39" s="52"/>
     </row>
     <row r="40" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B40" s="50"/>
-      <c r="C40" s="50"/>
-      <c r="D40" s="50"/>
-      <c r="E40" s="50"/>
-      <c r="F40" s="50"/>
-      <c r="G40" s="50"/>
-      <c r="H40" s="50"/>
-      <c r="I40" s="50"/>
-      <c r="J40" s="50"/>
-      <c r="K40" s="50"/>
-      <c r="L40" s="50"/>
-      <c r="M40" s="50"/>
-      <c r="N40" s="50"/>
-      <c r="O40" s="50"/>
-      <c r="P40" s="50"/>
+      <c r="B40" s="52"/>
+      <c r="C40" s="52"/>
+      <c r="D40" s="52"/>
+      <c r="E40" s="52"/>
+      <c r="F40" s="52"/>
+      <c r="G40" s="52"/>
+      <c r="H40" s="52"/>
+      <c r="I40" s="52"/>
+      <c r="J40" s="52"/>
+      <c r="K40" s="52"/>
+      <c r="L40" s="52"/>
+      <c r="M40" s="52"/>
+      <c r="N40" s="52"/>
+      <c r="O40" s="52"/>
+      <c r="P40" s="52"/>
     </row>
     <row r="41" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B41" s="39"/>
-      <c r="C41" s="39"/>
-      <c r="D41" s="39"/>
-      <c r="E41" s="39"/>
-      <c r="F41" s="39"/>
-      <c r="G41" s="39"/>
-      <c r="H41" s="39"/>
-      <c r="I41" s="39"/>
-      <c r="J41" s="39"/>
-      <c r="K41" s="39"/>
-      <c r="L41" s="39"/>
-      <c r="M41" s="39"/>
-      <c r="N41" s="39"/>
-      <c r="O41" s="39"/>
-      <c r="P41" s="39"/>
+      <c r="B41" s="52"/>
+      <c r="C41" s="52"/>
+      <c r="D41" s="52"/>
+      <c r="E41" s="52"/>
+      <c r="F41" s="52"/>
+      <c r="G41" s="52"/>
+      <c r="H41" s="52"/>
+      <c r="I41" s="52"/>
+      <c r="J41" s="52"/>
+      <c r="K41" s="52"/>
+      <c r="L41" s="52"/>
+      <c r="M41" s="52"/>
+      <c r="N41" s="52"/>
+      <c r="O41" s="52"/>
+      <c r="P41" s="52"/>
     </row>
     <row r="42" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B42" s="39"/>
-      <c r="C42" s="39"/>
-      <c r="D42" s="39"/>
-      <c r="E42" s="39"/>
-      <c r="F42" s="39"/>
-      <c r="G42" s="39"/>
-      <c r="H42" s="39"/>
-      <c r="I42" s="39"/>
-      <c r="J42" s="39"/>
-      <c r="K42" s="39"/>
-      <c r="L42" s="39"/>
-      <c r="M42" s="39"/>
-      <c r="N42" s="39"/>
-      <c r="O42" s="39"/>
-      <c r="P42" s="39"/>
-    </row>
-    <row r="43" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B43" s="39"/>
-      <c r="C43" s="39"/>
-      <c r="D43" s="39"/>
-      <c r="E43" s="39"/>
-      <c r="F43" s="39"/>
-      <c r="G43" s="39"/>
-      <c r="H43" s="39"/>
-      <c r="I43" s="39"/>
-      <c r="J43" s="39"/>
-      <c r="K43" s="39"/>
-      <c r="L43" s="39"/>
-      <c r="M43" s="39"/>
-      <c r="N43" s="39"/>
-      <c r="O43" s="39"/>
-      <c r="P43" s="39"/>
+      <c r="B42" s="52"/>
+      <c r="C42" s="52"/>
+      <c r="D42" s="52"/>
+      <c r="E42" s="52"/>
+      <c r="F42" s="52"/>
+      <c r="G42" s="52"/>
+      <c r="H42" s="52"/>
+      <c r="I42" s="52"/>
+      <c r="J42" s="52"/>
+      <c r="K42" s="52"/>
+      <c r="L42" s="52"/>
+      <c r="M42" s="52"/>
+      <c r="N42" s="52"/>
+      <c r="O42" s="52"/>
+      <c r="P42" s="52"/>
+    </row>
+    <row r="43" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B43" s="52"/>
+      <c r="C43" s="52"/>
+      <c r="D43" s="54"/>
+      <c r="E43" s="52"/>
+      <c r="F43" s="52"/>
+      <c r="G43" s="52"/>
+      <c r="H43" s="52"/>
+      <c r="I43" s="52"/>
+      <c r="J43" s="52"/>
+      <c r="K43" s="52"/>
+      <c r="L43" s="52"/>
+      <c r="M43" s="52"/>
+      <c r="N43" s="52"/>
+      <c r="O43" s="52"/>
+      <c r="P43" s="52"/>
     </row>
     <row r="44" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B44" s="39"/>
-      <c r="C44" s="39"/>
-      <c r="D44" s="39"/>
-      <c r="E44" s="39"/>
-      <c r="F44" s="39"/>
-      <c r="G44" s="39"/>
-      <c r="H44" s="39"/>
-      <c r="I44" s="39"/>
-      <c r="J44" s="39"/>
-      <c r="K44" s="39"/>
-      <c r="L44" s="39"/>
-      <c r="M44" s="39"/>
-      <c r="N44" s="39"/>
-      <c r="O44" s="39"/>
-      <c r="P44" s="39"/>
+      <c r="B44" s="52"/>
+      <c r="C44" s="52"/>
+      <c r="D44" s="52"/>
+      <c r="E44" s="52"/>
+      <c r="F44" s="52"/>
+      <c r="G44" s="52"/>
+      <c r="H44" s="52"/>
+      <c r="I44" s="52"/>
+      <c r="J44" s="52"/>
+      <c r="K44" s="52"/>
+      <c r="L44" s="52"/>
+      <c r="M44" s="52"/>
+      <c r="N44" s="52"/>
+      <c r="O44" s="52"/>
+      <c r="P44" s="52"/>
+    </row>
+    <row r="45" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B45" s="52"/>
+      <c r="C45" s="52"/>
+      <c r="D45" s="52"/>
+      <c r="E45" s="52"/>
+      <c r="F45" s="52"/>
+      <c r="G45" s="52"/>
+      <c r="H45" s="52"/>
+      <c r="I45" s="52"/>
+      <c r="J45" s="52"/>
+      <c r="K45" s="52"/>
+      <c r="L45" s="52"/>
+      <c r="M45" s="52"/>
+      <c r="N45" s="52"/>
+      <c r="O45" s="52"/>
+      <c r="P45" s="52"/>
+    </row>
+    <row r="46" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B46" s="52"/>
+      <c r="C46" s="52"/>
+      <c r="D46" s="52"/>
+      <c r="E46" s="52"/>
+      <c r="F46" s="52"/>
+      <c r="G46" s="52"/>
+      <c r="H46" s="52"/>
+      <c r="I46" s="52"/>
+      <c r="J46" s="52"/>
+      <c r="K46" s="52"/>
+      <c r="L46" s="52"/>
+      <c r="M46" s="52"/>
+      <c r="N46" s="52"/>
+      <c r="O46" s="52"/>
+      <c r="P46" s="52"/>
+    </row>
+    <row r="47" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B47" s="52"/>
+      <c r="C47" s="56"/>
+      <c r="D47" s="54"/>
+      <c r="E47" s="52"/>
+      <c r="F47" s="52"/>
+      <c r="G47" s="52"/>
+      <c r="H47" s="56"/>
+      <c r="I47" s="56"/>
+      <c r="J47" s="56"/>
+      <c r="K47" s="56"/>
+      <c r="L47" s="56"/>
+      <c r="M47" s="56"/>
+      <c r="N47" s="56"/>
+      <c r="O47" s="56"/>
+      <c r="P47" s="56"/>
+    </row>
+    <row r="48" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B48" s="52"/>
+      <c r="C48" s="56"/>
+      <c r="D48" s="52"/>
+      <c r="E48" s="52"/>
+      <c r="F48" s="52"/>
+      <c r="G48" s="52"/>
+      <c r="H48" s="52"/>
+      <c r="I48" s="52"/>
+      <c r="J48" s="52"/>
+      <c r="K48" s="56"/>
+      <c r="L48" s="56"/>
+      <c r="M48" s="56"/>
+      <c r="N48" s="56"/>
+      <c r="O48" s="56"/>
+      <c r="P48" s="56"/>
+    </row>
+    <row r="49" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B49" s="56"/>
+      <c r="C49" s="56"/>
+      <c r="D49" s="54"/>
+      <c r="E49" s="56"/>
+      <c r="F49" s="56"/>
+      <c r="G49" s="56"/>
+      <c r="H49" s="56"/>
+      <c r="I49" s="56"/>
+      <c r="J49" s="56"/>
+      <c r="K49" s="56"/>
+      <c r="L49" s="56"/>
+      <c r="M49" s="56"/>
+      <c r="N49" s="56"/>
+      <c r="O49" s="56"/>
+      <c r="P49" s="56"/>
+    </row>
+    <row r="50" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B50" s="56"/>
+      <c r="C50" s="56"/>
+      <c r="D50" s="54"/>
+      <c r="E50" s="56"/>
+      <c r="F50" s="56"/>
+      <c r="G50" s="56"/>
+      <c r="H50" s="56"/>
+      <c r="I50" s="56"/>
+      <c r="J50" s="56"/>
+      <c r="K50" s="56"/>
+      <c r="L50" s="56"/>
+      <c r="M50" s="56"/>
+      <c r="N50" s="56"/>
+      <c r="O50" s="56"/>
+      <c r="P50" s="56"/>
+    </row>
+    <row r="51" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B51" s="56"/>
+      <c r="C51" s="56"/>
+      <c r="D51" s="54"/>
+      <c r="E51" s="56"/>
+      <c r="F51" s="56"/>
+      <c r="G51" s="56"/>
+      <c r="H51" s="56"/>
+      <c r="I51" s="56"/>
+      <c r="J51" s="56"/>
+      <c r="K51" s="56"/>
+      <c r="L51" s="56"/>
+      <c r="M51" s="56"/>
+      <c r="N51" s="56"/>
+      <c r="O51" s="56"/>
+      <c r="P51" s="56"/>
+    </row>
+    <row r="52" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B52" s="56"/>
+      <c r="C52" s="56"/>
+      <c r="D52" s="54"/>
+      <c r="E52" s="56"/>
+      <c r="F52" s="56"/>
+      <c r="G52" s="56"/>
+      <c r="H52" s="56"/>
+      <c r="I52" s="56"/>
+      <c r="J52" s="56"/>
+      <c r="K52" s="56"/>
+      <c r="L52" s="56"/>
+      <c r="M52" s="56"/>
+      <c r="N52" s="56"/>
+      <c r="O52" s="56"/>
+      <c r="P52" s="56"/>
+    </row>
+    <row r="53" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B53" s="56"/>
+      <c r="C53" s="56"/>
+      <c r="D53" s="54"/>
+      <c r="E53" s="56"/>
+      <c r="F53" s="56"/>
+      <c r="G53" s="56"/>
+      <c r="H53" s="56"/>
+      <c r="I53" s="56"/>
+      <c r="J53" s="56"/>
+      <c r="K53" s="56"/>
+      <c r="L53" s="56"/>
+      <c r="M53" s="56"/>
+      <c r="N53" s="56"/>
+      <c r="O53" s="56"/>
+      <c r="P53" s="56"/>
+    </row>
+    <row r="54" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B54" s="56"/>
+      <c r="C54" s="56"/>
+      <c r="D54" s="52"/>
+      <c r="E54" s="56"/>
+      <c r="F54" s="56"/>
+      <c r="G54" s="56"/>
+      <c r="H54" s="56"/>
+      <c r="I54" s="56"/>
+      <c r="J54" s="56"/>
+      <c r="K54" s="56"/>
+      <c r="L54" s="56"/>
+      <c r="M54" s="56"/>
+      <c r="N54" s="56"/>
+      <c r="O54" s="56"/>
+      <c r="P54" s="56"/>
+    </row>
+    <row r="55" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B55" s="56"/>
+      <c r="C55" s="56"/>
+      <c r="D55" s="55"/>
+      <c r="E55" s="56"/>
+      <c r="F55" s="56"/>
+      <c r="G55" s="56"/>
+      <c r="H55" s="56"/>
+      <c r="I55" s="56"/>
+      <c r="J55" s="56"/>
+      <c r="K55" s="56"/>
+      <c r="L55" s="56"/>
+      <c r="M55" s="56"/>
+      <c r="N55" s="56"/>
+      <c r="O55" s="56"/>
+      <c r="P55" s="56"/>
+    </row>
+    <row r="56" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B56" s="56"/>
+      <c r="C56" s="56"/>
+      <c r="D56" s="55"/>
+      <c r="E56" s="56"/>
+      <c r="F56" s="56"/>
+      <c r="G56" s="56"/>
+      <c r="H56" s="56"/>
+      <c r="I56" s="56"/>
+      <c r="J56" s="56"/>
+      <c r="K56" s="56"/>
+      <c r="L56" s="56"/>
+      <c r="M56" s="56"/>
+      <c r="N56" s="56"/>
+      <c r="O56" s="56"/>
+      <c r="P56" s="56"/>
+    </row>
+    <row r="57" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B57" s="56"/>
+      <c r="C57" s="56"/>
+      <c r="D57" s="55"/>
+      <c r="E57" s="56"/>
+      <c r="F57" s="56"/>
+      <c r="G57" s="56"/>
+      <c r="H57" s="56"/>
+      <c r="I57" s="56"/>
+      <c r="J57" s="56"/>
+      <c r="K57" s="56"/>
+      <c r="L57" s="56"/>
+      <c r="M57" s="56"/>
+      <c r="N57" s="56"/>
+      <c r="O57" s="56"/>
+      <c r="P57" s="56"/>
+    </row>
+    <row r="58" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B58" s="56"/>
+      <c r="C58" s="56"/>
+      <c r="D58" s="55"/>
+      <c r="E58" s="56"/>
+      <c r="F58" s="56"/>
+      <c r="G58" s="56"/>
+      <c r="H58" s="56"/>
+      <c r="I58" s="56"/>
+      <c r="J58" s="56"/>
+      <c r="K58" s="56"/>
+      <c r="L58" s="56"/>
+      <c r="M58" s="56"/>
+      <c r="N58" s="56"/>
+      <c r="O58" s="56"/>
+      <c r="P58" s="56"/>
+    </row>
+    <row r="59" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B59" s="56"/>
+      <c r="C59" s="56"/>
+      <c r="D59" s="56"/>
+      <c r="E59" s="56"/>
+      <c r="F59" s="56"/>
+      <c r="G59" s="56"/>
+      <c r="H59" s="56"/>
+      <c r="I59" s="56"/>
+      <c r="J59" s="56"/>
+      <c r="K59" s="56"/>
+      <c r="L59" s="56"/>
+      <c r="M59" s="56"/>
+      <c r="N59" s="56"/>
+      <c r="O59" s="56"/>
+      <c r="P59" s="56"/>
     </row>
   </sheetData>
+  <autoFilter ref="B4:P34" xr:uid="{24D3D14F-C4FA-4576-ABA6-ACB55BFAAF61}"/>
   <mergeCells count="1">
     <mergeCell ref="B2:C2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="P15" formulaRange="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -3880,8 +4231,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:I35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10:E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3896,13 +4247,13 @@
   <sheetData>
     <row r="1" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="79" t="s">
+      <c r="B2" s="80" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="80"/>
+      <c r="C2" s="81"/>
       <c r="D2" s="43">
         <f>SUM(I5:I35)</f>
-        <v>20720</v>
+        <v>140730</v>
       </c>
     </row>
     <row r="4" spans="2:9" ht="45" x14ac:dyDescent="0.25">
@@ -4189,10 +4540,16 @@
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="39"/>
+      <c r="B15" s="56" t="s">
+        <v>91</v>
+      </c>
       <c r="C15" s="39"/>
-      <c r="D15" s="39"/>
-      <c r="E15" s="39"/>
+      <c r="D15" s="56" t="s">
+        <v>77</v>
+      </c>
+      <c r="E15" s="56" t="s">
+        <v>84</v>
+      </c>
       <c r="F15" s="49" t="s">
         <v>107</v>
       </c>
@@ -4213,17 +4570,17 @@
       <c r="D16" s="39"/>
       <c r="E16" s="39"/>
       <c r="F16" s="39" t="s">
-        <v>112</v>
+        <v>130</v>
       </c>
       <c r="G16" s="39">
-        <v>1000</v>
+        <v>10000</v>
       </c>
       <c r="H16" s="39">
         <v>1</v>
       </c>
       <c r="I16" s="39">
         <f t="shared" si="0"/>
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
@@ -4231,8 +4588,12 @@
       <c r="C17" s="39"/>
       <c r="D17" s="39"/>
       <c r="E17" s="39"/>
-      <c r="F17" s="39"/>
-      <c r="G17" s="39"/>
+      <c r="F17" s="39" t="s">
+        <v>132</v>
+      </c>
+      <c r="G17" s="39">
+        <v>980</v>
+      </c>
       <c r="H17" s="39"/>
       <c r="I17" s="39">
         <f t="shared" si="0"/>
@@ -4244,12 +4605,18 @@
       <c r="C18" s="39"/>
       <c r="D18" s="39"/>
       <c r="E18" s="39"/>
-      <c r="F18" s="39"/>
-      <c r="G18" s="39"/>
-      <c r="H18" s="39"/>
+      <c r="F18" s="39" t="s">
+        <v>131</v>
+      </c>
+      <c r="G18" s="39">
+        <v>98700</v>
+      </c>
+      <c r="H18" s="39">
+        <v>1</v>
+      </c>
       <c r="I18" s="39">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>98700</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
@@ -4257,12 +4624,18 @@
       <c r="C19" s="39"/>
       <c r="D19" s="39"/>
       <c r="E19" s="39"/>
-      <c r="F19" s="39"/>
-      <c r="G19" s="39"/>
-      <c r="H19" s="39"/>
+      <c r="F19" s="39" t="s">
+        <v>133</v>
+      </c>
+      <c r="G19" s="39">
+        <v>6155</v>
+      </c>
+      <c r="H19" s="39">
+        <v>2</v>
+      </c>
       <c r="I19" s="39">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>12310</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
@@ -4485,8 +4858,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4500,10 +4873,10 @@
   <sheetData>
     <row r="1" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="79" t="s">
+      <c r="B2" s="80" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="80"/>
+      <c r="C2" s="81"/>
       <c r="D2" s="43">
         <f>SUM(I5:I35)</f>
         <v>61200</v>
@@ -4549,7 +4922,7 @@
         <v>100</v>
       </c>
       <c r="F5" s="39" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G5" s="39">
         <v>140</v>
@@ -4564,7 +4937,7 @@
     </row>
     <row r="6" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="51" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C6" s="39"/>
       <c r="D6" s="54" t="s">
@@ -4574,7 +4947,7 @@
         <v>75</v>
       </c>
       <c r="F6" s="39" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G6" s="39">
         <v>40</v>
@@ -4589,7 +4962,7 @@
     </row>
     <row r="7" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="51" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C7" s="39"/>
       <c r="D7" s="55" t="s">
@@ -4599,7 +4972,7 @@
         <v>82</v>
       </c>
       <c r="F7" s="39" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G7" s="39">
         <v>20</v>
@@ -4614,7 +4987,7 @@
     </row>
     <row r="8" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="51" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C8" s="39"/>
       <c r="D8" s="55" t="s">
@@ -4624,7 +4997,7 @@
         <v>84</v>
       </c>
       <c r="F8" s="39" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G8" s="39">
         <v>20</v>
@@ -4639,7 +5012,7 @@
     </row>
     <row r="9" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="51" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C9" s="39"/>
       <c r="D9" s="55" t="s">
@@ -4649,7 +5022,7 @@
         <v>87</v>
       </c>
       <c r="F9" s="39" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G9" s="39">
         <v>20</v>
@@ -4664,7 +5037,7 @@
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="39" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C10" s="51" t="s">
         <v>92</v>
@@ -4676,7 +5049,7 @@
         <v>100</v>
       </c>
       <c r="F10" s="39" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G10" s="39">
         <v>30000</v>
@@ -4703,7 +5076,7 @@
         <v>100</v>
       </c>
       <c r="F11" s="39" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G11" s="39">
         <v>7000</v>
@@ -4728,7 +5101,7 @@
         <v>84</v>
       </c>
       <c r="F12" s="51" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G12" s="51">
         <v>7000</v>
@@ -4755,7 +5128,7 @@
         <v>100</v>
       </c>
       <c r="F13" s="39" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G13" s="39">
         <v>1000</v>
@@ -4780,7 +5153,7 @@
         <v>84</v>
       </c>
       <c r="F14" s="39" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G14" s="39">
         <v>15000</v>
@@ -4802,7 +5175,7 @@
       <c r="G15" s="39"/>
       <c r="H15" s="39"/>
       <c r="I15" s="39">
-        <f>G16*H16</f>
+        <f t="shared" ref="I15:I35" si="1">G16*H16</f>
         <v>0</v>
       </c>
     </row>
@@ -4815,7 +5188,7 @@
       <c r="G16" s="39"/>
       <c r="H16" s="39"/>
       <c r="I16" s="39">
-        <f>G17*H17</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -4828,7 +5201,7 @@
       <c r="G17" s="39"/>
       <c r="H17" s="39"/>
       <c r="I17" s="39">
-        <f>G18*H18</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -4841,7 +5214,7 @@
       <c r="G18" s="39"/>
       <c r="H18" s="39"/>
       <c r="I18" s="39">
-        <f>G19*H19</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -4854,7 +5227,7 @@
       <c r="G19" s="39"/>
       <c r="H19" s="39"/>
       <c r="I19" s="39">
-        <f>G20*H20</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -4867,7 +5240,7 @@
       <c r="G20" s="39"/>
       <c r="H20" s="39"/>
       <c r="I20" s="39">
-        <f>G21*H21</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -4880,7 +5253,7 @@
       <c r="G21" s="39"/>
       <c r="H21" s="39"/>
       <c r="I21" s="39">
-        <f>G22*H22</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -4893,7 +5266,7 @@
       <c r="G22" s="39"/>
       <c r="H22" s="39"/>
       <c r="I22" s="39">
-        <f>G23*H23</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -4906,7 +5279,7 @@
       <c r="G23" s="39"/>
       <c r="H23" s="39"/>
       <c r="I23" s="39">
-        <f>G24*H24</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -4919,7 +5292,7 @@
       <c r="G24" s="39"/>
       <c r="H24" s="39"/>
       <c r="I24" s="39">
-        <f>G25*H25</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -4932,7 +5305,7 @@
       <c r="G25" s="39"/>
       <c r="H25" s="39"/>
       <c r="I25" s="39">
-        <f>G26*H26</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -4945,7 +5318,7 @@
       <c r="G26" s="39"/>
       <c r="H26" s="39"/>
       <c r="I26" s="39">
-        <f>G27*H27</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -4958,7 +5331,7 @@
       <c r="G27" s="39"/>
       <c r="H27" s="39"/>
       <c r="I27" s="39">
-        <f>G28*H28</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -4971,7 +5344,7 @@
       <c r="G28" s="39"/>
       <c r="H28" s="39"/>
       <c r="I28" s="39">
-        <f>G29*H29</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -4984,7 +5357,7 @@
       <c r="G29" s="39"/>
       <c r="H29" s="39"/>
       <c r="I29" s="39">
-        <f>G30*H30</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -4997,7 +5370,7 @@
       <c r="G30" s="39"/>
       <c r="H30" s="39"/>
       <c r="I30" s="39">
-        <f>G31*H31</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -5010,7 +5383,7 @@
       <c r="G31" s="39"/>
       <c r="H31" s="39"/>
       <c r="I31" s="39">
-        <f>G32*H32</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -5023,7 +5396,7 @@
       <c r="G32" s="39"/>
       <c r="H32" s="39"/>
       <c r="I32" s="39">
-        <f>G33*H33</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -5036,7 +5409,7 @@
       <c r="G33" s="39"/>
       <c r="H33" s="39"/>
       <c r="I33" s="39">
-        <f>G34*H34</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -5049,7 +5422,7 @@
       <c r="G34" s="39"/>
       <c r="H34" s="39"/>
       <c r="I34" s="39">
-        <f>G35*H35</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -5062,7 +5435,7 @@
       <c r="G35" s="39"/>
       <c r="H35" s="39"/>
       <c r="I35" s="39">
-        <f>G36*H36</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Sub i equipment malo bolji
</commit_message>
<xml_diff>
--- a/2b Format partner budget - Horizon2020.xlsx
+++ b/2b Format partner budget - Horizon2020.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23901"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ZORAN\Desktop\USP_projekat\CardioGuardian\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{777409D9-2E42-4446-AB45-E2DD7C6A2C8B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Detaljno budzet" sheetId="1" r:id="rId1"/>
@@ -19,9 +18,10 @@
     <sheet name="Subcontracting - budzet" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Equipment - budzet'!$B$4:$I$34</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Travel - budzet'!$B$4:$P$34</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -37,12 +37,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Kampen, Jan-Joris van</author>
   </authors>
   <commentList>
-    <comment ref="O13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="O13" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="128">
   <si>
     <t>Partner budget Horizon 2020</t>
   </si>
@@ -391,9 +391,6 @@
     <t>Крвни притисак сензор - Опсег притиска: 0 mmHg to 258 mmHg, време одзива: 1 millisecond, тачност: ±1 mmHg</t>
   </si>
   <si>
-    <t>графичка картица - минималне карактеристике: 12GB RАМ, 1.6GHz GPU Clock rate, са “blower-style” вентилаторима, 3800 језгара</t>
-  </si>
-  <si>
     <t>Штампач - ласерски, брзина штампе: 19 страница у минути, месечни обим штампе: 8000 страница</t>
   </si>
   <si>
@@ -403,12 +400,6 @@
     <t>Мобилни телефон - смарт телефон са напредним функционалностима, најновије генерације</t>
   </si>
   <si>
-    <t>рачунар - 500GB SSD, 16GB RAM, CPU 7 или новија генерација</t>
-  </si>
-  <si>
-    <t>рачунар- 500GB SSD, 16GB RAM, CPU 7 или новија генерација</t>
-  </si>
-  <si>
     <t>WP2</t>
   </si>
   <si>
@@ -424,30 +415,6 @@
     <t>Токио, Јапан</t>
   </si>
   <si>
-    <t xml:space="preserve">Превођење извештаја о напретку </t>
-  </si>
-  <si>
-    <t>WP3</t>
-  </si>
-  <si>
-    <t>Превођење корисничких захтева за хардверску и софтверску компоненту</t>
-  </si>
-  <si>
-    <t>Превођење анализе и детаља система</t>
-  </si>
-  <si>
-    <t>Превођење извештаја о успешности интеграције</t>
-  </si>
-  <si>
-    <t>WP6</t>
-  </si>
-  <si>
-    <t>Превођење извештаја тестирања</t>
-  </si>
-  <si>
-    <t>WP7</t>
-  </si>
-  <si>
     <t>Адвокатске услуге</t>
   </si>
   <si>
@@ -463,22 +430,37 @@
     <t>Услуге фирме за маркетинг</t>
   </si>
   <si>
-    <t>Сервер - минимум: 256GB REG ECC DDR4 RAM, CPU: 22 језгра, 2.20GHz, 55MB Cache</t>
-  </si>
-  <si>
     <t xml:space="preserve">Сервер - минимум: 4 CPU: 22 jezgra, 2.10GHz, 55MB Cache; 1024GB REG DDR4 </t>
   </si>
   <si>
-    <t xml:space="preserve">Windows Server Standard 2019 </t>
-  </si>
-  <si>
     <t xml:space="preserve">Windows Server Datacenter 2019 </t>
+  </si>
+  <si>
+    <t>Autodesk Product Design &amp; Manufacturing Collection (AutoCad, Inventor, Fusion360)</t>
+  </si>
+  <si>
+    <t>Графичка карта - 32 GB, 32 CPUs, 640 Tensor Cores, deep learning:130 teraFLOPS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Google cloud - TPU (Tensor Processing Unit) </t>
+  </si>
+  <si>
+    <t>рачунар - 500GB SSD, 32GB RAM, CPU 7 или новија генерација</t>
+  </si>
+  <si>
+    <t>рачунар- 500GB SSD, 32GB RAM, CPU 7 или новија генерација</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Услуге - Equinix data center </t>
+  </si>
+  <si>
+    <t>WP4 - WP8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
@@ -840,7 +822,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -951,6 +933,8 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1069,7 +1053,7 @@
         <xdr:cNvPr id="3" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA4F558B-8D56-430D-AA83-772AD1DE26DE}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA4F558B-8D56-430D-AA83-772AD1DE26DE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1204,23 +1188,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1256,23 +1223,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1448,7 +1398,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -1480,65 +1430,65 @@
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="E3" s="58"/>
-      <c r="F3" s="58"/>
-      <c r="G3" s="58"/>
-      <c r="H3" s="58"/>
-      <c r="I3" s="58"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="60"/>
+      <c r="H3" s="60"/>
+      <c r="I3" s="60"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D4" s="2"/>
-      <c r="E4" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" s="60"/>
-      <c r="G4" s="60"/>
-      <c r="H4" s="60"/>
-      <c r="I4" s="60"/>
+      <c r="E4" s="61" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="62"/>
+      <c r="G4" s="62"/>
+      <c r="H4" s="62"/>
+      <c r="I4" s="62"/>
       <c r="J4" s="3"/>
-      <c r="L4" s="60" t="s">
+      <c r="L4" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="M4" s="60"/>
-      <c r="N4" s="60"/>
+      <c r="M4" s="62"/>
+      <c r="N4" s="62"/>
       <c r="O4" s="4">
         <v>0.25</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D5" s="2"/>
-      <c r="E5" s="59" t="s">
+      <c r="E5" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="60"/>
-      <c r="G5" s="60"/>
-      <c r="H5" s="60"/>
-      <c r="I5" s="60"/>
+      <c r="F5" s="62"/>
+      <c r="G5" s="62"/>
+      <c r="H5" s="62"/>
+      <c r="I5" s="62"/>
       <c r="J5" s="3"/>
-      <c r="L5" s="60" t="s">
+      <c r="L5" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="M5" s="60"/>
-      <c r="N5" s="60"/>
+      <c r="M5" s="62"/>
+      <c r="N5" s="62"/>
       <c r="O5" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D6" s="2"/>
-      <c r="E6" s="59" t="s">
+      <c r="E6" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="60"/>
-      <c r="G6" s="60"/>
-      <c r="H6" s="60"/>
-      <c r="I6" s="60"/>
+      <c r="F6" s="62"/>
+      <c r="G6" s="62"/>
+      <c r="H6" s="62"/>
+      <c r="I6" s="62"/>
       <c r="J6" s="3"/>
-      <c r="L6" s="60" t="s">
+      <c r="L6" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="M6" s="60"/>
-      <c r="N6" s="60"/>
+      <c r="M6" s="62"/>
+      <c r="N6" s="62"/>
       <c r="O6" s="5">
         <v>0.7</v>
       </c>
@@ -1548,19 +1498,19 @@
       <c r="Q6" s="6"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="E7" s="60" t="s">
+      <c r="E7" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="60"/>
-      <c r="G7" s="60"/>
-      <c r="H7" s="60"/>
-      <c r="I7" s="60"/>
+      <c r="F7" s="62"/>
+      <c r="G7" s="62"/>
+      <c r="H7" s="62"/>
+      <c r="I7" s="62"/>
       <c r="J7" s="3"/>
-      <c r="L7" s="60" t="s">
+      <c r="L7" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="M7" s="60"/>
-      <c r="N7" s="60"/>
+      <c r="M7" s="62"/>
+      <c r="N7" s="62"/>
       <c r="O7" s="4">
         <v>1</v>
       </c>
@@ -1571,56 +1521,56 @@
     </row>
     <row r="9" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="61" t="s">
+      <c r="A10" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="62"/>
-      <c r="C10" s="62"/>
-      <c r="D10" s="62"/>
-      <c r="E10" s="62"/>
-      <c r="F10" s="62"/>
-      <c r="G10" s="62"/>
-      <c r="H10" s="62"/>
-      <c r="I10" s="62"/>
-      <c r="J10" s="62"/>
-      <c r="K10" s="62"/>
-      <c r="L10" s="62"/>
-      <c r="M10" s="62"/>
-      <c r="N10" s="62"/>
-      <c r="O10" s="62"/>
-      <c r="P10" s="62"/>
-      <c r="Q10" s="62"/>
-      <c r="R10" s="62"/>
+      <c r="B10" s="64"/>
+      <c r="C10" s="64"/>
+      <c r="D10" s="64"/>
+      <c r="E10" s="64"/>
+      <c r="F10" s="64"/>
+      <c r="G10" s="64"/>
+      <c r="H10" s="64"/>
+      <c r="I10" s="64"/>
+      <c r="J10" s="64"/>
+      <c r="K10" s="64"/>
+      <c r="L10" s="64"/>
+      <c r="M10" s="64"/>
+      <c r="N10" s="64"/>
+      <c r="O10" s="64"/>
+      <c r="P10" s="64"/>
+      <c r="Q10" s="64"/>
+      <c r="R10" s="64"/>
       <c r="S10" s="8"/>
     </row>
     <row r="12" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D12" s="63" t="s">
+      <c r="D12" s="65" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="63"/>
-      <c r="F12" s="63"/>
-      <c r="G12" s="63"/>
-      <c r="H12" s="63"/>
-      <c r="I12" s="63"/>
-      <c r="J12" s="64" t="s">
+      <c r="E12" s="65"/>
+      <c r="F12" s="65"/>
+      <c r="G12" s="65"/>
+      <c r="H12" s="65"/>
+      <c r="I12" s="65"/>
+      <c r="J12" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="K12" s="64"/>
-      <c r="L12" s="64"/>
-      <c r="M12" s="64"/>
-      <c r="N12" s="64"/>
-      <c r="O12" s="64"/>
-      <c r="P12" s="64"/>
-      <c r="Q12" s="64"/>
-      <c r="R12" s="64"/>
+      <c r="K12" s="66"/>
+      <c r="L12" s="66"/>
+      <c r="M12" s="66"/>
+      <c r="N12" s="66"/>
+      <c r="O12" s="66"/>
+      <c r="P12" s="66"/>
+      <c r="Q12" s="66"/>
+      <c r="R12" s="66"/>
       <c r="S12" s="9"/>
     </row>
     <row r="13" spans="1:19" s="14" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="57" t="s">
+      <c r="A13" s="59" t="s">
         <v>61</v>
       </c>
-      <c r="B13" s="57"/>
-      <c r="C13" s="57"/>
+      <c r="B13" s="59"/>
+      <c r="C13" s="59"/>
       <c r="D13" s="48" t="s">
         <v>70</v>
       </c>
@@ -1671,11 +1621,11 @@
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="66" t="s">
+      <c r="A14" s="68" t="s">
         <v>42</v>
       </c>
-      <c r="B14" s="66"/>
-      <c r="C14" s="66"/>
+      <c r="B14" s="68"/>
+      <c r="C14" s="68"/>
       <c r="D14" s="15"/>
       <c r="E14" s="15"/>
       <c r="F14" s="15"/>
@@ -1706,11 +1656,11 @@
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="66" t="s">
+      <c r="A15" s="68" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="66"/>
-      <c r="C15" s="66"/>
+      <c r="B15" s="68"/>
+      <c r="C15" s="68"/>
       <c r="D15" s="15"/>
       <c r="E15" s="15"/>
       <c r="F15" s="15"/>
@@ -1741,11 +1691,11 @@
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" s="66" t="s">
+      <c r="A16" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="66"/>
-      <c r="C16" s="66"/>
+      <c r="B16" s="68"/>
+      <c r="C16" s="68"/>
       <c r="D16" s="15"/>
       <c r="E16" s="15"/>
       <c r="F16" s="15"/>
@@ -1776,11 +1726,11 @@
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" s="66" t="s">
+      <c r="A17" s="68" t="s">
         <v>45</v>
       </c>
-      <c r="B17" s="66"/>
-      <c r="C17" s="66"/>
+      <c r="B17" s="68"/>
+      <c r="C17" s="68"/>
       <c r="D17" s="15"/>
       <c r="E17" s="15"/>
       <c r="F17" s="15"/>
@@ -1811,11 +1761,11 @@
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A18" s="66" t="s">
+      <c r="A18" s="68" t="s">
         <v>46</v>
       </c>
-      <c r="B18" s="66"/>
-      <c r="C18" s="66"/>
+      <c r="B18" s="68"/>
+      <c r="C18" s="68"/>
       <c r="D18" s="15"/>
       <c r="E18" s="15"/>
       <c r="F18" s="15"/>
@@ -1846,11 +1796,11 @@
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" s="66" t="s">
+      <c r="A19" s="68" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="66"/>
-      <c r="C19" s="66"/>
+      <c r="B19" s="68"/>
+      <c r="C19" s="68"/>
       <c r="D19" s="15"/>
       <c r="E19" s="15"/>
       <c r="F19" s="15"/>
@@ -1881,11 +1831,11 @@
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A20" s="66" t="s">
+      <c r="A20" s="68" t="s">
         <v>48</v>
       </c>
-      <c r="B20" s="66"/>
-      <c r="C20" s="66"/>
+      <c r="B20" s="68"/>
+      <c r="C20" s="68"/>
       <c r="D20" s="15"/>
       <c r="E20" s="15"/>
       <c r="F20" s="15"/>
@@ -1916,11 +1866,11 @@
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A21" s="66" t="s">
+      <c r="A21" s="68" t="s">
         <v>49</v>
       </c>
-      <c r="B21" s="66"/>
-      <c r="C21" s="66"/>
+      <c r="B21" s="68"/>
+      <c r="C21" s="68"/>
       <c r="D21" s="15"/>
       <c r="E21" s="15"/>
       <c r="F21" s="15"/>
@@ -1951,11 +1901,11 @@
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A22" s="66" t="s">
+      <c r="A22" s="68" t="s">
         <v>50</v>
       </c>
-      <c r="B22" s="66"/>
-      <c r="C22" s="66"/>
+      <c r="B22" s="68"/>
+      <c r="C22" s="68"/>
       <c r="D22" s="15"/>
       <c r="E22" s="15"/>
       <c r="F22" s="15"/>
@@ -1986,11 +1936,11 @@
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A23" s="66" t="s">
+      <c r="A23" s="68" t="s">
         <v>51</v>
       </c>
-      <c r="B23" s="66"/>
-      <c r="C23" s="66"/>
+      <c r="B23" s="68"/>
+      <c r="C23" s="68"/>
       <c r="D23" s="15"/>
       <c r="E23" s="15"/>
       <c r="F23" s="15"/>
@@ -2021,11 +1971,11 @@
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A24" s="67" t="s">
+      <c r="A24" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="67"/>
-      <c r="C24" s="67"/>
+      <c r="B24" s="69"/>
+      <c r="C24" s="69"/>
       <c r="D24" s="15">
         <f>SUM(D14:D23)</f>
         <v>0</v>
@@ -2146,24 +2096,24 @@
       <c r="S27" s="31"/>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A28" s="65" t="s">
+      <c r="A28" s="67" t="s">
         <v>30</v>
       </c>
-      <c r="B28" s="65"/>
-      <c r="C28" s="65"/>
-      <c r="D28" s="65"/>
-      <c r="E28" s="65"/>
-      <c r="F28" s="65"/>
-      <c r="G28" s="65"/>
-      <c r="H28" s="65"/>
-      <c r="I28" s="65"/>
-      <c r="J28" s="65"/>
-      <c r="K28" s="65"/>
-      <c r="L28" s="65"/>
-      <c r="M28" s="65"/>
-      <c r="N28" s="65"/>
-      <c r="O28" s="65"/>
-      <c r="P28" s="65"/>
+      <c r="B28" s="67"/>
+      <c r="C28" s="67"/>
+      <c r="D28" s="67"/>
+      <c r="E28" s="67"/>
+      <c r="F28" s="67"/>
+      <c r="G28" s="67"/>
+      <c r="H28" s="67"/>
+      <c r="I28" s="67"/>
+      <c r="J28" s="67"/>
+      <c r="K28" s="67"/>
+      <c r="L28" s="67"/>
+      <c r="M28" s="67"/>
+      <c r="N28" s="67"/>
+      <c r="O28" s="67"/>
+      <c r="P28" s="67"/>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="32"/>
@@ -2204,95 +2154,95 @@
       <c r="P30" s="32"/>
     </row>
     <row r="31" spans="1:20" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="68" t="str">
+      <c r="A31" s="70" t="str">
         <f>CONCATENATE("participant"," ",J6)</f>
         <v xml:space="preserve">participant </v>
       </c>
-      <c r="B31" s="69"/>
+      <c r="B31" s="71"/>
       <c r="C31" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="D31" s="66" t="s">
+      <c r="D31" s="68" t="s">
         <v>33</v>
       </c>
-      <c r="E31" s="70"/>
-      <c r="F31" s="70"/>
-      <c r="G31" s="70"/>
-      <c r="H31" s="70"/>
-      <c r="I31" s="70"/>
-      <c r="J31" s="70"/>
-      <c r="K31" s="70"/>
-      <c r="L31" s="70"/>
-      <c r="M31" s="70"/>
-      <c r="N31" s="70"/>
-      <c r="O31" s="70"/>
-      <c r="P31" s="70"/>
+      <c r="E31" s="72"/>
+      <c r="F31" s="72"/>
+      <c r="G31" s="72"/>
+      <c r="H31" s="72"/>
+      <c r="I31" s="72"/>
+      <c r="J31" s="72"/>
+      <c r="K31" s="72"/>
+      <c r="L31" s="72"/>
+      <c r="M31" s="72"/>
+      <c r="N31" s="72"/>
+      <c r="O31" s="72"/>
+      <c r="P31" s="72"/>
     </row>
     <row r="32" spans="1:20" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="71" t="s">
+      <c r="A32" s="73" t="s">
         <v>34</v>
       </c>
-      <c r="B32" s="71"/>
+      <c r="B32" s="73"/>
       <c r="C32" s="34"/>
-      <c r="D32" s="72" t="s">
+      <c r="D32" s="74" t="s">
         <v>67</v>
       </c>
-      <c r="E32" s="73"/>
-      <c r="F32" s="73"/>
-      <c r="G32" s="73"/>
-      <c r="H32" s="73"/>
-      <c r="I32" s="73"/>
-      <c r="J32" s="73"/>
-      <c r="K32" s="73"/>
-      <c r="L32" s="73"/>
-      <c r="M32" s="73"/>
-      <c r="N32" s="73"/>
-      <c r="O32" s="73"/>
-      <c r="P32" s="73"/>
+      <c r="E32" s="75"/>
+      <c r="F32" s="75"/>
+      <c r="G32" s="75"/>
+      <c r="H32" s="75"/>
+      <c r="I32" s="75"/>
+      <c r="J32" s="75"/>
+      <c r="K32" s="75"/>
+      <c r="L32" s="75"/>
+      <c r="M32" s="75"/>
+      <c r="N32" s="75"/>
+      <c r="O32" s="75"/>
+      <c r="P32" s="75"/>
       <c r="S32" s="31"/>
     </row>
     <row r="33" spans="1:19" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="71" t="s">
+      <c r="A33" s="73" t="s">
         <v>35</v>
       </c>
-      <c r="B33" s="71"/>
+      <c r="B33" s="73"/>
       <c r="C33" s="35"/>
-      <c r="D33" s="73" t="s">
+      <c r="D33" s="75" t="s">
         <v>68</v>
       </c>
-      <c r="E33" s="73"/>
-      <c r="F33" s="73"/>
-      <c r="G33" s="73"/>
-      <c r="H33" s="73"/>
-      <c r="I33" s="73"/>
-      <c r="J33" s="73"/>
-      <c r="K33" s="73"/>
-      <c r="L33" s="73"/>
-      <c r="M33" s="73"/>
-      <c r="N33" s="73"/>
-      <c r="O33" s="73"/>
-      <c r="P33" s="73"/>
+      <c r="E33" s="75"/>
+      <c r="F33" s="75"/>
+      <c r="G33" s="75"/>
+      <c r="H33" s="75"/>
+      <c r="I33" s="75"/>
+      <c r="J33" s="75"/>
+      <c r="K33" s="75"/>
+      <c r="L33" s="75"/>
+      <c r="M33" s="75"/>
+      <c r="N33" s="75"/>
+      <c r="O33" s="75"/>
+      <c r="P33" s="75"/>
       <c r="S33" s="31"/>
     </row>
     <row r="34" spans="1:19" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="71" t="s">
+      <c r="A34" s="73" t="s">
         <v>36</v>
       </c>
-      <c r="B34" s="71"/>
+      <c r="B34" s="73"/>
       <c r="C34" s="35"/>
-      <c r="D34" s="73"/>
-      <c r="E34" s="73"/>
-      <c r="F34" s="73"/>
-      <c r="G34" s="73"/>
-      <c r="H34" s="73"/>
-      <c r="I34" s="73"/>
-      <c r="J34" s="73"/>
-      <c r="K34" s="73"/>
-      <c r="L34" s="73"/>
-      <c r="M34" s="73"/>
-      <c r="N34" s="73"/>
-      <c r="O34" s="73"/>
-      <c r="P34" s="73"/>
+      <c r="D34" s="75"/>
+      <c r="E34" s="75"/>
+      <c r="F34" s="75"/>
+      <c r="G34" s="75"/>
+      <c r="H34" s="75"/>
+      <c r="I34" s="75"/>
+      <c r="J34" s="75"/>
+      <c r="K34" s="75"/>
+      <c r="L34" s="75"/>
+      <c r="M34" s="75"/>
+      <c r="N34" s="75"/>
+      <c r="O34" s="75"/>
+      <c r="P34" s="75"/>
       <c r="S34" s="31"/>
     </row>
     <row r="35" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.25">
@@ -2326,97 +2276,97 @@
       <c r="P36" s="38"/>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A37" s="68" t="str">
+      <c r="A37" s="70" t="str">
         <f>CONCATENATE("participant"," ",C9)</f>
         <v xml:space="preserve">participant </v>
       </c>
-      <c r="B37" s="69"/>
+      <c r="B37" s="71"/>
       <c r="C37" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="D37" s="78" t="s">
+      <c r="D37" s="80" t="s">
         <v>33</v>
       </c>
-      <c r="E37" s="79"/>
-      <c r="F37" s="79"/>
-      <c r="G37" s="79"/>
-      <c r="H37" s="79"/>
-      <c r="I37" s="79"/>
-      <c r="J37" s="79"/>
-      <c r="K37" s="79"/>
-      <c r="L37" s="79"/>
-      <c r="M37" s="79"/>
-      <c r="N37" s="79"/>
-      <c r="O37" s="79"/>
-      <c r="P37" s="79"/>
+      <c r="E37" s="81"/>
+      <c r="F37" s="81"/>
+      <c r="G37" s="81"/>
+      <c r="H37" s="81"/>
+      <c r="I37" s="81"/>
+      <c r="J37" s="81"/>
+      <c r="K37" s="81"/>
+      <c r="L37" s="81"/>
+      <c r="M37" s="81"/>
+      <c r="N37" s="81"/>
+      <c r="O37" s="81"/>
+      <c r="P37" s="81"/>
     </row>
     <row r="38" spans="1:19" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="71" t="s">
+      <c r="A38" s="73" t="s">
         <v>37</v>
       </c>
-      <c r="B38" s="71"/>
+      <c r="B38" s="73"/>
       <c r="C38" s="35"/>
-      <c r="D38" s="77" t="s">
+      <c r="D38" s="79" t="s">
         <v>69</v>
       </c>
-      <c r="E38" s="73"/>
-      <c r="F38" s="73"/>
-      <c r="G38" s="73"/>
-      <c r="H38" s="73"/>
-      <c r="I38" s="73"/>
-      <c r="J38" s="73"/>
-      <c r="K38" s="73"/>
-      <c r="L38" s="73"/>
-      <c r="M38" s="73"/>
-      <c r="N38" s="73"/>
-      <c r="O38" s="73"/>
-      <c r="P38" s="73"/>
+      <c r="E38" s="75"/>
+      <c r="F38" s="75"/>
+      <c r="G38" s="75"/>
+      <c r="H38" s="75"/>
+      <c r="I38" s="75"/>
+      <c r="J38" s="75"/>
+      <c r="K38" s="75"/>
+      <c r="L38" s="75"/>
+      <c r="M38" s="75"/>
+      <c r="N38" s="75"/>
+      <c r="O38" s="75"/>
+      <c r="P38" s="75"/>
       <c r="S38" s="31"/>
     </row>
     <row r="39" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="71" t="s">
+      <c r="A39" s="73" t="s">
         <v>38</v>
       </c>
-      <c r="B39" s="71"/>
+      <c r="B39" s="73"/>
       <c r="C39" s="35"/>
-      <c r="D39" s="74" t="s">
+      <c r="D39" s="76" t="s">
         <v>39</v>
       </c>
-      <c r="E39" s="75"/>
-      <c r="F39" s="75"/>
-      <c r="G39" s="75"/>
-      <c r="H39" s="75"/>
-      <c r="I39" s="75"/>
-      <c r="J39" s="75"/>
-      <c r="K39" s="75"/>
-      <c r="L39" s="75"/>
-      <c r="M39" s="75"/>
-      <c r="N39" s="75"/>
-      <c r="O39" s="75"/>
-      <c r="P39" s="76"/>
+      <c r="E39" s="77"/>
+      <c r="F39" s="77"/>
+      <c r="G39" s="77"/>
+      <c r="H39" s="77"/>
+      <c r="I39" s="77"/>
+      <c r="J39" s="77"/>
+      <c r="K39" s="77"/>
+      <c r="L39" s="77"/>
+      <c r="M39" s="77"/>
+      <c r="N39" s="77"/>
+      <c r="O39" s="77"/>
+      <c r="P39" s="78"/>
       <c r="S39" s="31"/>
     </row>
     <row r="40" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="71" t="s">
+      <c r="A40" s="73" t="s">
         <v>40</v>
       </c>
-      <c r="B40" s="71"/>
+      <c r="B40" s="73"/>
       <c r="C40" s="35"/>
-      <c r="D40" s="77" t="s">
+      <c r="D40" s="79" t="s">
         <v>41</v>
       </c>
-      <c r="E40" s="73"/>
-      <c r="F40" s="73"/>
-      <c r="G40" s="73"/>
-      <c r="H40" s="73"/>
-      <c r="I40" s="73"/>
-      <c r="J40" s="73"/>
-      <c r="K40" s="73"/>
-      <c r="L40" s="73"/>
-      <c r="M40" s="73"/>
-      <c r="N40" s="73"/>
-      <c r="O40" s="73"/>
-      <c r="P40" s="73"/>
+      <c r="E40" s="75"/>
+      <c r="F40" s="75"/>
+      <c r="G40" s="75"/>
+      <c r="H40" s="75"/>
+      <c r="I40" s="75"/>
+      <c r="J40" s="75"/>
+      <c r="K40" s="75"/>
+      <c r="L40" s="75"/>
+      <c r="M40" s="75"/>
+      <c r="N40" s="75"/>
+      <c r="O40" s="75"/>
+      <c r="P40" s="75"/>
       <c r="S40" s="31"/>
     </row>
   </sheetData>
@@ -2472,7 +2422,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O6" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O6">
       <formula1>"70%, 100%"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2484,11 +2434,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:P59"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2501,10 +2451,10 @@
   <sheetData>
     <row r="1" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="80" t="s">
+      <c r="B2" s="82" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="81"/>
+      <c r="C2" s="83"/>
       <c r="D2" s="43">
         <f>SUM(P5:P60)</f>
         <v>129580</v>
@@ -2633,7 +2583,7 @@
         <v>620</v>
       </c>
       <c r="P6" s="52">
-        <f t="shared" ref="P6:P25" si="0">N6+O6</f>
+        <f t="shared" ref="P6:P14" si="0">N6+O6</f>
         <v>1820</v>
       </c>
     </row>
@@ -2795,7 +2745,7 @@
     </row>
     <row r="11" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="52" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C11" s="52"/>
       <c r="D11" s="54" t="s">
@@ -2808,7 +2758,7 @@
         <v>74</v>
       </c>
       <c r="G11" s="52" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="H11" s="52">
         <v>1</v>
@@ -2837,7 +2787,7 @@
     </row>
     <row r="12" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="52" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C12" s="52"/>
       <c r="D12" s="54" t="s">
@@ -2850,7 +2800,7 @@
         <v>81</v>
       </c>
       <c r="G12" s="52" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="H12" s="52"/>
       <c r="I12" s="52"/>
@@ -2877,7 +2827,7 @@
     </row>
     <row r="13" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="52" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C13" s="52"/>
       <c r="D13" s="54" t="s">
@@ -2890,7 +2840,7 @@
         <v>74</v>
       </c>
       <c r="G13" s="52" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="H13" s="52">
         <v>1</v>
@@ -2919,7 +2869,7 @@
     </row>
     <row r="14" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="52" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C14" s="52"/>
       <c r="D14" s="54" t="s">
@@ -2932,7 +2882,7 @@
         <v>81</v>
       </c>
       <c r="G14" s="52" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="H14" s="52"/>
       <c r="I14" s="52"/>
@@ -2959,7 +2909,7 @@
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B15" s="52" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C15" s="52" t="s">
         <v>92</v>
@@ -2974,7 +2924,7 @@
         <v>85</v>
       </c>
       <c r="G15" s="52" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="H15" s="52">
         <v>1</v>
@@ -3041,7 +2991,7 @@
         <v>6660</v>
       </c>
       <c r="P16" s="52">
-        <f t="shared" ref="P16:P32" si="1">N16+O16</f>
+        <f t="shared" ref="P16:P28" si="1">N16+O16</f>
         <v>12660</v>
       </c>
     </row>
@@ -3356,7 +3306,7 @@
         <v>85</v>
       </c>
       <c r="G24" s="52" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="H24" s="52">
         <v>1</v>
@@ -3398,7 +3348,7 @@
         <v>90</v>
       </c>
       <c r="G25" s="52" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="H25" s="52">
         <v>1</v>
@@ -3440,7 +3390,7 @@
         <v>85</v>
       </c>
       <c r="G26" s="52" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="H26" s="52">
         <v>2</v>
@@ -3486,7 +3436,7 @@
         <v>83</v>
       </c>
       <c r="G27" s="52" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="H27" s="56"/>
       <c r="I27" s="56"/>
@@ -3524,7 +3474,7 @@
         <v>90</v>
       </c>
       <c r="G28" s="52" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="H28" s="52">
         <v>1</v>
@@ -4215,7 +4165,7 @@
       <c r="P59" s="56"/>
     </row>
   </sheetData>
-  <autoFilter ref="B4:P34" xr:uid="{24D3D14F-C4FA-4576-ABA6-ACB55BFAAF61}"/>
+  <autoFilter ref="B4:P34"/>
   <mergeCells count="1">
     <mergeCell ref="B2:C2"/>
   </mergeCells>
@@ -4228,11 +4178,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="B1:I35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4247,13 +4197,13 @@
   <sheetData>
     <row r="1" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="80" t="s">
+      <c r="B2" s="82" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="81"/>
+      <c r="C2" s="83"/>
       <c r="D2" s="43">
-        <f>SUM(I5:I35)</f>
-        <v>140730</v>
+        <f>SUM(I5:I34)</f>
+        <v>346905</v>
       </c>
     </row>
     <row r="4" spans="2:9" ht="45" x14ac:dyDescent="0.25">
@@ -4327,7 +4277,7 @@
         <v>12</v>
       </c>
       <c r="I6" s="39">
-        <f t="shared" ref="I6:I35" si="0">G6*H6</f>
+        <f t="shared" ref="I6:I34" si="0">G6*H6</f>
         <v>840</v>
       </c>
     </row>
@@ -4420,17 +4370,17 @@
         <v>100</v>
       </c>
       <c r="F10" s="47" t="s">
-        <v>106</v>
-      </c>
-      <c r="G10" s="47">
-        <v>1500</v>
+        <v>122</v>
+      </c>
+      <c r="G10" s="58">
+        <v>12825</v>
       </c>
       <c r="H10" s="47">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="I10" s="39">
         <f t="shared" si="0"/>
-        <v>6000</v>
+        <v>102600</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
@@ -4447,7 +4397,7 @@
         <v>100</v>
       </c>
       <c r="F11" s="39" t="s">
-        <v>110</v>
+        <v>124</v>
       </c>
       <c r="G11" s="39">
         <v>1200</v>
@@ -4472,7 +4422,7 @@
         <v>89</v>
       </c>
       <c r="F12" s="47" t="s">
-        <v>111</v>
+        <v>125</v>
       </c>
       <c r="G12" s="39">
         <v>1200</v>
@@ -4499,7 +4449,7 @@
         <v>100</v>
       </c>
       <c r="F13" s="39" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G13" s="39">
         <v>250</v>
@@ -4526,7 +4476,7 @@
         <v>100</v>
       </c>
       <c r="F14" s="39" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G14" s="39">
         <v>900</v>
@@ -4551,7 +4501,7 @@
         <v>84</v>
       </c>
       <c r="F15" s="49" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G15" s="49">
         <v>80</v>
@@ -4565,77 +4515,107 @@
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="39"/>
+      <c r="B16" s="39" t="s">
+        <v>127</v>
+      </c>
       <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="39"/>
-      <c r="F16" s="39" t="s">
-        <v>130</v>
-      </c>
-      <c r="G16" s="39">
-        <v>10000</v>
+      <c r="D16" s="58" t="s">
+        <v>80</v>
+      </c>
+      <c r="E16" s="58" t="s">
+        <v>89</v>
+      </c>
+      <c r="F16" s="58" t="s">
+        <v>119</v>
+      </c>
+      <c r="G16" s="58">
+        <v>98700</v>
       </c>
       <c r="H16" s="39">
         <v>1</v>
       </c>
-      <c r="I16" s="39">
+      <c r="I16" s="58">
         <f t="shared" si="0"/>
-        <v>10000</v>
+        <v>98700</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="39"/>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="39"/>
+      <c r="B17" s="58" t="s">
+        <v>127</v>
+      </c>
+      <c r="C17" s="58" t="s">
+        <v>92</v>
+      </c>
+      <c r="D17" s="58" t="s">
+        <v>94</v>
+      </c>
+      <c r="E17" s="58" t="s">
+        <v>100</v>
+      </c>
       <c r="F17" s="39" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="G17" s="39">
-        <v>980</v>
-      </c>
-      <c r="H17" s="39"/>
+        <v>98700</v>
+      </c>
+      <c r="H17" s="39">
+        <v>1</v>
+      </c>
       <c r="I17" s="39">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>98700</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="39"/>
-      <c r="C18" s="39"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="39"/>
+      <c r="B18" s="58" t="s">
+        <v>127</v>
+      </c>
+      <c r="C18" s="58" t="s">
+        <v>92</v>
+      </c>
+      <c r="D18" s="58" t="s">
+        <v>94</v>
+      </c>
+      <c r="E18" s="58" t="s">
+        <v>100</v>
+      </c>
       <c r="F18" s="39" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="G18" s="39">
-        <v>98700</v>
+        <v>6155</v>
       </c>
       <c r="H18" s="39">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I18" s="39">
         <f t="shared" si="0"/>
-        <v>98700</v>
+        <v>24620</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="39"/>
-      <c r="C19" s="39"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="39"/>
+      <c r="B19" s="57" t="s">
+        <v>91</v>
+      </c>
+      <c r="C19" s="57"/>
+      <c r="D19" s="57" t="s">
+        <v>77</v>
+      </c>
+      <c r="E19" s="57" t="s">
+        <v>84</v>
+      </c>
       <c r="F19" s="39" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="G19" s="39">
-        <v>6155</v>
+        <v>2855</v>
       </c>
       <c r="H19" s="39">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I19" s="39">
         <f t="shared" si="0"/>
-        <v>12310</v>
+        <v>8565</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
@@ -4833,20 +4813,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B35" s="39"/>
-      <c r="C35" s="39"/>
-      <c r="D35" s="39"/>
-      <c r="E35" s="39"/>
-      <c r="F35" s="39"/>
-      <c r="G35" s="39"/>
-      <c r="H35" s="39"/>
-      <c r="I35" s="39">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
+  <autoFilter ref="B4:I34"/>
   <mergeCells count="1">
     <mergeCell ref="B2:C2"/>
   </mergeCells>
@@ -4855,17 +4823,18 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:I9"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18.5703125" customWidth="1"/>
     <col min="4" max="4" width="37.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" customWidth="1"/>
     <col min="6" max="6" width="70.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="34.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
@@ -4873,13 +4842,13 @@
   <sheetData>
     <row r="1" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="80" t="s">
+      <c r="B2" s="82" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="81"/>
+      <c r="C2" s="83"/>
       <c r="D2" s="43">
         <f>SUM(I5:I35)</f>
-        <v>61200</v>
+        <v>193000</v>
       </c>
     </row>
     <row r="4" spans="2:9" ht="45" x14ac:dyDescent="0.25">
@@ -4909,261 +4878,237 @@
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="39" t="s">
-        <v>72</v>
-      </c>
-      <c r="C5" s="51" t="s">
+      <c r="B5" s="57" t="s">
+        <v>115</v>
+      </c>
+      <c r="C5" s="57" t="s">
         <v>92</v>
       </c>
-      <c r="D5" s="51" t="s">
+      <c r="D5" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="E5" s="51" t="s">
+      <c r="E5" s="57" t="s">
         <v>100</v>
       </c>
-      <c r="F5" s="39" t="s">
-        <v>117</v>
-      </c>
-      <c r="G5" s="39">
-        <v>140</v>
-      </c>
-      <c r="H5" s="39">
-        <v>5</v>
-      </c>
-      <c r="I5" s="39">
-        <f>G5*H5</f>
-        <v>700</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="51" t="s">
-        <v>112</v>
-      </c>
-      <c r="C6" s="39"/>
-      <c r="D6" s="54" t="s">
-        <v>73</v>
-      </c>
-      <c r="E6" s="52" t="s">
-        <v>75</v>
-      </c>
-      <c r="F6" s="39" t="s">
-        <v>119</v>
-      </c>
-      <c r="G6" s="39">
-        <v>40</v>
-      </c>
-      <c r="H6" s="39">
-        <v>5</v>
-      </c>
-      <c r="I6" s="39">
-        <f t="shared" ref="I6:I11" si="0">G6*H6</f>
-        <v>200</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="51" t="s">
-        <v>118</v>
-      </c>
-      <c r="C7" s="39"/>
-      <c r="D7" s="55" t="s">
-        <v>76</v>
-      </c>
-      <c r="E7" s="51" t="s">
-        <v>82</v>
-      </c>
-      <c r="F7" s="39" t="s">
-        <v>120</v>
-      </c>
-      <c r="G7" s="39">
-        <v>20</v>
-      </c>
-      <c r="H7" s="39">
-        <v>5</v>
-      </c>
-      <c r="I7" s="39">
-        <f t="shared" si="0"/>
+      <c r="F5" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="G5" s="57">
+        <v>30000</v>
+      </c>
+      <c r="H5" s="57">
+        <v>1</v>
+      </c>
+      <c r="I5" s="57">
+        <f t="shared" ref="I5:I6" si="0">G5*H5</f>
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="57" t="s">
+        <v>95</v>
+      </c>
+      <c r="C6" s="57" t="s">
+        <v>92</v>
+      </c>
+      <c r="D6" s="57" t="s">
+        <v>94</v>
+      </c>
+      <c r="E6" s="57" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="8" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="51" t="s">
-        <v>122</v>
-      </c>
-      <c r="C8" s="39"/>
-      <c r="D8" s="55" t="s">
-        <v>78</v>
-      </c>
-      <c r="E8" s="51" t="s">
-        <v>84</v>
-      </c>
-      <c r="F8" s="39" t="s">
-        <v>121</v>
-      </c>
-      <c r="G8" s="39">
-        <v>20</v>
-      </c>
-      <c r="H8" s="39">
-        <v>5</v>
-      </c>
-      <c r="I8" s="39">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="51" t="s">
-        <v>124</v>
-      </c>
-      <c r="C9" s="39"/>
-      <c r="D9" s="55" t="s">
-        <v>79</v>
-      </c>
-      <c r="E9" s="51" t="s">
-        <v>87</v>
-      </c>
-      <c r="F9" s="39" t="s">
-        <v>123</v>
-      </c>
-      <c r="G9" s="39">
-        <v>20</v>
-      </c>
-      <c r="H9" s="39">
-        <v>5</v>
-      </c>
-      <c r="I9" s="39">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="39" t="s">
-        <v>126</v>
-      </c>
-      <c r="C10" s="51" t="s">
-        <v>92</v>
-      </c>
-      <c r="D10" s="51" t="s">
-        <v>94</v>
-      </c>
-      <c r="E10" s="51" t="s">
-        <v>100</v>
-      </c>
-      <c r="F10" s="39" t="s">
-        <v>125</v>
-      </c>
-      <c r="G10" s="39">
-        <v>30000</v>
-      </c>
-      <c r="H10" s="39">
-        <v>1</v>
-      </c>
-      <c r="I10" s="39">
-        <f t="shared" si="0"/>
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="39" t="s">
-        <v>95</v>
-      </c>
-      <c r="C11" s="51" t="s">
-        <v>92</v>
-      </c>
-      <c r="D11" s="51" t="s">
-        <v>94</v>
-      </c>
-      <c r="E11" s="51" t="s">
-        <v>100</v>
-      </c>
-      <c r="F11" s="39" t="s">
-        <v>127</v>
-      </c>
-      <c r="G11" s="39">
+      <c r="F6" s="57" t="s">
+        <v>116</v>
+      </c>
+      <c r="G6" s="57">
         <v>7000</v>
       </c>
-      <c r="H11" s="39">
-        <v>1</v>
-      </c>
-      <c r="I11" s="39">
+      <c r="H6" s="57">
+        <v>1</v>
+      </c>
+      <c r="I6" s="57">
         <f t="shared" si="0"/>
         <v>7000</v>
       </c>
     </row>
-    <row r="12" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="51" t="s">
+    <row r="7" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="57" t="s">
         <v>91</v>
       </c>
+      <c r="C7" s="57"/>
+      <c r="D7" s="55" t="s">
+        <v>77</v>
+      </c>
+      <c r="E7" s="57" t="s">
+        <v>84</v>
+      </c>
+      <c r="F7" s="57" t="s">
+        <v>116</v>
+      </c>
+      <c r="G7" s="57">
+        <v>7000</v>
+      </c>
+      <c r="H7" s="57">
+        <v>1</v>
+      </c>
+      <c r="I7" s="57">
+        <f>G7*H7</f>
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="57" t="s">
+        <v>96</v>
+      </c>
+      <c r="C8" s="57" t="s">
+        <v>92</v>
+      </c>
+      <c r="D8" s="57" t="s">
+        <v>94</v>
+      </c>
+      <c r="E8" s="57" t="s">
+        <v>100</v>
+      </c>
+      <c r="F8" s="57" t="s">
+        <v>117</v>
+      </c>
+      <c r="G8" s="57">
+        <v>1000</v>
+      </c>
+      <c r="H8" s="57">
+        <v>1</v>
+      </c>
+      <c r="I8" s="57">
+        <f>G8*H8</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="57" t="s">
+        <v>96</v>
+      </c>
+      <c r="C9" s="57"/>
+      <c r="D9" s="55" t="s">
+        <v>77</v>
+      </c>
+      <c r="E9" s="57" t="s">
+        <v>84</v>
+      </c>
+      <c r="F9" s="57" t="s">
+        <v>118</v>
+      </c>
+      <c r="G9" s="57">
+        <v>15000</v>
+      </c>
+      <c r="H9" s="57">
+        <v>1</v>
+      </c>
+      <c r="I9" s="57">
+        <f>G9*H9</f>
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="58" t="s">
+        <v>91</v>
+      </c>
+      <c r="C10" s="58" t="s">
+        <v>92</v>
+      </c>
+      <c r="D10" s="58" t="s">
+        <v>94</v>
+      </c>
+      <c r="E10" s="58" t="s">
+        <v>100</v>
+      </c>
+      <c r="F10" s="39" t="s">
+        <v>123</v>
+      </c>
+      <c r="G10" s="39">
+        <v>58000</v>
+      </c>
+      <c r="H10" s="39">
+        <v>1</v>
+      </c>
+      <c r="I10" s="57">
+        <f>G10*H10</f>
+        <v>58000</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="58" t="s">
+        <v>91</v>
+      </c>
+      <c r="C11" s="51"/>
+      <c r="D11" s="52" t="s">
+        <v>80</v>
+      </c>
+      <c r="E11" s="52" t="s">
+        <v>89</v>
+      </c>
+      <c r="F11" s="58" t="s">
+        <v>123</v>
+      </c>
+      <c r="G11" s="58">
+        <v>58000</v>
+      </c>
+      <c r="H11" s="39">
+        <v>1</v>
+      </c>
+      <c r="I11" s="57">
+        <f>G11*H11</f>
+        <v>58000</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="58" t="s">
+        <v>127</v>
+      </c>
       <c r="C12" s="51"/>
-      <c r="D12" s="55" t="s">
-        <v>77</v>
-      </c>
-      <c r="E12" s="51" t="s">
-        <v>84</v>
+      <c r="D12" s="52" t="s">
+        <v>80</v>
+      </c>
+      <c r="E12" s="52" t="s">
+        <v>89</v>
       </c>
       <c r="F12" s="51" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G12" s="51">
-        <v>7000</v>
+        <v>8500</v>
       </c>
       <c r="H12" s="51">
-        <v>1</v>
-      </c>
-      <c r="I12" s="39">
+        <v>2</v>
+      </c>
+      <c r="I12" s="57">
         <f>G12*H12</f>
-        <v>7000</v>
+        <v>17000</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="39" t="s">
-        <v>96</v>
-      </c>
-      <c r="C13" s="51" t="s">
-        <v>92</v>
-      </c>
-      <c r="D13" s="51" t="s">
-        <v>94</v>
-      </c>
-      <c r="E13" s="51" t="s">
-        <v>100</v>
-      </c>
-      <c r="F13" s="39" t="s">
-        <v>128</v>
-      </c>
-      <c r="G13" s="39">
-        <v>1000</v>
-      </c>
-      <c r="H13" s="39">
-        <v>1</v>
-      </c>
-      <c r="I13" s="39">
-        <f>G13*H13</f>
-        <v>1000</v>
+      <c r="B13" s="39"/>
+      <c r="C13" s="51"/>
+      <c r="D13" s="51"/>
+      <c r="E13" s="51"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="39"/>
+      <c r="I13" s="57">
+        <f t="shared" ref="I10:I35" si="1">G14*H14</f>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="39" t="s">
-        <v>96</v>
-      </c>
+      <c r="B14" s="39"/>
       <c r="C14" s="51"/>
-      <c r="D14" s="55" t="s">
-        <v>77</v>
-      </c>
-      <c r="E14" s="51" t="s">
-        <v>84</v>
-      </c>
-      <c r="F14" s="39" t="s">
-        <v>129</v>
-      </c>
-      <c r="G14" s="39">
-        <v>15000</v>
-      </c>
-      <c r="H14" s="39">
-        <v>1</v>
-      </c>
-      <c r="I14" s="39">
-        <f>G14*H14</f>
-        <v>15000</v>
+      <c r="D14" s="55"/>
+      <c r="E14" s="51"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="39"/>
+      <c r="H14" s="39"/>
+      <c r="I14" s="57">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
@@ -5175,7 +5120,7 @@
       <c r="G15" s="39"/>
       <c r="H15" s="39"/>
       <c r="I15" s="39">
-        <f t="shared" ref="I15:I35" si="1">G16*H16</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>